<commit_message>
Merged dynamic creation of Jobs and Papers
</commit_message>
<xml_diff>
--- a/data/CV.xlsx
+++ b/data/CV.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9048" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9048" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Papers" sheetId="1" r:id="rId1"/>
     <sheet name="Presentations" sheetId="2" r:id="rId2"/>
     <sheet name="Jobs" sheetId="3" r:id="rId3"/>
-    <sheet name="ArtItems" sheetId="6" r:id="rId4"/>
-    <sheet name="ProgrammingItems" sheetId="4" r:id="rId5"/>
+    <sheet name="Art" sheetId="6" r:id="rId4"/>
+    <sheet name="Programming" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1099,8 +1099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A24053F2-2CC5-4EAC-BEAB-64F1B89D9BFF}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1228,10 +1228,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94D0DD9B-3A24-4EEE-B532-5A3AF00D7B57}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1276,6 +1276,9 @@
         <v>86</v>
       </c>
     </row>
+    <row r="21" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G21" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added working experience to CV Database.
- Also some minor display settings
</commit_message>
<xml_diff>
--- a/data/CV.xlsx
+++ b/data/CV.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9048" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9048" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Papers" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="113">
   <si>
     <t>ID</t>
   </si>
@@ -295,13 +295,73 @@
     <t>ERC Postdoctoral Research Fellow</t>
   </si>
   <si>
-    <t>2016-Now</t>
-  </si>
-  <si>
     <t>Department of Computer Science, Ben Gurion University of the Negev</t>
   </si>
   <si>
-    <t>ERC Proect: "Combinatorial Aspects of Computational Geometry"</t>
+    <t>Web Administrator</t>
+  </si>
+  <si>
+    <t>2016 - Now</t>
+  </si>
+  <si>
+    <t>ERC Project: "Combinatorial Aspects of Computational Geometry"</t>
+  </si>
+  <si>
+    <t>2013 - Now</t>
+  </si>
+  <si>
+    <t>Olimpiada Mexicana de Matemáticas</t>
+  </si>
+  <si>
+    <t>Server set-up, domain management and annual update of official website</t>
+  </si>
+  <si>
+    <t>Chair</t>
+  </si>
+  <si>
+    <t>2016 - 2018</t>
+  </si>
+  <si>
+    <t>Asian Pacific Mathematical Olympiad</t>
+  </si>
+  <si>
+    <t>Lead the organization of annual competition for students in 45 countries &lt;br&gt; Set up of official website to publish resullts and statistics.</t>
+  </si>
+  <si>
+    <t>Jury Member and Coordinator</t>
+  </si>
+  <si>
+    <t>International Mathematical Olympiad</t>
+  </si>
+  <si>
+    <t>2012 - 2017</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt; &lt;li&gt; 2012-2015 Member of the Jury of the International Mathematical Olympiad. Select problems and marking schemes for the competition. Grading and coordination of scores as Team Leader for Mexico &lt;/li&gt; &lt;li&gt; 2017 Coordinator of the International Matematical Olympiad. Ellaboration of marking schemes and grading of international students &lt;/li&gt; &lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>Audiovisual Translator</t>
+  </si>
+  <si>
+    <t>2012 - 2014</t>
+  </si>
+  <si>
+    <t>Khan Academy via Fundación Slim</t>
+  </si>
+  <si>
+    <t>Translation from English to Spanish of 550 videos in mathematics, finance and physics</t>
+  </si>
+  <si>
+    <t>Adjunct Professor and Teaching Assistant</t>
+  </si>
+  <si>
+    <t>2010 - 2013</t>
+  </si>
+  <si>
+    <t>Universidad Nacional Autónoma de México</t>
+  </si>
+  <si>
+    <t>Courses: Analytic Geometry, Calculus, Complex Analysis, Probability, Problem-Solving Seminar, Real Analysis, Stochastic Processes</t>
   </si>
 </sst>
 </file>
@@ -1097,10 +1157,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A24053F2-2CC5-4EAC-BEAB-64F1B89D9BFF}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1147,17 +1207,99 @@
         <v>89</v>
       </c>
       <c r="C3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" t="s">
         <v>90</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>112</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1230,8 +1372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94D0DD9B-3A24-4EEE-B532-5A3AF00D7B57}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Introduced Award class, awards.html template and control for it
- Also, minor visual adjustments
</commit_message>
<xml_diff>
--- a/data/CV.xlsx
+++ b/data/CV.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9048" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9048" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Papers" sheetId="1" r:id="rId1"/>
-    <sheet name="Presentations" sheetId="2" r:id="rId2"/>
+    <sheet name="Awards" sheetId="7" r:id="rId1"/>
+    <sheet name="Art" sheetId="6" r:id="rId2"/>
     <sheet name="Jobs" sheetId="3" r:id="rId3"/>
-    <sheet name="Art" sheetId="6" r:id="rId4"/>
-    <sheet name="Programming" sheetId="4" r:id="rId5"/>
+    <sheet name="Papers" sheetId="1" r:id="rId4"/>
+    <sheet name="Presentations" sheetId="2" r:id="rId5"/>
+    <sheet name="Programming" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="121">
   <si>
     <t>ID</t>
   </si>
@@ -362,6 +363,30 @@
   </si>
   <si>
     <t>Courses: Analytic Geometry, Calculus, Complex Analysis, Probability, Problem-Solving Seminar, Real Analysis, Stochastic Processes</t>
+  </si>
+  <si>
+    <t>Institution</t>
+  </si>
+  <si>
+    <t>institution</t>
+  </si>
+  <si>
+    <t>Great institution</t>
+  </si>
+  <si>
+    <t>Moon</t>
+  </si>
+  <si>
+    <t>Award Name</t>
+  </si>
+  <si>
+    <t>award</t>
+  </si>
+  <si>
+    <t>Given to 3 people!</t>
+  </si>
+  <si>
+    <t>Diamond Medal</t>
   </si>
 </sst>
 </file>
@@ -688,6 +713,298 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEAE7294-192C-46DF-96EB-A7CACD84CB01}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C4" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE156D2-7E33-4447-A53C-1EA25432072D}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A24053F2-2CC5-4EAC-BEAB-64F1B89D9BFF}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
@@ -1094,7 +1411,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{820DCA41-7065-4B6F-8FCC-B838DB872725}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1155,220 +1472,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A24053F2-2CC5-4EAC-BEAB-64F1B89D9BFF}">
-  <dimension ref="A1:E8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D7" t="s">
-        <v>107</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C8" t="s">
-        <v>110</v>
-      </c>
-      <c r="D8" t="s">
-        <v>111</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE156D2-7E33-4447-A53C-1EA25432072D}">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94D0DD9B-3A24-4EEE-B532-5A3AF00D7B57}">
   <dimension ref="A1:G21"/>
   <sheetViews>

</xml_diff>

<commit_message>
Implemented Programming section. Added high-school.
- Added property type to ProgrammingItem
- Created timeline function for ProgrammingItem and added it to script
- Created pages for Python, Web and Data Science projects
- Added the corresponding entries to the CV
- Renamed section slides to presentations
</commit_message>
<xml_diff>
--- a/data/CV.xlsx
+++ b/data/CV.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9048" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9048" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Awards" sheetId="7" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="193">
   <si>
     <t>ID</t>
   </si>
@@ -287,12 +287,6 @@
     <t>link</t>
   </si>
   <si>
-    <t>Technology</t>
-  </si>
-  <si>
-    <t>technology</t>
-  </si>
-  <si>
     <t>ERC Postdoctoral Research Fellow</t>
   </si>
   <si>
@@ -468,13 +462,154 @@
   </si>
   <si>
     <t>Research Fellow at Sistema Nacional de Investigadores in Mexico</t>
+  </si>
+  <si>
+    <t>GH1</t>
+  </si>
+  <si>
+    <t>GH2</t>
+  </si>
+  <si>
+    <t>GH3</t>
+  </si>
+  <si>
+    <t>Python scripts to create the official webpage of the Asian Pacific Mathematical Olympiad for the period 2016 - 2018. It includes functions to create problem difficulty statistics and plots.</t>
+  </si>
+  <si>
+    <t>APMO Website Scripts</t>
+  </si>
+  <si>
+    <t>Personal Page</t>
+  </si>
+  <si>
+    <t>Flask webapp to create a personal professional page using a CV managed with CV Utilities. This personal page is created itself with personalpage!</t>
+  </si>
+  <si>
+    <t>Collect Definitions</t>
+  </si>
+  <si>
+    <t>GH4</t>
+  </si>
+  <si>
+    <t>Golden Cookie Clicker</t>
+  </si>
+  <si>
+    <t>GH5</t>
+  </si>
+  <si>
+    <t>This is a computer vision project. In the game &lt;a href="http://orteil.dashnet.org/cookieclicker/" target="_blank"&gt; Cookie Clicker&lt;/a&gt; there is a golden cookie that appears from time to time and boosts the cookie production. It is one of the few mechanics that require that the user is paying attention. This is a Python bot that automatically clicks on a golden cookie when it appears.</t>
+  </si>
+  <si>
+    <t>Object Oriented library for managing a Curriculum Vitae from an .xlsx file. Implements basically everything that you can see in this page.</t>
+  </si>
+  <si>
+    <t>CV Utilities (cvutils)</t>
+  </si>
+  <si>
+    <t>ConvierTex</t>
+  </si>
+  <si>
+    <t>Personal Blog</t>
+  </si>
+  <si>
+    <t>Mexican Mathematical Olympiad Website</t>
+  </si>
+  <si>
+    <t>technologies</t>
+  </si>
+  <si>
+    <t>python</t>
+  </si>
+  <si>
+    <t>webadmin</t>
+  </si>
+  <si>
+    <t>http://blog.nekomath.com</t>
+  </si>
+  <si>
+    <t>http://www.ommenlinea.org</t>
+  </si>
+  <si>
+    <t>VII CIIM Website</t>
+  </si>
+  <si>
+    <t>SNI Conacyt</t>
+  </si>
+  <si>
+    <t>Technologies</t>
+  </si>
+  <si>
+    <t>matplotlib, openpyxl</t>
+  </si>
+  <si>
+    <t>flask, cvutils, HTML, CSS, JavaScript, AJAX, jinja2</t>
+  </si>
+  <si>
+    <t>open_cv, SIFT, winsound, time, pyautogui, ImageGrab</t>
+  </si>
+  <si>
+    <t>openpyxl, numpy, matplotlib, HTML, CSS, JavaScript</t>
+  </si>
+  <si>
+    <t>API, CSS, HTML, BeautifulSoup</t>
+  </si>
+  <si>
+    <t>LaTeX, sha, HTML, CSS, BeautifulSoup</t>
+  </si>
+  <si>
+    <t>WordPress, HTML, CSS, PHP, FTP, SSH, MathJax</t>
+  </si>
+  <si>
+    <t>HTML, CSS, lightbox</t>
+  </si>
+  <si>
+    <t>python, pandas, matplotlib</t>
+  </si>
+  <si>
+    <t>WordPress, HTML, CSS, WPStats, PHP, Avada, FTP, SSH, MathJax, SQL</t>
+  </si>
+  <si>
+    <t>Mexico City Mathematical Olympiad Website</t>
+  </si>
+  <si>
+    <t>Write a LaTeX formula, click a button, and share it with the world! Created from scratch.</t>
+  </si>
+  <si>
+    <t>Do you have troubles reading english text with unusual words? By giving a list of words to this script, it gathers all the definitions that you need from … and creates an HTML file to see all of them in a beautiful way.</t>
+  </si>
+  <si>
+    <t>My personal blog.</t>
+  </si>
+  <si>
+    <t>The official website of the Mexican Mathematical Olympiad.</t>
+  </si>
+  <si>
+    <t>The official website of the VII Competencia Iberoamericana Interuniversitaria de Matemáticas.</t>
+  </si>
+  <si>
+    <t>Data visualization project on the information of the researchers at Conacyt in Mexico.</t>
+  </si>
+  <si>
+    <t>The official webpage for the Mathematical Olympiad of Mexico City from 2010 to 2013 (check).</t>
+  </si>
+  <si>
+    <t>webdev</t>
+  </si>
+  <si>
+    <t>datasc</t>
+  </si>
+  <si>
+    <t>http://ciim2015.ommenlinea.org</t>
+  </si>
+  <si>
+    <t>WordPress, HTML, CSS, FTP, SSH, Nirvana</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -486,6 +621,14 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -508,15 +651,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -797,7 +943,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEAE7294-192C-46DF-96EB-A7CACD84CB01}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -811,10 +957,10 @@
         <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E1" t="s">
         <v>81</v>
@@ -831,10 +977,10 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E2" t="s">
         <v>82</v>
@@ -848,19 +994,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E3" t="s">
         <v>145</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D3" t="s">
-        <v>143</v>
-      </c>
-      <c r="E3" t="s">
-        <v>147</v>
-      </c>
       <c r="F3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -871,16 +1017,16 @@
         <v>2016</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D4" t="s">
         <v>34</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -891,16 +1037,16 @@
         <v>2014</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E5" t="s">
         <v>119</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>120</v>
-      </c>
-      <c r="E5" t="s">
-        <v>121</v>
-      </c>
-      <c r="F5" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -911,16 +1057,16 @@
         <v>2012</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F6" t="s">
         <v>123</v>
-      </c>
-      <c r="D6" t="s">
-        <v>120</v>
-      </c>
-      <c r="E6" t="s">
-        <v>124</v>
-      </c>
-      <c r="F6" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -931,13 +1077,13 @@
         <v>2010</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F7" t="s">
         <v>127</v>
-      </c>
-      <c r="D7" t="s">
-        <v>131</v>
-      </c>
-      <c r="F7" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -948,13 +1094,13 @@
         <v>2009</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F8" t="s">
         <v>126</v>
-      </c>
-      <c r="D8" t="s">
-        <v>131</v>
-      </c>
-      <c r="F8" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -962,17 +1108,17 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -983,16 +1129,16 @@
         <v>2008</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D10" t="s">
         <v>130</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
+        <v>131</v>
+      </c>
+      <c r="F10" t="s">
         <v>132</v>
-      </c>
-      <c r="E10" t="s">
-        <v>133</v>
-      </c>
-      <c r="F10" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1003,16 +1149,16 @@
         <v>2007</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" t="s">
         <v>130</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
+        <v>134</v>
+      </c>
+      <c r="F11" t="s">
         <v>132</v>
-      </c>
-      <c r="E11" t="s">
-        <v>136</v>
-      </c>
-      <c r="F11" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1023,13 +1169,13 @@
         <v>2007</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1040,16 +1186,16 @@
         <v>2006</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1060,16 +1206,16 @@
         <v>2006</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D14" t="s">
+        <v>130</v>
+      </c>
+      <c r="E14" t="s">
+        <v>134</v>
+      </c>
+      <c r="F14" t="s">
         <v>132</v>
-      </c>
-      <c r="E14" t="s">
-        <v>136</v>
-      </c>
-      <c r="F14" t="s">
-        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1191,16 +1337,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1208,16 +1354,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" t="s">
         <v>94</v>
-      </c>
-      <c r="D4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1225,16 +1371,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" t="s">
         <v>97</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>98</v>
-      </c>
-      <c r="D5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E5" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1242,16 +1388,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" t="s">
         <v>101</v>
       </c>
-      <c r="C6" t="s">
-        <v>103</v>
-      </c>
       <c r="D6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" t="s">
         <v>102</v>
-      </c>
-      <c r="E6" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1259,16 +1405,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" t="s">
         <v>105</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="D7" t="s">
-        <v>107</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1276,16 +1422,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" t="s">
         <v>109</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="D8" t="s">
-        <v>111</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1764,15 +1910,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94D0DD9B-3A24-4EEE-B532-5A3AF00D7B57}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1783,16 +1929,19 @@
         <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="E1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F1" t="s">
         <v>81</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1803,20 +1952,279 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="E2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F2" t="s">
         <v>82</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G21" s="2"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3">
+        <v>2018</v>
+      </c>
+      <c r="D3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F3" t="s">
+        <v>158</v>
+      </c>
+      <c r="G3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4">
+        <v>2018</v>
+      </c>
+      <c r="D4" t="s">
+        <v>164</v>
+      </c>
+      <c r="E4" t="s">
+        <v>172</v>
+      </c>
+      <c r="F4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C5">
+        <v>2017</v>
+      </c>
+      <c r="D5" t="s">
+        <v>164</v>
+      </c>
+      <c r="E5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6">
+        <v>2016</v>
+      </c>
+      <c r="D6" t="s">
+        <v>164</v>
+      </c>
+      <c r="E6" t="s">
+        <v>174</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G6" t="s">
+        <v>148</v>
+      </c>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7">
+        <v>2015</v>
+      </c>
+      <c r="D7" t="s">
+        <v>164</v>
+      </c>
+      <c r="E7" t="s">
+        <v>175</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C8">
+        <v>2011</v>
+      </c>
+      <c r="D8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E8" t="s">
+        <v>176</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C9">
+        <v>2011</v>
+      </c>
+      <c r="D9" t="s">
+        <v>189</v>
+      </c>
+      <c r="E9" t="s">
+        <v>177</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>162</v>
+      </c>
+      <c r="C10">
+        <v>2013</v>
+      </c>
+      <c r="D10" t="s">
+        <v>189</v>
+      </c>
+      <c r="E10" t="s">
+        <v>180</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>168</v>
+      </c>
+      <c r="C11">
+        <v>2015</v>
+      </c>
+      <c r="D11" t="s">
+        <v>189</v>
+      </c>
+      <c r="E11" t="s">
+        <v>192</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>169</v>
+      </c>
+      <c r="C12">
+        <v>2016</v>
+      </c>
+      <c r="D12" t="s">
+        <v>190</v>
+      </c>
+      <c r="E12" t="s">
+        <v>179</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>181</v>
+      </c>
+      <c r="C13">
+        <v>2010</v>
+      </c>
+      <c r="D13" t="s">
+        <v>165</v>
+      </c>
+      <c r="E13" t="s">
+        <v>178</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="20" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H20" s="2"/>
     </row>
   </sheetData>
+  <sortState ref="B3:G7">
+    <sortCondition descending="1" ref="C3:C7"/>
+  </sortState>
+  <hyperlinks>
+    <hyperlink ref="G9" r:id="rId1" xr:uid="{905EA6D7-19FC-40A7-9776-023EBCA825B9}"/>
+    <hyperlink ref="G10" r:id="rId2" xr:uid="{D02A8CA5-EDC0-4CAF-8C51-DF4FD7EEB47B}"/>
+    <hyperlink ref="G11" r:id="rId3" xr:uid="{12AC93BA-BAD2-443D-93F3-0E0A59751E0F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Additional sections and minor visual adjustments
</commit_message>
<xml_diff>
--- a/data/CV.xlsx
+++ b/data/CV.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9048" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9048" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Awards" sheetId="7" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="202">
   <si>
     <t>ID</t>
   </si>
@@ -299,9 +299,6 @@
     <t>2016 - Now</t>
   </si>
   <si>
-    <t>ERC Project: "Combinatorial Aspects of Computational Geometry"</t>
-  </si>
-  <si>
     <t>2013 - Now</t>
   </si>
   <si>
@@ -320,9 +317,6 @@
     <t>Asian Pacific Mathematical Olympiad</t>
   </si>
   <si>
-    <t>Lead the organization of annual competition for students in 45 countries &lt;br&gt; Set up of official website to publish resullts and statistics.</t>
-  </si>
-  <si>
     <t>Jury Member and Coordinator</t>
   </si>
   <si>
@@ -479,12 +473,6 @@
     <t>APMO Website Scripts</t>
   </si>
   <si>
-    <t>Personal Page</t>
-  </si>
-  <si>
-    <t>Flask webapp to create a personal professional page using a CV managed with CV Utilities. This personal page is created itself with personalpage!</t>
-  </si>
-  <si>
     <t>Collect Definitions</t>
   </si>
   <si>
@@ -497,9 +485,6 @@
     <t>GH5</t>
   </si>
   <si>
-    <t>This is a computer vision project. In the game &lt;a href="http://orteil.dashnet.org/cookieclicker/" target="_blank"&gt; Cookie Clicker&lt;/a&gt; there is a golden cookie that appears from time to time and boosts the cookie production. It is one of the few mechanics that require that the user is paying attention. This is a Python bot that automatically clicks on a golden cookie when it appears.</t>
-  </si>
-  <si>
     <t>Object Oriented library for managing a Curriculum Vitae from an .xlsx file. Implements basically everything that you can see in this page.</t>
   </si>
   <si>
@@ -521,9 +506,6 @@
     <t>python</t>
   </si>
   <si>
-    <t>webadmin</t>
-  </si>
-  <si>
     <t>http://blog.nekomath.com</t>
   </si>
   <si>
@@ -560,9 +542,6 @@
     <t>WordPress, HTML, CSS, PHP, FTP, SSH, MathJax</t>
   </si>
   <si>
-    <t>HTML, CSS, lightbox</t>
-  </si>
-  <si>
     <t>python, pandas, matplotlib</t>
   </si>
   <si>
@@ -578,9 +557,6 @@
     <t>Do you have troubles reading english text with unusual words? By giving a list of words to this script, it gathers all the definitions that you need from … and creates an HTML file to see all of them in a beautiful way.</t>
   </si>
   <si>
-    <t>My personal blog.</t>
-  </si>
-  <si>
     <t>The official website of the Mexican Mathematical Olympiad.</t>
   </si>
   <si>
@@ -603,6 +579,57 @@
   </si>
   <si>
     <t>WordPress, HTML, CSS, FTP, SSH, Nirvana</t>
+  </si>
+  <si>
+    <t>This is an image detection project. In the game &lt;a href="http://orteil.dashnet.org/cookieclicker/" target="_blank"&gt; Cookie Clicker&lt;/a&gt; there is a golden cookie that appears from time to time and boosts the cookie production. It is one of the few mechanics that require that the user is paying attention. This is a Python bot that automatically clicks on a golden cookie when it appears.</t>
+  </si>
+  <si>
+    <t>Flask webapp to create a personal/professional page using a CV managed with CV Utilities. This personal page is created itself with PyPersonalPage!</t>
+  </si>
+  <si>
+    <t>PyPersonalPage</t>
+  </si>
+  <si>
+    <t>My personal blog about life and mathematics.</t>
+  </si>
+  <si>
+    <t>HTML, CSS, lightbox, SSH</t>
+  </si>
+  <si>
+    <t>European Research Council H2020 Project: "Combinatorial Aspects of Computational Geometry"</t>
+  </si>
+  <si>
+    <t>Lead the organization of annual competition for students in 45 countries &lt;br&gt; Set up of official website to publish resullts and statistics</t>
+  </si>
+  <si>
+    <t>OIMU Organizers</t>
+  </si>
+  <si>
+    <t>CIIM Organizers</t>
+  </si>
+  <si>
+    <t>For an outstanding results in undergraduate studies</t>
+  </si>
+  <si>
+    <t>Thesis</t>
+  </si>
+  <si>
+    <t>Distinct circumradii, geometric Hall-type theorems, fractional Turán-type theorems, lattice path matroids and Kneser transversals</t>
+  </si>
+  <si>
+    <t>El problema del ángel de Conway y gráficas angelicales</t>
+  </si>
+  <si>
+    <t>L. I. Martínez Sandoval</t>
+  </si>
+  <si>
+    <t>L. Martínez</t>
+  </si>
+  <si>
+    <t>PhD Dissertation</t>
+  </si>
+  <si>
+    <t>BSc Dissertation</t>
   </si>
 </sst>
 </file>
@@ -944,7 +971,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -957,10 +984,10 @@
         <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E1" t="s">
         <v>81</v>
@@ -977,10 +1004,10 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E2" t="s">
         <v>82</v>
@@ -994,19 +1021,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" t="s">
         <v>143</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E3" t="s">
-        <v>145</v>
-      </c>
       <c r="F3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1017,16 +1044,16 @@
         <v>2016</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D4" t="s">
         <v>34</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1037,16 +1064,16 @@
         <v>2014</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5" t="s">
         <v>117</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>118</v>
-      </c>
-      <c r="E5" t="s">
-        <v>119</v>
-      </c>
-      <c r="F5" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1057,16 +1084,16 @@
         <v>2012</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6" t="s">
+        <v>120</v>
+      </c>
+      <c r="F6" t="s">
         <v>121</v>
-      </c>
-      <c r="D6" t="s">
-        <v>118</v>
-      </c>
-      <c r="E6" t="s">
-        <v>122</v>
-      </c>
-      <c r="F6" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1077,13 +1104,16 @@
         <v>2010</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" t="s">
+        <v>193</v>
+      </c>
+      <c r="E7" t="s">
+        <v>127</v>
+      </c>
+      <c r="F7" t="s">
         <v>125</v>
-      </c>
-      <c r="D7" t="s">
-        <v>129</v>
-      </c>
-      <c r="F7" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1094,13 +1124,16 @@
         <v>2009</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8" t="s">
+        <v>193</v>
+      </c>
+      <c r="E8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F8" t="s">
         <v>124</v>
-      </c>
-      <c r="D8" t="s">
-        <v>129</v>
-      </c>
-      <c r="F8" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1108,17 +1141,19 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E9" s="2"/>
+        <v>135</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>194</v>
+      </c>
       <c r="F9" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1129,16 +1164,16 @@
         <v>2008</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" t="s">
         <v>128</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F10" t="s">
         <v>130</v>
-      </c>
-      <c r="E10" t="s">
-        <v>131</v>
-      </c>
-      <c r="F10" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1149,16 +1184,16 @@
         <v>2007</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D11" t="s">
         <v>128</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
+        <v>132</v>
+      </c>
+      <c r="F11" t="s">
         <v>130</v>
-      </c>
-      <c r="E11" t="s">
-        <v>134</v>
-      </c>
-      <c r="F11" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1169,13 +1204,16 @@
         <v>2007</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
+      </c>
+      <c r="D12" t="s">
+        <v>192</v>
       </c>
       <c r="E12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1186,16 +1224,16 @@
         <v>2006</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D13" t="s">
-        <v>118</v>
+        <v>122</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="E13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1206,16 +1244,16 @@
         <v>2006</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" t="s">
+        <v>132</v>
+      </c>
+      <c r="F14" t="s">
         <v>130</v>
-      </c>
-      <c r="E14" t="s">
-        <v>134</v>
-      </c>
-      <c r="F14" t="s">
-        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1293,7 +1331,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1346,7 +1384,7 @@
         <v>88</v>
       </c>
       <c r="E3" t="s">
-        <v>91</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1357,13 +1395,13 @@
         <v>89</v>
       </c>
       <c r="C4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" t="s">
         <v>92</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>93</v>
-      </c>
-      <c r="E4" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1371,16 +1409,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" t="s">
         <v>95</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>96</v>
       </c>
-      <c r="D5" t="s">
-        <v>97</v>
-      </c>
       <c r="E5" t="s">
-        <v>98</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1388,16 +1426,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" t="s">
         <v>99</v>
       </c>
-      <c r="C6" t="s">
-        <v>101</v>
-      </c>
       <c r="D6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" t="s">
         <v>100</v>
-      </c>
-      <c r="E6" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1405,16 +1443,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" t="s">
         <v>103</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="D7" t="s">
-        <v>105</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1422,16 +1460,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" t="s">
         <v>107</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="D8" t="s">
-        <v>109</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1444,8 +1482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1830,6 +1868,46 @@
       </c>
       <c r="I14" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>195</v>
+      </c>
+      <c r="C15" t="s">
+        <v>196</v>
+      </c>
+      <c r="D15" t="s">
+        <v>198</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F15">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>195</v>
+      </c>
+      <c r="C16" t="s">
+        <v>197</v>
+      </c>
+      <c r="D16" t="s">
+        <v>199</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F16">
+        <v>2011</v>
       </c>
     </row>
     <row r="17" spans="5:6" x14ac:dyDescent="0.3">
@@ -1912,8 +1990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94D0DD9B-3A24-4EEE-B532-5A3AF00D7B57}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1932,7 +2010,7 @@
         <v>67</v>
       </c>
       <c r="E1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F1" t="s">
         <v>81</v>
@@ -1955,7 +2033,7 @@
         <v>68</v>
       </c>
       <c r="E2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="F2" t="s">
         <v>82</v>
@@ -1969,22 +2047,22 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C3">
         <v>2018</v>
       </c>
       <c r="D3" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F3" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1992,22 +2070,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>151</v>
+        <v>187</v>
       </c>
       <c r="C4">
         <v>2018</v>
       </c>
       <c r="D4" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="F4" t="s">
-        <v>152</v>
+        <v>186</v>
       </c>
       <c r="G4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -2015,22 +2093,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C5">
         <v>2017</v>
       </c>
       <c r="D5" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E5" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>157</v>
+        <v>185</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -2038,22 +2116,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C6">
         <v>2016</v>
       </c>
       <c r="D6" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E6" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H6" s="2"/>
     </row>
@@ -2062,22 +2140,22 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C7">
         <v>2015</v>
       </c>
       <c r="D7" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E7" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -2085,22 +2163,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C8">
         <v>2011</v>
       </c>
       <c r="D8" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E8" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -2108,22 +2186,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C9">
-        <v>2011</v>
+        <v>2015</v>
       </c>
       <c r="D9" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="E9" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>166</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -2131,22 +2209,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C10">
         <v>2013</v>
       </c>
       <c r="D10" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="E10" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -2154,22 +2232,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="C11">
-        <v>2015</v>
+        <v>2011</v>
       </c>
       <c r="D11" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="E11" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>191</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -2177,19 +2255,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C12">
         <v>2016</v>
       </c>
       <c r="D12" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="E12" t="s">
+        <v>172</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -2197,32 +2275,32 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C13">
         <v>2010</v>
       </c>
       <c r="D13" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="E13" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H20" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="B3:G7">
-    <sortCondition descending="1" ref="C3:C7"/>
+  <sortState ref="B9:G11">
+    <sortCondition descending="1" ref="C9:C11"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="G9" r:id="rId1" xr:uid="{905EA6D7-19FC-40A7-9776-023EBCA825B9}"/>
+    <hyperlink ref="G11" r:id="rId1" xr:uid="{905EA6D7-19FC-40A7-9776-023EBCA825B9}"/>
     <hyperlink ref="G10" r:id="rId2" xr:uid="{D02A8CA5-EDC0-4CAF-8C51-DF4FD7EEB47B}"/>
-    <hyperlink ref="G11" r:id="rId3" xr:uid="{12AC93BA-BAD2-443D-93F3-0E0A59751E0F}"/>
+    <hyperlink ref="G9" r:id="rId3" xr:uid="{12AC93BA-BAD2-443D-93F3-0E0A59751E0F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>

<commit_message>
Progress on art, fairs and olympiad sections. Header is now link.
- Template handling for the three of them
- CSS for art items
- Added drawings
</commit_message>
<xml_diff>
--- a/data/CV.xlsx
+++ b/data/CV.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9048" tabRatio="714" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9048" tabRatio="714" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONFIG" sheetId="11" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="477">
   <si>
     <t>ID</t>
   </si>
@@ -732,12 +732,6 @@
     <t>role</t>
   </si>
   <si>
-    <t>professor</t>
-  </si>
-  <si>
-    <t>undergraduate</t>
-  </si>
-  <si>
     <t>Seminar on Problem Solving Techniques</t>
   </si>
   <si>
@@ -750,9 +744,6 @@
     <t>2011-2</t>
   </si>
   <si>
-    <t>ta</t>
-  </si>
-  <si>
     <t>Mathematical Analysis</t>
   </si>
   <si>
@@ -792,21 +783,12 @@
     <t>2012-1</t>
   </si>
   <si>
-    <t>student</t>
-  </si>
-  <si>
     <t>Stanford University</t>
   </si>
   <si>
-    <t>highschool</t>
-  </si>
-  <si>
     <t>Stanford University Mathematics Camp</t>
   </si>
   <si>
-    <t>technical</t>
-  </si>
-  <si>
     <t>A new perspective on four classical theorems in additive number theory</t>
   </si>
   <si>
@@ -817,9 +799,6 @@
   </si>
   <si>
     <t>Translation and making of educational videos using a pen tablet</t>
-  </si>
-  <si>
-    <t>olympiad</t>
   </si>
   <si>
     <t>Course for coaches for the Mexican Mathematical Olympiad</t>
@@ -1273,18 +1252,9 @@
     <t>Lion</t>
   </si>
   <si>
-    <t>A great lion</t>
-  </si>
-  <si>
     <t>Vector Art</t>
   </si>
   <si>
-    <t>/goes/to/lion.png</t>
-  </si>
-  <si>
-    <t>red, blue, green</t>
-  </si>
-  <si>
     <t>Book</t>
   </si>
   <si>
@@ -1346,6 +1316,153 @@
   </si>
   <si>
     <t>Newspaper</t>
+  </si>
+  <si>
+    <t>Professor</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>undergraduate, given</t>
+  </si>
+  <si>
+    <t>highschool, taken</t>
+  </si>
+  <si>
+    <t>olympiad, given</t>
+  </si>
+  <si>
+    <t>undergraduate, taken</t>
+  </si>
+  <si>
+    <t>olympiad, taken</t>
+  </si>
+  <si>
+    <t>problem-solving, given</t>
+  </si>
+  <si>
+    <t>California, USA</t>
+  </si>
+  <si>
+    <t>Oaxaca, Mexico</t>
+  </si>
+  <si>
+    <t>Guanajuato, Mexico</t>
+  </si>
+  <si>
+    <t>Aguascalientes, Mexico</t>
+  </si>
+  <si>
+    <t>Campeche, Mexico</t>
+  </si>
+  <si>
+    <t>Teaching Assistant</t>
+  </si>
+  <si>
+    <t>2008+</t>
+  </si>
+  <si>
+    <t>I ate 100 tacos</t>
+  </si>
+  <si>
+    <t>tacos, eating</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Devourer</t>
+  </si>
+  <si>
+    <t>Hungry and fat</t>
+  </si>
+  <si>
+    <t>Eating tacos fair</t>
+  </si>
+  <si>
+    <t>Taco AC</t>
+  </si>
+  <si>
+    <t>Eating tacos olympiad</t>
+  </si>
+  <si>
+    <t>Chef</t>
+  </si>
+  <si>
+    <t>I made 100 tacos</t>
+  </si>
+  <si>
+    <t>red, blue, green, drawing</t>
+  </si>
+  <si>
+    <t>blue, gray, black, drawing</t>
+  </si>
+  <si>
+    <t>Man with Hat</t>
+  </si>
+  <si>
+    <t>Cat in Wall</t>
+  </si>
+  <si>
+    <t>Girl</t>
+  </si>
+  <si>
+    <t>Husky</t>
+  </si>
+  <si>
+    <t>Viena</t>
+  </si>
+  <si>
+    <t>/static/images/lion.png</t>
+  </si>
+  <si>
+    <t>/static/images/manhat.png</t>
+  </si>
+  <si>
+    <t>/static/images/catwall.png</t>
+  </si>
+  <si>
+    <t>/static/images/girl.png</t>
+  </si>
+  <si>
+    <t>/static/images/husky.png</t>
+  </si>
+  <si>
+    <t>/static/images/viena.png</t>
+  </si>
+  <si>
+    <t>drawing</t>
+  </si>
+  <si>
+    <t>Map-man</t>
+  </si>
+  <si>
+    <t>/static/stories/mapman.txt</t>
+  </si>
+  <si>
+    <t>short-story</t>
+  </si>
+  <si>
+    <t>Beer-Sheva Blues</t>
+  </si>
+  <si>
+    <t>/static/scores/score.pdf</t>
+  </si>
+  <si>
+    <t>music, blues</t>
+  </si>
+  <si>
+    <t>Reloj</t>
+  </si>
+  <si>
+    <t>Piano</t>
+  </si>
+  <si>
+    <t>youtube</t>
+  </si>
+  <si>
+    <t>youtube, music</t>
   </si>
 </sst>
 </file>
@@ -1700,8 +1817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4124AE-DF8A-4F61-BE3E-B761EBF17BD8}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1714,105 +1831,105 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="C5" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="B7" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="C7" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="B8" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="B9" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="D9" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="B10" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="D10" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="B12" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="C12" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="B13" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="C13" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="B14" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="C14" t="s">
         <v>83</v>
@@ -1820,125 +1937,125 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="B15" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="C15" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="B16" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="C16" t="s">
+        <v>402</v>
+      </c>
+      <c r="D16" t="s">
         <v>409</v>
-      </c>
-      <c r="D16" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="B18" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B19" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="C19" t="s">
         <v>65</v>
       </c>
       <c r="D19" t="s">
-        <v>423</v>
+        <v>413</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="B20" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="C20" t="s">
         <v>129</v>
       </c>
       <c r="D20" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="B22" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="C22" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="B23" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="C23" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="B24" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="C24" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="D24" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
       <c r="B25" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="B28" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1948,17 +2065,17 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
     </row>
   </sheetData>
@@ -1984,16 +2101,16 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="D1" t="s">
         <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
       <c r="F1" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="G1" t="s">
         <v>135</v>
@@ -2007,16 +2124,16 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="D2" t="s">
         <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F2" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="G2" t="s">
         <v>129</v>
@@ -2304,22 +2421,22 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="D1" t="s">
         <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="F1" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -2330,22 +2447,22 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="D2" t="s">
         <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="F2" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -2353,13 +2470,13 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="C3">
         <v>2015</v>
       </c>
       <c r="G3" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="H3" t="s">
         <v>212</v>
@@ -2370,13 +2487,13 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="C4">
         <v>2015</v>
       </c>
       <c r="G4" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="H4" t="s">
         <v>87</v>
@@ -2387,13 +2504,13 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="C5">
         <v>2014</v>
       </c>
       <c r="G5" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="H5" t="s">
         <v>69</v>
@@ -2404,13 +2521,13 @@
         <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="C6">
         <v>2011</v>
       </c>
       <c r="G6" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="H6" t="s">
         <v>212</v>
@@ -2421,13 +2538,13 @@
         <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="C7">
         <v>2010</v>
       </c>
       <c r="G7" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="H7" t="s">
         <v>212</v>
@@ -2442,7 +2559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BB14F89-81DD-48BF-BD72-6AB1ED9495A4}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -2459,28 +2576,28 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="D1" t="s">
         <v>63</v>
       </c>
       <c r="E1" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="F1" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="I1" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="J1" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -2491,28 +2608,28 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="D2" t="s">
         <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="F2" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="I2" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
       <c r="J2" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -2520,7 +2637,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="C3" s="2">
         <v>2015</v>
@@ -2529,16 +2646,16 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="J3" t="s">
-        <v>437</v>
+        <v>427</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -2546,7 +2663,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="C4" s="2">
         <v>2015</v>
@@ -2555,14 +2672,14 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="J4" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -2570,7 +2687,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="C5" s="2">
         <v>2015</v>
@@ -2579,14 +2696,14 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="J5" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -2594,22 +2711,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="C6">
         <v>2015</v>
       </c>
       <c r="G6" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="J6" t="s">
-        <v>437</v>
+        <v>427</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -2617,20 +2734,20 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="C7">
         <v>2014</v>
       </c>
       <c r="G7" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="J7" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -2638,22 +2755,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="C8">
         <v>2014</v>
       </c>
       <c r="G8" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="J8" t="s">
-        <v>437</v>
+        <v>427</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -2661,22 +2778,22 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="C9">
         <v>2014</v>
       </c>
       <c r="G9" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="J9" t="s">
-        <v>437</v>
+        <v>427</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -2684,20 +2801,20 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="C10">
         <v>2014</v>
       </c>
       <c r="G10" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="J10" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -2705,20 +2822,20 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="C11">
         <v>2014</v>
       </c>
       <c r="G11" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="J11" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -2726,22 +2843,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="C12">
         <v>2014</v>
       </c>
       <c r="G12" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="H12" t="s">
         <v>80</v>
       </c>
       <c r="I12" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="J12" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -2749,22 +2866,22 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="C13">
         <v>2014</v>
       </c>
       <c r="G13" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="I13" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>437</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -2799,28 +2916,28 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="D1" t="s">
         <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="F1" t="s">
         <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="H1" t="s">
-        <v>433</v>
+        <v>423</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
       </c>
       <c r="J1" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="K1" t="s">
         <v>6</v>
@@ -2840,28 +2957,28 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="D2" t="s">
         <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="F2" t="s">
         <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="H2" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
       <c r="I2" t="s">
         <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="K2" t="s">
         <v>7</v>
@@ -2913,7 +3030,7 @@
         <v>2018</v>
       </c>
       <c r="E4" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="I4" t="s">
         <v>33</v>
@@ -2974,7 +3091,7 @@
         <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>434</v>
+        <v>424</v>
       </c>
       <c r="I6" t="s">
         <v>33</v>
@@ -3000,10 +3117,10 @@
         <v>2017</v>
       </c>
       <c r="E7" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="G7" t="s">
-        <v>435</v>
+        <v>425</v>
       </c>
       <c r="I7" t="s">
         <v>44</v>
@@ -3024,7 +3141,7 @@
         <v>2017</v>
       </c>
       <c r="E8" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="I8" t="s">
         <v>48</v>
@@ -3073,7 +3190,7 @@
         <v>2016</v>
       </c>
       <c r="E10" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>43</v>
@@ -3095,7 +3212,7 @@
         <v>2015</v>
       </c>
       <c r="E11" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="F11" t="s">
         <v>56</v>
@@ -3125,7 +3242,7 @@
         <v>2015</v>
       </c>
       <c r="E12" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="F12" t="s">
         <v>57</v>
@@ -3184,7 +3301,7 @@
         <v>2013</v>
       </c>
       <c r="E14" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="F14" t="s">
         <v>58</v>
@@ -3214,7 +3331,7 @@
         <v>2015</v>
       </c>
       <c r="E15" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="I15" t="s">
         <v>167</v>
@@ -3237,7 +3354,7 @@
         <v>2011</v>
       </c>
       <c r="E16" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="I16" t="s">
         <v>168</v>
@@ -3254,23 +3371,23 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="C17">
         <v>2014</v>
       </c>
       <c r="E17" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="I17" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="L17" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -3278,23 +3395,23 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="C18">
         <v>2015</v>
       </c>
       <c r="E18" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="I18" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="L18" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
@@ -3302,23 +3419,23 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="C19">
         <v>2015</v>
       </c>
       <c r="E19" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="I19" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="J19" s="2"/>
       <c r="K19" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="L19" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -3326,23 +3443,23 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="C20">
         <v>2015</v>
       </c>
       <c r="E20" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="I20" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="J20" s="2"/>
       <c r="K20" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="L20" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
@@ -3350,23 +3467,23 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="C21">
         <v>2016</v>
       </c>
       <c r="E21" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="I21" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="J21" s="2"/>
       <c r="K21" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="L21" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
@@ -3374,21 +3491,21 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="C22" s="2">
         <v>2017</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="I22" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="J22" s="2"/>
       <c r="K22" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>38</v>
@@ -3399,14 +3516,14 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="C23" s="2">
         <v>2011</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="I23" t="s">
         <v>168</v>
@@ -3415,13 +3532,13 @@
         <v>69</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
@@ -3429,14 +3546,14 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="C24" s="2">
         <v>2011</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="I24" t="s">
         <v>168</v>
@@ -3445,13 +3562,13 @@
         <v>69</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -3459,14 +3576,14 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="C25" s="2">
         <v>2011</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="I25" t="s">
         <v>168</v>
@@ -3475,7 +3592,7 @@
         <v>87</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="L25">
         <v>52</v>
@@ -3508,13 +3625,13 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="D1" t="s">
         <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="F1" t="s">
         <v>82</v>
@@ -3531,13 +3648,13 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="D2" t="s">
         <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="F2" t="s">
         <v>83</v>
@@ -3813,16 +3930,16 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="D1" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="E1" t="s">
         <v>62</v>
       </c>
       <c r="F1" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="G1" t="s">
         <v>82</v>
@@ -3839,16 +3956,16 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="D2" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="E2" t="s">
         <v>63</v>
       </c>
       <c r="F2" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="G2" t="s">
         <v>83</v>
@@ -3862,7 +3979,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="C3">
         <v>2012</v>
@@ -3871,13 +3988,13 @@
         <v>2016</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="G3" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="H3" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -3885,7 +4002,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="C4">
         <v>2007</v>
@@ -3894,13 +4011,13 @@
         <v>2011</v>
       </c>
       <c r="E4" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="G4" t="s">
         <v>80</v>
       </c>
       <c r="H4" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -3908,7 +4025,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="C5">
         <v>2004</v>
@@ -3917,10 +4034,10 @@
         <v>2007</v>
       </c>
       <c r="G5" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="H5" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -3946,16 +4063,16 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="D1" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="E1" t="s">
         <v>62</v>
       </c>
       <c r="F1" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="G1" t="s">
         <v>82</v>
@@ -3972,16 +4089,16 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="D2" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="E2" t="s">
         <v>63</v>
       </c>
       <c r="F2" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="G2" t="s">
         <v>83</v>
@@ -4001,7 +4118,7 @@
         <v>2016</v>
       </c>
       <c r="D3" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="E3" t="s">
         <v>160</v>
@@ -4010,7 +4127,7 @@
         <v>67</v>
       </c>
       <c r="H3" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -4024,7 +4141,7 @@
         <v>2013</v>
       </c>
       <c r="D4" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="E4" t="s">
         <v>70</v>
@@ -4033,7 +4150,7 @@
         <v>69</v>
       </c>
       <c r="H4" t="s">
-        <v>429</v>
+        <v>419</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -4056,7 +4173,7 @@
         <v>72</v>
       </c>
       <c r="H5" t="s">
-        <v>429</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -4079,7 +4196,7 @@
         <v>74</v>
       </c>
       <c r="H6" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -4102,7 +4219,7 @@
         <v>77</v>
       </c>
       <c r="H7" t="s">
-        <v>429</v>
+        <v>419</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -4125,7 +4242,7 @@
         <v>80</v>
       </c>
       <c r="H8" t="s">
-        <v>429</v>
+        <v>419</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -4133,7 +4250,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="C9" s="2">
         <v>2014</v>
@@ -4142,13 +4259,13 @@
         <v>2015</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="G9" t="s">
         <v>80</v>
       </c>
       <c r="H9" t="s">
-        <v>431</v>
+        <v>421</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -4163,15 +4280,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04072B98-6DD0-4DEA-89F3-ADD9EED64B4B}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4179,25 +4296,28 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>369</v>
+        <v>384</v>
       </c>
       <c r="D1" t="s">
+        <v>385</v>
+      </c>
+      <c r="E1" t="s">
         <v>62</v>
       </c>
-      <c r="E1" t="s">
-        <v>384</v>
-      </c>
       <c r="F1" t="s">
+        <v>377</v>
+      </c>
+      <c r="G1" t="s">
         <v>60</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>231</v>
       </c>
-      <c r="H1" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -4205,22 +4325,83 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>365</v>
+        <v>344</v>
       </c>
       <c r="D2" t="s">
+        <v>345</v>
+      </c>
+      <c r="E2" t="s">
         <v>63</v>
       </c>
-      <c r="E2" t="s">
-        <v>385</v>
-      </c>
       <c r="F2" t="s">
+        <v>378</v>
+      </c>
+      <c r="G2" t="s">
         <v>61</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>232</v>
       </c>
-      <c r="H2" t="s">
-        <v>406</v>
+      <c r="I2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>450</v>
+      </c>
+      <c r="C3">
+        <v>2010</v>
+      </c>
+      <c r="D3">
+        <v>2012</v>
+      </c>
+      <c r="E3" t="s">
+        <v>443</v>
+      </c>
+      <c r="F3" t="s">
+        <v>444</v>
+      </c>
+      <c r="G3" t="s">
+        <v>445</v>
+      </c>
+      <c r="H3" t="s">
+        <v>446</v>
+      </c>
+      <c r="I3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>450</v>
+      </c>
+      <c r="C4">
+        <v>2010</v>
+      </c>
+      <c r="D4">
+        <v>2012</v>
+      </c>
+      <c r="E4" t="s">
+        <v>452</v>
+      </c>
+      <c r="F4" t="s">
+        <v>444</v>
+      </c>
+      <c r="G4" t="s">
+        <v>451</v>
+      </c>
+      <c r="H4" t="s">
+        <v>446</v>
+      </c>
+      <c r="I4" t="s">
+        <v>447</v>
       </c>
     </row>
   </sheetData>
@@ -4230,10 +4411,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A30D27AF-95C4-4435-9869-A417A9206028}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4249,13 +4430,13 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="D1" t="s">
         <v>231</v>
       </c>
       <c r="E1" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="F1" t="s">
         <v>60</v>
@@ -4272,13 +4453,13 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="D2" t="s">
         <v>232</v>
       </c>
       <c r="E2" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="F2" t="s">
         <v>61</v>
@@ -4292,16 +4473,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D3" t="s">
-        <v>233</v>
+        <v>428</v>
       </c>
       <c r="E3" t="s">
-        <v>234</v>
+        <v>430</v>
+      </c>
+      <c r="F3" t="s">
+        <v>419</v>
       </c>
       <c r="G3" t="s">
         <v>212</v>
@@ -4312,16 +4496,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>233</v>
+      </c>
+      <c r="C4" t="s">
         <v>235</v>
       </c>
-      <c r="C4" t="s">
-        <v>237</v>
-      </c>
       <c r="D4" t="s">
-        <v>233</v>
+        <v>428</v>
       </c>
       <c r="E4" t="s">
-        <v>234</v>
+        <v>430</v>
+      </c>
+      <c r="F4" t="s">
+        <v>419</v>
       </c>
       <c r="G4" t="s">
         <v>212</v>
@@ -4332,16 +4519,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D5" t="s">
-        <v>233</v>
+        <v>428</v>
       </c>
       <c r="E5" t="s">
-        <v>234</v>
+        <v>430</v>
+      </c>
+      <c r="F5" t="s">
+        <v>419</v>
       </c>
       <c r="G5" t="s">
         <v>212</v>
@@ -4352,16 +4542,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C6" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D6" t="s">
-        <v>239</v>
+        <v>441</v>
       </c>
       <c r="E6" t="s">
-        <v>234</v>
+        <v>430</v>
+      </c>
+      <c r="F6" t="s">
+        <v>419</v>
       </c>
       <c r="G6" t="s">
         <v>212</v>
@@ -4372,16 +4565,19 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C7" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D7" t="s">
-        <v>239</v>
+        <v>441</v>
       </c>
       <c r="E7" t="s">
-        <v>234</v>
+        <v>430</v>
+      </c>
+      <c r="F7" t="s">
+        <v>419</v>
       </c>
       <c r="G7" t="s">
         <v>212</v>
@@ -4392,16 +4588,19 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D8" t="s">
-        <v>239</v>
+        <v>441</v>
       </c>
       <c r="E8" t="s">
-        <v>234</v>
+        <v>430</v>
+      </c>
+      <c r="F8" t="s">
+        <v>419</v>
       </c>
       <c r="G8" t="s">
         <v>212</v>
@@ -4412,16 +4611,19 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C9" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D9" t="s">
-        <v>239</v>
+        <v>441</v>
       </c>
       <c r="E9" t="s">
-        <v>234</v>
+        <v>430</v>
+      </c>
+      <c r="F9" t="s">
+        <v>419</v>
       </c>
       <c r="G9" t="s">
         <v>212</v>
@@ -4432,16 +4634,19 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C10" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D10" t="s">
-        <v>239</v>
+        <v>441</v>
       </c>
       <c r="E10" t="s">
-        <v>234</v>
+        <v>430</v>
+      </c>
+      <c r="F10" t="s">
+        <v>419</v>
       </c>
       <c r="G10" t="s">
         <v>212</v>
@@ -4452,16 +4657,19 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C11" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D11" t="s">
-        <v>239</v>
+        <v>441</v>
       </c>
       <c r="E11" t="s">
-        <v>234</v>
+        <v>430</v>
+      </c>
+      <c r="F11" t="s">
+        <v>419</v>
       </c>
       <c r="G11" t="s">
         <v>212</v>
@@ -4472,16 +4680,19 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C12" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D12" t="s">
-        <v>239</v>
+        <v>441</v>
       </c>
       <c r="E12" t="s">
-        <v>234</v>
+        <v>430</v>
+      </c>
+      <c r="F12" t="s">
+        <v>419</v>
       </c>
       <c r="G12" t="s">
         <v>212</v>
@@ -4492,16 +4703,19 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C13" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D13" t="s">
-        <v>239</v>
+        <v>441</v>
       </c>
       <c r="E13" t="s">
-        <v>234</v>
+        <v>430</v>
+      </c>
+      <c r="F13" t="s">
+        <v>419</v>
       </c>
       <c r="G13" t="s">
         <v>212</v>
@@ -4512,16 +4726,19 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C14" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D14" t="s">
-        <v>239</v>
+        <v>441</v>
       </c>
       <c r="E14" t="s">
-        <v>234</v>
+        <v>430</v>
+      </c>
+      <c r="F14" t="s">
+        <v>419</v>
       </c>
       <c r="G14" t="s">
         <v>212</v>
@@ -4532,16 +4749,19 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C15" t="s">
-        <v>241</v>
-      </c>
-      <c r="D15" t="s">
-        <v>239</v>
+        <v>238</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>441</v>
       </c>
       <c r="E15" t="s">
-        <v>234</v>
+        <v>430</v>
+      </c>
+      <c r="F15" t="s">
+        <v>419</v>
       </c>
       <c r="G15" t="s">
         <v>212</v>
@@ -4558,13 +4778,16 @@
         <v>2017</v>
       </c>
       <c r="D16" t="s">
-        <v>233</v>
+        <v>428</v>
       </c>
       <c r="E16" t="s">
-        <v>234</v>
+        <v>430</v>
+      </c>
+      <c r="F16" t="s">
+        <v>421</v>
       </c>
       <c r="G16" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -4572,16 +4795,19 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="D17" t="s">
-        <v>233</v>
+        <v>428</v>
       </c>
       <c r="E17" t="s">
-        <v>234</v>
+        <v>430</v>
+      </c>
+      <c r="F17" t="s">
+        <v>421</v>
       </c>
       <c r="G17" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -4589,19 +4815,22 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="C18">
         <v>2013</v>
       </c>
       <c r="D18" t="s">
-        <v>233</v>
+        <v>428</v>
       </c>
       <c r="E18" t="s">
-        <v>257</v>
+        <v>430</v>
+      </c>
+      <c r="F18" t="s">
+        <v>419</v>
       </c>
       <c r="G18" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -4609,19 +4838,22 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C19">
         <v>2006</v>
       </c>
       <c r="D19" t="s">
-        <v>253</v>
+        <v>429</v>
       </c>
       <c r="E19" t="s">
-        <v>255</v>
+        <v>431</v>
+      </c>
+      <c r="F19" t="s">
+        <v>436</v>
       </c>
       <c r="G19" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -4629,19 +4861,22 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="C20">
         <v>2014</v>
       </c>
       <c r="D20" t="s">
-        <v>233</v>
+        <v>428</v>
       </c>
       <c r="E20" t="s">
-        <v>262</v>
+        <v>432</v>
+      </c>
+      <c r="F20" t="s">
+        <v>437</v>
       </c>
       <c r="G20" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -4649,16 +4884,19 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="C21">
         <v>2010</v>
       </c>
       <c r="D21" t="s">
-        <v>233</v>
+        <v>428</v>
       </c>
       <c r="E21" t="s">
-        <v>262</v>
+        <v>432</v>
+      </c>
+      <c r="F21" t="s">
+        <v>438</v>
       </c>
       <c r="G21" t="s">
         <v>223</v>
@@ -4669,16 +4907,19 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="C22">
         <v>2012</v>
       </c>
       <c r="D22" t="s">
-        <v>233</v>
+        <v>428</v>
       </c>
       <c r="E22" t="s">
-        <v>262</v>
+        <v>432</v>
+      </c>
+      <c r="F22" t="s">
+        <v>438</v>
       </c>
       <c r="G22" t="s">
         <v>223</v>
@@ -4689,16 +4930,19 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="C23">
         <v>2014</v>
       </c>
       <c r="D23" t="s">
-        <v>233</v>
+        <v>428</v>
       </c>
       <c r="E23" t="s">
-        <v>262</v>
+        <v>432</v>
+      </c>
+      <c r="F23" t="s">
+        <v>438</v>
       </c>
       <c r="G23" t="s">
         <v>223</v>
@@ -4709,16 +4953,22 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="C24" t="s">
-        <v>267</v>
+        <v>442</v>
       </c>
       <c r="D24" t="s">
-        <v>233</v>
+        <v>428</v>
       </c>
       <c r="E24" t="s">
-        <v>262</v>
+        <v>432</v>
+      </c>
+      <c r="F24" t="s">
+        <v>420</v>
+      </c>
+      <c r="G24" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -4726,19 +4976,22 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="C25">
         <v>2010</v>
       </c>
       <c r="D25" t="s">
-        <v>233</v>
+        <v>428</v>
       </c>
       <c r="E25" t="s">
+        <v>432</v>
+      </c>
+      <c r="F25" t="s">
+        <v>439</v>
+      </c>
+      <c r="G25" t="s">
         <v>262</v>
-      </c>
-      <c r="G25" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -4746,16 +4999,19 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="C26">
         <v>2015</v>
       </c>
       <c r="D26" t="s">
-        <v>253</v>
+        <v>429</v>
       </c>
       <c r="E26" t="s">
-        <v>234</v>
+        <v>433</v>
+      </c>
+      <c r="F26" t="s">
+        <v>421</v>
       </c>
       <c r="G26" t="s">
         <v>223</v>
@@ -4766,16 +5022,19 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="C27">
         <v>2014</v>
       </c>
       <c r="D27" t="s">
-        <v>253</v>
+        <v>429</v>
       </c>
       <c r="E27" t="s">
-        <v>234</v>
+        <v>433</v>
+      </c>
+      <c r="F27" t="s">
+        <v>438</v>
       </c>
       <c r="G27" t="s">
         <v>223</v>
@@ -4786,16 +5045,19 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="C28">
         <v>2010</v>
       </c>
       <c r="D28" t="s">
-        <v>253</v>
+        <v>429</v>
       </c>
       <c r="E28" t="s">
-        <v>234</v>
+        <v>433</v>
+      </c>
+      <c r="F28" t="s">
+        <v>438</v>
       </c>
       <c r="G28" t="s">
         <v>223</v>
@@ -4806,16 +5068,19 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="C29">
         <v>2009</v>
       </c>
       <c r="D29" t="s">
-        <v>253</v>
+        <v>429</v>
       </c>
       <c r="E29" t="s">
-        <v>262</v>
+        <v>434</v>
+      </c>
+      <c r="F29" t="s">
+        <v>438</v>
       </c>
       <c r="G29" t="s">
         <v>223</v>
@@ -4826,19 +5091,22 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="C30">
         <v>2008</v>
       </c>
       <c r="D30" t="s">
-        <v>253</v>
+        <v>429</v>
       </c>
       <c r="E30" t="s">
-        <v>262</v>
+        <v>434</v>
+      </c>
+      <c r="F30" t="s">
+        <v>440</v>
       </c>
       <c r="G30" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -4846,16 +5114,19 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="C31">
         <v>2008</v>
       </c>
       <c r="D31" t="s">
-        <v>253</v>
+        <v>429</v>
       </c>
       <c r="E31" t="s">
-        <v>262</v>
+        <v>434</v>
+      </c>
+      <c r="F31" t="s">
+        <v>438</v>
       </c>
       <c r="G31" t="s">
         <v>223</v>
@@ -4866,20 +5137,26 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="C32">
         <v>2015</v>
       </c>
       <c r="D32" t="s">
-        <v>233</v>
+        <v>428</v>
       </c>
       <c r="E32" t="s">
-        <v>405</v>
+        <v>435</v>
+      </c>
+      <c r="F32" t="s">
+        <v>421</v>
       </c>
       <c r="G32" t="s">
         <v>229</v>
       </c>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F33" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4888,10 +5165,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F22342A-9809-473D-ADB1-AF47B630B508}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4904,13 +5181,13 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="D1" t="s">
         <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="F1" t="s">
         <v>60</v>
@@ -4919,7 +5196,7 @@
         <v>231</v>
       </c>
       <c r="H1" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="I1" t="s">
         <v>82</v>
@@ -4933,13 +5210,13 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="D2" t="s">
         <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="F2" t="s">
         <v>61</v>
@@ -4948,10 +5225,39 @@
         <v>232</v>
       </c>
       <c r="H2" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="I2" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>448</v>
+      </c>
+      <c r="C3">
+        <v>2011</v>
+      </c>
+      <c r="D3" t="s">
+        <v>443</v>
+      </c>
+      <c r="E3" t="s">
+        <v>444</v>
+      </c>
+      <c r="F3" t="s">
+        <v>445</v>
+      </c>
+      <c r="G3" t="s">
+        <v>446</v>
+      </c>
+      <c r="H3" t="s">
+        <v>447</v>
+      </c>
+      <c r="I3" t="s">
+        <v>449</v>
       </c>
     </row>
   </sheetData>
@@ -4977,22 +5283,22 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="D1" t="s">
         <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="F1" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="G1" t="s">
         <v>60</v>
       </c>
       <c r="H1" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="I1" t="s">
         <v>82</v>
@@ -5006,22 +5312,22 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="D2" t="s">
         <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="F2" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="G2" t="s">
         <v>61</v>
       </c>
       <c r="H2" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="I2" t="s">
         <v>83</v>
@@ -5038,7 +5344,7 @@
         <v>2017</v>
       </c>
       <c r="F3" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="G3" t="s">
         <v>178</v>
@@ -5058,7 +5364,7 @@
         <v>2016</v>
       </c>
       <c r="F4" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="G4" t="s">
         <v>177</v>
@@ -5078,7 +5384,7 @@
         <v>2016</v>
       </c>
       <c r="F5" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="G5" t="s">
         <v>85</v>
@@ -5098,7 +5404,7 @@
         <v>2016</v>
       </c>
       <c r="F6" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="G6" t="s">
         <v>182</v>
@@ -5121,7 +5427,7 @@
         <v>2015</v>
       </c>
       <c r="F7" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="G7" t="s">
         <v>184</v>
@@ -5141,7 +5447,7 @@
         <v>2014</v>
       </c>
       <c r="F8" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="G8" t="s">
         <v>186</v>
@@ -5161,10 +5467,10 @@
         <v>2013</v>
       </c>
       <c r="F9" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="G9" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="H9" t="s">
         <v>183</v>
@@ -5359,7 +5665,7 @@
         <v>187</v>
       </c>
       <c r="G18" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="H18" t="s">
         <v>228</v>
@@ -5425,7 +5731,7 @@
         <v>2015</v>
       </c>
       <c r="F21" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="G21" t="s">
         <v>203</v>
@@ -5448,7 +5754,7 @@
         <v>2015</v>
       </c>
       <c r="F22" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="G22" t="s">
         <v>177</v>
@@ -5468,7 +5774,7 @@
         <v>2014</v>
       </c>
       <c r="F23" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="G23" t="s">
         <v>210</v>
@@ -5491,7 +5797,7 @@
         <v>2014</v>
       </c>
       <c r="F24" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="G24" t="s">
         <v>101</v>
@@ -5514,7 +5820,7 @@
         <v>2014</v>
       </c>
       <c r="F25" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="G25" t="s">
         <v>216</v>
@@ -5537,7 +5843,7 @@
         <v>2014</v>
       </c>
       <c r="F26" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="G26" t="s">
         <v>219</v>
@@ -5557,7 +5863,7 @@
         <v>2014</v>
       </c>
       <c r="F27" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="G27" t="s">
         <v>89</v>
@@ -5580,10 +5886,10 @@
         <v>2013</v>
       </c>
       <c r="F28" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="G28" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="H28" t="s">
         <v>202</v>
@@ -5603,10 +5909,10 @@
         <v>2013</v>
       </c>
       <c r="F29" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="G29" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="H29" t="s">
         <v>218</v>
@@ -5623,7 +5929,7 @@
         <v>2013</v>
       </c>
       <c r="F30" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="G30" t="s">
         <v>101</v>
@@ -5646,7 +5952,7 @@
         <v>2012</v>
       </c>
       <c r="F31" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="G31" t="s">
         <v>89</v>
@@ -5663,19 +5969,19 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="C32">
         <v>2015</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="G32" t="s">
         <v>207</v>
       </c>
       <c r="H32" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="I32" t="s">
         <v>205</v>
@@ -5686,13 +5992,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="C33">
         <v>2015</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="G33" t="s">
         <v>225</v>
@@ -5706,22 +6012,22 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="C34">
         <v>2015</v>
       </c>
       <c r="F34" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="G34" t="s">
         <v>329</v>
       </c>
-      <c r="G34" t="s">
-        <v>336</v>
-      </c>
       <c r="H34" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="I34" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -5729,19 +6035,19 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="C35">
         <v>2015</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="G35" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="I35" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
@@ -5749,19 +6055,19 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="C36">
         <v>2014</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="G36" t="s">
         <v>101</v>
       </c>
       <c r="H36" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="I36" t="s">
         <v>197</v>
@@ -5772,13 +6078,13 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="C37">
         <v>2014</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="G37" t="s">
         <v>225</v>
@@ -5792,19 +6098,19 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="C38">
         <v>2014</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="G38" t="s">
         <v>177</v>
       </c>
       <c r="I38" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
@@ -5812,16 +6118,16 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="C39">
         <v>2013</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="G39" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="H39" t="s">
         <v>202</v>
@@ -5832,13 +6138,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="C40">
         <v>2012</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="G40" t="s">
         <v>89</v>
@@ -5852,22 +6158,22 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="C41">
         <v>2013</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="G41" t="s">
         <v>89</v>
       </c>
       <c r="H41" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="I41" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
@@ -5875,19 +6181,19 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="C42">
         <v>2013</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="G42" t="s">
         <v>101</v>
       </c>
       <c r="H42" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="I42" t="s">
         <v>197</v>
@@ -5898,22 +6204,22 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="C43">
         <v>2013</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="G43" t="s">
         <v>101</v>
       </c>
       <c r="H43" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="I43" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -5924,10 +6230,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE156D2-7E33-4447-A53C-1EA25432072D}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5940,16 +6246,16 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="D1" t="s">
         <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="F1" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="G1" t="s">
         <v>64</v>
@@ -5963,16 +6269,16 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="D2" t="s">
         <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="F2" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="G2" t="s">
         <v>65</v>
@@ -5983,25 +6289,180 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="C3">
         <v>2017</v>
       </c>
-      <c r="D3" t="s">
-        <v>413</v>
-      </c>
       <c r="E3" t="s">
-        <v>415</v>
+        <v>460</v>
       </c>
       <c r="F3" t="s">
-        <v>416</v>
+        <v>453</v>
       </c>
       <c r="G3" t="s">
-        <v>414</v>
+        <v>406</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>455</v>
+      </c>
+      <c r="C4">
+        <v>2017</v>
+      </c>
+      <c r="E4" t="s">
+        <v>461</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>456</v>
+      </c>
+      <c r="C5">
+        <v>2017</v>
+      </c>
+      <c r="E5" t="s">
+        <v>462</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="G5" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>457</v>
+      </c>
+      <c r="C6">
+        <v>2017</v>
+      </c>
+      <c r="E6" t="s">
+        <v>463</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>458</v>
+      </c>
+      <c r="C7">
+        <v>2017</v>
+      </c>
+      <c r="E7" t="s">
+        <v>464</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="G7" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>459</v>
+      </c>
+      <c r="C8">
+        <v>2017</v>
+      </c>
+      <c r="E8" t="s">
+        <v>465</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>467</v>
+      </c>
+      <c r="C9">
+        <v>2018</v>
+      </c>
+      <c r="E9" t="s">
+        <v>468</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>470</v>
+      </c>
+      <c r="C10">
+        <v>2018</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>473</v>
+      </c>
+      <c r="C11">
+        <v>2018</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="G11" t="s">
+        <v>474</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Responsive Bootstrap big update
- New .goodie to get items
- Deprecated the .J .Y etc tags. Now it is managed by Bootstrap
- Slide to go to section on click
- Better responsiveness
</commit_message>
<xml_diff>
--- a/data/CV.xlsx
+++ b/data/CV.xlsx
@@ -1549,6 +1549,21 @@
     <t>SNI Conacyt Visualization</t>
   </si>
   <si>
+    <t>Youtube</t>
+  </si>
+  <si>
+    <t>/static/scores/Blues-Beer-Sheva.pdf</t>
+  </si>
+  <si>
+    <t>This should embed YouTube videos</t>
+  </si>
+  <si>
+    <t>Interesting video</t>
+  </si>
+  <si>
+    <t>xfr64zoBTAQ</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sentado bajo el viejo sauce retorcido donde descubrí mis poderes, miré una vez más la minúscula cantidad de ceros que tenía el cheque expedido por la Súper Escuadra Heroica. Recordé con forzada nostalgia la breve docena de años en que mi visión hyperterrenal me permitió realizar hazañas consideradas como espectaculares como cerrar los párpados para describir la geografía precisa de mis alrededores y trazar caminos óptimos entre dos puntos lejanos con la facilidad con la que un universitario resuelve un laberinto para niños en la caja del cereal.&lt;br&gt;&lt;br&gt;
 Las cosas no habían salido como pensaba. Ser Mapman parecía tener un perfil de bajo riesgo. A diferencia de los héroes al frente de la línea de batalla, yo era partícipe principalmente de las reuniones de táctica y estrategia. Tras hacer mis cuentas a lápiz y calculadora, había concluido que podía permanecer activo como hasta los sesenta o sesenta y cinco, después de lo cual la Súper Escuadra Heroica me otorgaría una pensión nada despreciable. Pero tras el recorte efectuado en la institución debido a una serie de legislaciones vendidas por políticos como una prometedora reforma tecnológica, las entidades como la Súper Escuadra Heroica no sólo tenían permiso, sino incluso jugosos estímulos fiscales para substituir a sus empleados por algoritmos, computadoras y toscos robots humanoides que, aunque fueran más feos, eran más eficientes.&lt;br&gt;&lt;br&gt;
 A falta de habilidades de liderazgo (como las de mi colega Smartman), de una fisionomía sorprendente (como la de Bigman) o de llamativos poderes de colores (como los de Flameboy o Sparkgirl), me encontré en una precaria situación laboral. Había pocos empleos que coincidieran con mi particular capacidad. Sólo pude circular de rojo con un desgastado crayón bicolor dos ofertas de empleo en el periódico que había arrugado por frustración y tirado junto al sauce.&lt;br&gt;
@@ -1559,24 +1574,9 @@
 El gran trabajo de Mapman le dio a la pizzería un auge de popularidad espectacular. El fenómeno llegó a tal grado que un importante y agradable Científico Ejecutivo de Compucorp llamó para pedir la famosa receta de champiñones con emmental en su versión familiar. Al enterarse de a dónde había que entregar el manjar, Mapman dudó en querer realizar la entrega. Pero el amplio sentido de responsabilidad que había desarrollado en la Súper Escuadra Heroica y su deseo por mantener impecable su récord pesaron más en la balanza. Subió a la moto y en un abrir y cerrar de ojos llegó a las magníficas y modernas instalaciones de la antagónica corporación.&lt;br&gt;&lt;br&gt;
 El Científico Ejecutivo no lo podía creer. Por pura curiosidad, hábito del oficio, había decidido medir el tiempo de entrega. Él estaba a cargo del algoritmo cuántico del problema de trayectoria mínima y esta entrega superaba por varias desviaciones estándar las simulaciones incluso bajo las hipótesis más optimistas. Además, si los avances que habían presentado sus colegas en la última Conferencia Nacional de Aproximaciones Automatizadas se concretaban, este tiempo récord podía tener históricas implicaciones en el algoritmo de Optimización de Liderazgo, un problema hasta ahora en la categoría de NHP-difíciles. &lt;br&gt;&lt;br&gt;
 Con su más carismático vocabulario pidió a Mapman quedarse para un recorrido por los laboratorios. Lo mejor que pudo obtener fueron dos escépticos minutos de su atención. Mediante el más conciso y seductor vocabulario explicó de las maravillas creadas en Compucorp y de sus sensacionales condiciones laborales. Prometió compartir una medalla Startech y la garantía de ascender sin dificultad alguna en la escalera de estímulos del Sistema Nacional de Diseñadores Algorítmicos. Mapman despreció todo esto y preparaba sus cosas para irse, pero los últimos segundos del discurso se quedaron resonando en sus oídos: “En fin”, dijo el Científico Ejecutivo, “exactamente lo que necesita alguien que merece una gran vida. Piénsalo.”&lt;br&gt;&lt;br&gt;
-El único día en que quebré mi inigualable entrega de pedidos fue un par de meses después de la visita a Compucorp, un cálido martes de agosto. Al trazar la ruta óptima para el pedido no me di cuenta de que pasaría frente a mi sauce. Al ver el follaje amarillo de mi compañero de vida, un pensamiento me paralizó como un relámpago insoportable. Invadió mi mente con más fuerza que cualquier imagen que mi poder me hubiera mostrado jamás. Tuve que frenar. Me resultó imposible quitarme de la mente el pensamiento del otoño de la vida. Recordé mi épica primavera y eso me hizo dudar si estaba viviendo mi verano como quería. Pensó en mis colegas de la Escuadra. Pensé en el chef de Pizzaplace. Y sobre todo pensé en aquellas palabras que meses antes se habían sembrado en mi mente como una semilla.&lt;br&gt;
+El único día en que quebré mi inigualable entrega de pedidos fue un par de meses después de la visita a Compucorp, un cálido martes de agosto. Al trazar la ruta óptima para el pedido no me di cuenta de que pasaría frente a mi sauce. Al ver el follaje amarillo de mi compañero de vida, un pensamiento me paralizó como un relámpago insoportable. Invadió mi mente con más fuerza que cualquier imagen que mi poder me hubiera mostrado jamás. Tuve que frenar. Me resultó imposible quitarme de la mente el pensamiento del otoño de la vida. Recordé mi épica primavera y eso me hizo dudar si estaba viviendo mi verano como quería. Pensó en mis colegas de la Escuadra. Pensé en el chef de Pizzaplace. Y sobre todo pensé en aquellas palabras que meses antes se habían sembrado en mi mente como una semilla.&lt;br&gt;&lt;br&gt;
 Bajé de mi motocicleta y la dejé recargada bajo el árbol. Boté el casco sobre las hojas caídas. Cerré los ojos para usar mi poder por tercera vez en el día y comencé mi camino.
 </t>
-  </si>
-  <si>
-    <t>Youtube</t>
-  </si>
-  <si>
-    <t>/static/scores/Blues-Beer-Sheva.pdf</t>
-  </si>
-  <si>
-    <t>This should embed YouTube videos</t>
-  </si>
-  <si>
-    <t>Interesting video</t>
-  </si>
-  <si>
-    <t>xfr64zoBTAQ</t>
   </si>
 </sst>
 </file>
@@ -6564,8 +6564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE156D2-7E33-4447-A53C-1EA25432072D}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6587,7 +6587,7 @@
         <v>385</v>
       </c>
       <c r="F1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G1" t="s">
         <v>368</v>
@@ -6753,7 +6753,7 @@
         <v>2018</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>505</v>
+        <v>510</v>
       </c>
       <c r="E9" t="s">
         <v>457</v>
@@ -6766,18 +6766,21 @@
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
-        <v>459</v>
-      </c>
-      <c r="C10">
+      <c r="B10" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="C10" s="2">
         <v>2018</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>509</v>
+      </c>
       <c r="G10" s="2" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>461</v>
@@ -6787,23 +6790,21 @@
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
-        <v>509</v>
-      </c>
-      <c r="C11">
+      <c r="B11" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="C11" s="2">
         <v>2018</v>
       </c>
-      <c r="D11" t="s">
-        <v>508</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2" t="s">
-        <v>510</v>
-      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="F11" s="2"/>
       <c r="G11" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="H11" t="s">
+        <v>460</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>461</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CV Database updated as of today
- Added Service worksheet
- Added participation in math contests and various service activities
</commit_message>
<xml_diff>
--- a/data/CV.xlsx
+++ b/data/CV.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9048" tabRatio="714" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9048" tabRatio="714" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONFIG" sheetId="11" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="Job" sheetId="3" r:id="rId4"/>
     <sheet name="Contest" sheetId="13" r:id="rId5"/>
     <sheet name="Course" sheetId="8" r:id="rId6"/>
-    <sheet name="ScienceFair" sheetId="14" r:id="rId7"/>
-    <sheet name="Talk" sheetId="2" r:id="rId8"/>
-    <sheet name="ArtItem" sheetId="6" r:id="rId9"/>
-    <sheet name="CodingItem" sheetId="4" r:id="rId10"/>
-    <sheet name="Book" sheetId="12" r:id="rId11"/>
-    <sheet name="MainstreamMedia" sheetId="10" r:id="rId12"/>
-    <sheet name="ScientificPublication" sheetId="1" r:id="rId13"/>
+    <sheet name="Service" sheetId="16" r:id="rId7"/>
+    <sheet name="ScienceFair" sheetId="17" r:id="rId8"/>
+    <sheet name="Talk" sheetId="2" r:id="rId9"/>
+    <sheet name="ArtItem" sheetId="6" r:id="rId10"/>
+    <sheet name="CodingItem" sheetId="4" r:id="rId11"/>
+    <sheet name="Book" sheetId="12" r:id="rId12"/>
+    <sheet name="MainstreamMedia" sheetId="10" r:id="rId13"/>
+    <sheet name="ScientificPublication" sheetId="1" r:id="rId14"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="618">
   <si>
     <t>ID</t>
   </si>
@@ -1120,9 +1121,6 @@
   </si>
   <si>
     <t>Event</t>
-  </si>
-  <si>
-    <t>location,role</t>
   </si>
   <si>
     <t>Education</t>
@@ -1330,34 +1328,7 @@
     <t>2008+</t>
   </si>
   <si>
-    <t>I ate 100 tacos</t>
-  </si>
-  <si>
-    <t>tacos, eating</t>
-  </si>
-  <si>
     <t>Mexico</t>
-  </si>
-  <si>
-    <t>Devourer</t>
-  </si>
-  <si>
-    <t>Hungry and fat</t>
-  </si>
-  <si>
-    <t>Eating tacos fair</t>
-  </si>
-  <si>
-    <t>Taco AC</t>
-  </si>
-  <si>
-    <t>Eating tacos olympiad</t>
-  </si>
-  <si>
-    <t>Chef</t>
-  </si>
-  <si>
-    <t>I made 100 tacos</t>
   </si>
   <si>
     <t>red, blue, green, drawing</t>
@@ -1577,6 +1548,357 @@
 El único día en que quebré mi inigualable entrega de pedidos fue un par de meses después de la visita a Compucorp, un cálido martes de agosto. Al trazar la ruta óptima para el pedido no me di cuenta de que pasaría frente a mi sauce. Al ver el follaje amarillo de mi compañero de vida, un pensamiento me paralizó como un relámpago insoportable. Invadió mi mente con más fuerza que cualquier imagen que mi poder me hubiera mostrado jamás. Tuve que frenar. Me resultó imposible quitarme de la mente el pensamiento del otoño de la vida. Recordé mi épica primavera y eso me hizo dudar si estaba viviendo mi verano como quería. Pensó en mis colegas de la Escuadra. Pensé en el chef de Pizzaplace. Y sobre todo pensé en aquellas palabras que meses antes se habían sembrado en mi mente como una semilla.&lt;br&gt;&lt;br&gt;
 Bajé de mi motocicleta y la dejé recargada bajo el árbol. Boté el casco sobre las hojas caídas. Cerré los ojos para usar mi poder por tercera vez en el día y comencé mi camino.
 </t>
+  </si>
+  <si>
+    <t>International competition for undergraduate students in Latin America</t>
+  </si>
+  <si>
+    <t>Asian Pacific Mathematics Olympiad</t>
+  </si>
+  <si>
+    <t>High-school</t>
+  </si>
+  <si>
+    <t>Undergraduate</t>
+  </si>
+  <si>
+    <t>apmo, olympiad, high-school</t>
+  </si>
+  <si>
+    <t>Long Distance</t>
+  </si>
+  <si>
+    <t>Contestant</t>
+  </si>
+  <si>
+    <t>Team Leader</t>
+  </si>
+  <si>
+    <t>Chair Organizer</t>
+  </si>
+  <si>
+    <t>Annual competition for students in the Asian-Pacific region and the Americas</t>
+  </si>
+  <si>
+    <t>Ecuador, Mexico, Colombia, Costa Rica</t>
+  </si>
+  <si>
+    <t>Zacatecas, Mexico</t>
+  </si>
+  <si>
+    <t>Gold Medalist</t>
+  </si>
+  <si>
+    <t>Organizing Committee</t>
+  </si>
+  <si>
+    <t>Founder and Organizing Committee</t>
+  </si>
+  <si>
+    <t>Resolución de Problemas y Concursos Matemáticos Universitarios, UNAM</t>
+  </si>
+  <si>
+    <t>Whole project in problem-solving and partitipation in mathematical contests for undergraduate students.</t>
+  </si>
+  <si>
+    <t>Olimpiada de Matemáticas del Distrito Federal</t>
+  </si>
+  <si>
+    <t>Mexico City annual mathematics competition</t>
+  </si>
+  <si>
+    <t>Olimpiada Iberoamericana Interuniversitaria de Matemáticas</t>
+  </si>
+  <si>
+    <t>Long-distance mathematical competition for undergraduate students</t>
+  </si>
+  <si>
+    <t>oimu, undergraduate</t>
+  </si>
+  <si>
+    <t>UNAM Representative</t>
+  </si>
+  <si>
+    <t>Silver Medalist</t>
+  </si>
+  <si>
+    <t>oimu, undegraduate</t>
+  </si>
+  <si>
+    <t>Olimpiada Iberoamericana de Matemáticas</t>
+  </si>
+  <si>
+    <t>Annual competition for high-school students in Latin-America</t>
+  </si>
+  <si>
+    <t>Romanian Masters in Mathematics</t>
+  </si>
+  <si>
+    <t>International Mathematics Competition for University Students</t>
+  </si>
+  <si>
+    <t>Olimpiada Centroamericana de Matemáticas</t>
+  </si>
+  <si>
+    <t>Deputy Leader</t>
+  </si>
+  <si>
+    <t>Observer C</t>
+  </si>
+  <si>
+    <t>Coordinator</t>
+  </si>
+  <si>
+    <t>IMO, high-school</t>
+  </si>
+  <si>
+    <t>IMC, undergraduate</t>
+  </si>
+  <si>
+    <t>Romania</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Argentina, Colombia, South Africa, Thailand</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>Puerto Rico</t>
+  </si>
+  <si>
+    <t>Mathematical competition for the best teams in the world</t>
+  </si>
+  <si>
+    <t>centro, highschool</t>
+  </si>
+  <si>
+    <t>omm, olympiad, high-school</t>
+  </si>
+  <si>
+    <t>oimu, ciim, imc, undergraduate</t>
+  </si>
+  <si>
+    <t>omdf, omcdmx, highschool</t>
+  </si>
+  <si>
+    <t>ibero, high-school</t>
+  </si>
+  <si>
+    <t>romanian, highschool</t>
+  </si>
+  <si>
+    <t>olympiad, undergraduate, organization</t>
+  </si>
+  <si>
+    <t>Deputy Leaders accompany students, grade their papers and coordinate the final scores.</t>
+  </si>
+  <si>
+    <t>Team Leaders select the paper problems, approve marking schemes, do what Deputy Leaders do, among other things.</t>
+  </si>
+  <si>
+    <t>Observers C follow the same program as Team Leaders</t>
+  </si>
+  <si>
+    <t>Largest open international competition for undergraduate students. Team leaders select the problems and mark the papers.</t>
+  </si>
+  <si>
+    <t>Coordinators prepare marking schemes, grade the papers and coordinate the results with Team Leaders</t>
+  </si>
+  <si>
+    <t>International competition for young students in CentroAmerica</t>
+  </si>
+  <si>
+    <t>Coach</t>
+  </si>
+  <si>
+    <t>Panamá Mathematical Olympiad</t>
+  </si>
+  <si>
+    <t>Part of the international olympiad coaches</t>
+  </si>
+  <si>
+    <t>Annual competition for mexican students. Several roles including: web administrator, olympiad coach, coordinator, chief coordinator, problem selection committee</t>
+  </si>
+  <si>
+    <t>Annual competition for mexican students.</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>Concurso Nacional de Matemáticas Pierre Fermat</t>
+  </si>
+  <si>
+    <t>Mathematical contest organized by Instituto Politécnico Nacional</t>
+  </si>
+  <si>
+    <t>undergraduate</t>
+  </si>
+  <si>
+    <t>high-school</t>
+  </si>
+  <si>
+    <t>First Place</t>
+  </si>
+  <si>
+    <t>Concurso de Problemas</t>
+  </si>
+  <si>
+    <t>Problem creation contest</t>
+  </si>
+  <si>
+    <t>problem, undergraduate</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>location, role</t>
+  </si>
+  <si>
+    <t>Reviewer</t>
+  </si>
+  <si>
+    <t>Book by Radmila Bulajich Manfrino, José Antonio Gómez Ortega, Rogelio Valdez Delgado</t>
+  </si>
+  <si>
+    <t>Algebra: The basis of the mathematical olympiad</t>
+  </si>
+  <si>
+    <t>Principio de las casillas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problem solving methods in combinatorics </t>
+  </si>
+  <si>
+    <t>Álgebra</t>
+  </si>
+  <si>
+    <t>Inequalities</t>
+  </si>
+  <si>
+    <t>Desigualdades</t>
+  </si>
+  <si>
+    <t>Combinatoria para olimpiadas internacionales</t>
+  </si>
+  <si>
+    <t>Book by José Antonio Gómez, Rogelio Valdez Delgado, Rita Vázquez Padilla</t>
+  </si>
+  <si>
+    <t>Book by Pablo Soberón</t>
+  </si>
+  <si>
+    <t>algebra</t>
+  </si>
+  <si>
+    <t>combinatorics</t>
+  </si>
+  <si>
+    <t>2016 - 2018</t>
+  </si>
+  <si>
+    <t>SoCG '17, SoCG '18, EuroCG '18</t>
+  </si>
+  <si>
+    <t>SIAGA, Sci. Math. Hungarica</t>
+  </si>
+  <si>
+    <t>Various Locations</t>
+  </si>
+  <si>
+    <t>Thesis Reviewer</t>
+  </si>
+  <si>
+    <t>Thesis by David Rivera Bermúdez</t>
+  </si>
+  <si>
+    <t>Polímeros aleatorios suaves en dimensión 1.</t>
+  </si>
+  <si>
+    <t>research</t>
+  </si>
+  <si>
+    <t>conference</t>
+  </si>
+  <si>
+    <t>Fiesta de las Ciencias</t>
+  </si>
+  <si>
+    <t>Science fair</t>
+  </si>
+  <si>
+    <t>science</t>
+  </si>
+  <si>
+    <t>Concyteq</t>
+  </si>
+  <si>
+    <t>Expocyteq</t>
+  </si>
+  <si>
+    <t>Leader of IM-UNAM</t>
+  </si>
+  <si>
+    <t>2014 - 2015</t>
+  </si>
+  <si>
+    <t>Aquelarre Matemático UAQ</t>
+  </si>
+  <si>
+    <t>Academic conference for undergraduate students</t>
+  </si>
+  <si>
+    <t>UNAM and UAQ</t>
+  </si>
+  <si>
+    <t>Various research papers</t>
+  </si>
+  <si>
+    <t>Various conference papers</t>
+  </si>
+  <si>
+    <t>Check papers for originality, presentation and relevance</t>
+  </si>
+  <si>
+    <t>Mathematics fair</t>
+  </si>
+  <si>
+    <t>math</t>
+  </si>
+  <si>
+    <t>Volunteer</t>
+  </si>
+  <si>
+    <t>General Public</t>
+  </si>
+  <si>
+    <t>Matemáticas en la calle</t>
+  </si>
+  <si>
+    <t>Festival Matemático en Morelos</t>
+  </si>
+  <si>
+    <t>Festival Matemático</t>
+  </si>
+  <si>
+    <t>Morelos, Mexico</t>
+  </si>
+  <si>
+    <t>Freshman Undergraduates</t>
+  </si>
+  <si>
+    <t>SMM</t>
   </si>
 </sst>
 </file>
@@ -1929,10 +2251,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4124AE-DF8A-4F61-BE3E-B761EBF17BD8}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1964,7 +2286,7 @@
         <v>343</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1972,7 +2294,7 @@
         <v>346</v>
       </c>
       <c r="C5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1996,24 +2318,24 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B9" t="s">
         <v>360</v>
       </c>
       <c r="D9" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B10" t="s">
         <v>360</v>
       </c>
       <c r="D10" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -2024,18 +2346,18 @@
         <v>346</v>
       </c>
       <c r="C12" t="s">
-        <v>363</v>
+        <v>572</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B13" t="s">
         <v>362</v>
       </c>
       <c r="C13" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -2051,151 +2373,162 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>395</v>
+        <v>571</v>
       </c>
       <c r="B15" t="s">
         <v>362</v>
       </c>
       <c r="C15" t="s">
-        <v>393</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>371</v>
+        <v>394</v>
       </c>
       <c r="B16" t="s">
         <v>362</v>
       </c>
       <c r="C16" t="s">
-        <v>393</v>
-      </c>
-      <c r="D16" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>365</v>
-      </c>
-      <c r="B18" t="s">
-        <v>346</v>
+        <v>389</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>370</v>
+      </c>
+      <c r="B17" t="s">
+        <v>362</v>
+      </c>
+      <c r="C17" t="s">
+        <v>392</v>
+      </c>
+      <c r="D17" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B19" t="s">
-        <v>365</v>
-      </c>
-      <c r="C19" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" t="s">
-        <v>404</v>
+        <v>346</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="B20" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C20" t="s">
-        <v>124</v>
+        <v>65</v>
       </c>
       <c r="D20" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>347</v>
-      </c>
-      <c r="B22" t="s">
-        <v>346</v>
-      </c>
-      <c r="C22" t="s">
-        <v>350</v>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>369</v>
+      </c>
+      <c r="B21" t="s">
+        <v>364</v>
+      </c>
+      <c r="C21" t="s">
+        <v>124</v>
+      </c>
+      <c r="D21" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="B23" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C23" t="s">
-        <v>386</v>
+        <v>350</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="B24" t="s">
         <v>347</v>
       </c>
       <c r="C24" t="s">
-        <v>356</v>
-      </c>
-      <c r="D24" t="s">
-        <v>405</v>
+        <v>385</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>398</v>
+        <v>348</v>
       </c>
       <c r="B25" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>357</v>
+      <c r="C25" t="s">
+        <v>356</v>
+      </c>
+      <c r="D25" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>397</v>
+      </c>
+      <c r="B26" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>339</v>
-      </c>
-      <c r="B28" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>338</v>
+        <v>339</v>
+      </c>
+      <c r="B29" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>338</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>359</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>373</v>
+        <v>359</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>367</v>
-      </c>
-      <c r="B33" s="1"/>
+        <v>372</v>
+      </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>462</v>
+        <v>366</v>
+      </c>
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>452</v>
       </c>
     </row>
   </sheetData>
@@ -2204,6 +2537,260 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE156D2-7E33-4447-A53C-1EA25432072D}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>353</v>
+      </c>
+      <c r="D1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s">
+        <v>384</v>
+      </c>
+      <c r="F1" t="s">
+        <v>495</v>
+      </c>
+      <c r="G1" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>349</v>
+      </c>
+      <c r="D2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" t="s">
+        <v>372</v>
+      </c>
+      <c r="F2" t="s">
+        <v>452</v>
+      </c>
+      <c r="G2" t="s">
+        <v>368</v>
+      </c>
+      <c r="H2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>395</v>
+      </c>
+      <c r="C3">
+        <v>2017</v>
+      </c>
+      <c r="E3" t="s">
+        <v>439</v>
+      </c>
+      <c r="G3" t="s">
+        <v>432</v>
+      </c>
+      <c r="H3" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>434</v>
+      </c>
+      <c r="C4">
+        <v>2017</v>
+      </c>
+      <c r="E4" t="s">
+        <v>440</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>435</v>
+      </c>
+      <c r="C5">
+        <v>2017</v>
+      </c>
+      <c r="E5" t="s">
+        <v>441</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="H5" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>436</v>
+      </c>
+      <c r="C6">
+        <v>2017</v>
+      </c>
+      <c r="E6" t="s">
+        <v>442</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>437</v>
+      </c>
+      <c r="C7">
+        <v>2017</v>
+      </c>
+      <c r="E7" t="s">
+        <v>443</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="H7" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>438</v>
+      </c>
+      <c r="C8">
+        <v>2017</v>
+      </c>
+      <c r="E8" t="s">
+        <v>444</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>446</v>
+      </c>
+      <c r="C9">
+        <v>2018</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="E9" t="s">
+        <v>447</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2018</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2018</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>451</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94D0DD9B-3A24-4EEE-B532-5A3AF00D7B57}">
   <dimension ref="A1:H15"/>
   <sheetViews>
@@ -2230,13 +2817,13 @@
         <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="H1" t="s">
         <v>129</v>
@@ -2256,13 +2843,13 @@
         <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H2" t="s">
         <v>124</v>
@@ -2282,7 +2869,7 @@
         <v>119</v>
       </c>
       <c r="F3" t="s">
-        <v>493</v>
+        <v>483</v>
       </c>
       <c r="G3" t="s">
         <v>125</v>
@@ -2305,7 +2892,7 @@
         <v>148</v>
       </c>
       <c r="F4" t="s">
-        <v>493</v>
+        <v>483</v>
       </c>
       <c r="G4" t="s">
         <v>125</v>
@@ -2325,7 +2912,7 @@
         <v>2017</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>495</v>
+        <v>485</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -2395,7 +2982,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" t="s">
-        <v>494</v>
+        <v>484</v>
       </c>
       <c r="H8" t="s">
         <v>135</v>
@@ -2475,7 +3062,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>504</v>
+        <v>494</v>
       </c>
       <c r="C12">
         <v>2016</v>
@@ -2502,7 +3089,7 @@
         <v>2010</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>497</v>
+        <v>487</v>
       </c>
       <c r="E13" s="2"/>
       <c r="G13" t="s">
@@ -2517,19 +3104,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>491</v>
+        <v>481</v>
       </c>
       <c r="C14">
         <v>2018</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>496</v>
+        <v>486</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>492</v>
+        <v>482</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>493</v>
+        <v>483</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>144</v>
@@ -2556,7 +3143,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E9DC452-8FB8-48D7-9200-F8DA05DAADE9}">
   <dimension ref="A1:H7"/>
   <sheetViews>
@@ -2583,10 +3170,10 @@
         <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -2609,10 +3196,10 @@
         <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
@@ -2711,7 +3298,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BB14F89-81DD-48BF-BD72-6AB1ED9495A4}">
   <dimension ref="A1:J13"/>
   <sheetViews>
@@ -2738,10 +3325,10 @@
         <v>63</v>
       </c>
       <c r="E1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -2770,10 +3357,10 @@
         <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
@@ -2782,7 +3369,7 @@
         <v>299</v>
       </c>
       <c r="I2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="J2" t="s">
         <v>355</v>
@@ -2811,7 +3398,7 @@
         <v>281</v>
       </c>
       <c r="J3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -2835,7 +3422,7 @@
         <v>282</v>
       </c>
       <c r="J4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -2859,7 +3446,7 @@
         <v>282</v>
       </c>
       <c r="J5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -2882,7 +3469,7 @@
         <v>281</v>
       </c>
       <c r="J6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -2903,7 +3490,7 @@
         <v>282</v>
       </c>
       <c r="J7" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -2926,7 +3513,7 @@
         <v>281</v>
       </c>
       <c r="J8" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -2949,7 +3536,7 @@
         <v>281</v>
       </c>
       <c r="J9" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -2970,7 +3557,7 @@
         <v>282</v>
       </c>
       <c r="J10" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -2991,7 +3578,7 @@
         <v>282</v>
       </c>
       <c r="J11" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -3014,7 +3601,7 @@
         <v>291</v>
       </c>
       <c r="J12" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3037,7 +3624,7 @@
         <v>281</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -3045,12 +3632,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3078,7 +3665,7 @@
         <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F1" t="s">
         <v>12</v>
@@ -3087,7 +3674,7 @@
         <v>337</v>
       </c>
       <c r="H1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -3119,7 +3706,7 @@
         <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F2" t="s">
         <v>13</v>
@@ -3128,7 +3715,7 @@
         <v>338</v>
       </c>
       <c r="H2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="I2" t="s">
         <v>5</v>
@@ -3282,7 +3869,7 @@
         <v>2017</v>
       </c>
       <c r="E7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I7" t="s">
         <v>44</v>
@@ -3358,7 +3945,7 @@
         <v>2016</v>
       </c>
       <c r="E10" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G10">
         <v>1612.0343499999999</v>
@@ -3383,7 +3970,7 @@
         <v>2015</v>
       </c>
       <c r="E11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F11" t="s">
         <v>56</v>
@@ -3413,7 +4000,7 @@
         <v>2015</v>
       </c>
       <c r="E12" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F12" t="s">
         <v>57</v>
@@ -3475,7 +4062,7 @@
         <v>2013</v>
       </c>
       <c r="E14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F14" t="s">
         <v>58</v>
@@ -3551,10 +4138,10 @@
         <v>2014</v>
       </c>
       <c r="E17" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>466</v>
+        <v>456</v>
       </c>
       <c r="I17" t="s">
         <v>254</v>
@@ -3578,10 +4165,10 @@
         <v>2015</v>
       </c>
       <c r="E18" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>467</v>
+        <v>457</v>
       </c>
       <c r="I18" t="s">
         <v>254</v>
@@ -3605,10 +4192,10 @@
         <v>2015</v>
       </c>
       <c r="E19" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>468</v>
+        <v>458</v>
       </c>
       <c r="I19" t="s">
         <v>254</v>
@@ -3632,10 +4219,10 @@
         <v>2015</v>
       </c>
       <c r="E20" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>469</v>
+        <v>459</v>
       </c>
       <c r="I20" t="s">
         <v>254</v>
@@ -3659,7 +4246,7 @@
         <v>2016</v>
       </c>
       <c r="E21" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I21" t="s">
         <v>254</v>
@@ -3684,7 +4271,7 @@
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I22" t="s">
         <v>254</v>
@@ -3709,7 +4296,7 @@
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I23" t="s">
         <v>160</v>
@@ -3739,7 +4326,7 @@
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I24" t="s">
         <v>160</v>
@@ -3769,10 +4356,10 @@
       </c>
       <c r="D25" s="2"/>
       <c r="E25" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>470</v>
+        <v>460</v>
       </c>
       <c r="I25" t="s">
         <v>160</v>
@@ -3792,7 +4379,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>464</v>
+        <v>454</v>
       </c>
       <c r="C26" s="2">
         <v>2015</v>
@@ -3804,7 +4391,7 @@
         <v>1505.0517</v>
       </c>
       <c r="I26" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>45</v>
@@ -3850,7 +4437,7 @@
         <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F1" t="s">
         <v>82</v>
@@ -3873,7 +4460,7 @@
         <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F2" t="s">
         <v>83</v>
@@ -4136,7 +4723,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4149,16 +4736,16 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>374</v>
+      </c>
+      <c r="D1" t="s">
         <v>375</v>
-      </c>
-      <c r="D1" t="s">
-        <v>376</v>
       </c>
       <c r="E1" t="s">
         <v>62</v>
       </c>
       <c r="F1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G1" t="s">
         <v>82</v>
@@ -4184,7 +4771,7 @@
         <v>63</v>
       </c>
       <c r="F2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G2" t="s">
         <v>83</v>
@@ -4198,7 +4785,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C3">
         <v>2012</v>
@@ -4207,13 +4794,13 @@
         <v>2016</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="G3" t="s">
         <v>379</v>
       </c>
-      <c r="G3" t="s">
-        <v>380</v>
-      </c>
       <c r="H3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -4221,7 +4808,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C4">
         <v>2007</v>
@@ -4230,13 +4817,13 @@
         <v>2011</v>
       </c>
       <c r="E4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G4" t="s">
         <v>80</v>
       </c>
       <c r="H4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -4244,7 +4831,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C5">
         <v>2004</v>
@@ -4253,14 +4840,15 @@
         <v>2007</v>
       </c>
       <c r="G5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4282,16 +4870,16 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>374</v>
+      </c>
+      <c r="D1" t="s">
         <v>375</v>
-      </c>
-      <c r="D1" t="s">
-        <v>376</v>
       </c>
       <c r="E1" t="s">
         <v>62</v>
       </c>
       <c r="F1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G1" t="s">
         <v>82</v>
@@ -4317,7 +4905,7 @@
         <v>63</v>
       </c>
       <c r="F2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G2" t="s">
         <v>83</v>
@@ -4337,7 +4925,7 @@
         <v>2016</v>
       </c>
       <c r="D3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E3" t="s">
         <v>152</v>
@@ -4346,7 +4934,7 @@
         <v>67</v>
       </c>
       <c r="H3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -4360,7 +4948,7 @@
         <v>2013</v>
       </c>
       <c r="D4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E4" t="s">
         <v>70</v>
@@ -4369,7 +4957,7 @@
         <v>69</v>
       </c>
       <c r="H4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -4392,7 +4980,7 @@
         <v>72</v>
       </c>
       <c r="H5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -4415,7 +5003,7 @@
         <v>74</v>
       </c>
       <c r="H6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -4438,7 +5026,7 @@
         <v>77</v>
       </c>
       <c r="H7" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -4461,7 +5049,7 @@
         <v>80</v>
       </c>
       <c r="H8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -4484,7 +5072,7 @@
         <v>80</v>
       </c>
       <c r="H9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -4499,13 +5087,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04072B98-6DD0-4DEA-89F3-ADD9EED64B4B}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="44.109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -4515,16 +5106,16 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>374</v>
+      </c>
+      <c r="D1" t="s">
         <v>375</v>
-      </c>
-      <c r="D1" t="s">
-        <v>376</v>
       </c>
       <c r="E1" t="s">
         <v>62</v>
       </c>
       <c r="F1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G1" t="s">
         <v>60</v>
@@ -4533,7 +5124,7 @@
         <v>222</v>
       </c>
       <c r="I1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -4553,7 +5144,7 @@
         <v>63</v>
       </c>
       <c r="F2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G2" t="s">
         <v>61</v>
@@ -4562,7 +5153,7 @@
         <v>223</v>
       </c>
       <c r="I2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -4570,57 +5161,777 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>439</v>
+        <v>98</v>
       </c>
       <c r="C3">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="D3">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="E3" t="s">
-        <v>432</v>
+        <v>501</v>
       </c>
       <c r="F3" t="s">
-        <v>433</v>
+        <v>550</v>
       </c>
       <c r="G3" t="s">
-        <v>434</v>
+        <v>562</v>
       </c>
       <c r="H3" t="s">
-        <v>435</v>
+        <v>513</v>
       </c>
       <c r="I3" t="s">
-        <v>436</v>
+        <v>504</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>439</v>
+        <v>98</v>
       </c>
       <c r="C4">
         <v>2010</v>
       </c>
       <c r="D4">
+        <v>2010</v>
+      </c>
+      <c r="E4" t="s">
+        <v>501</v>
+      </c>
+      <c r="F4" t="s">
+        <v>550</v>
+      </c>
+      <c r="G4" t="s">
+        <v>540</v>
+      </c>
+      <c r="H4" t="s">
+        <v>524</v>
+      </c>
+      <c r="I4" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5">
+        <v>2011</v>
+      </c>
+      <c r="D5">
+        <v>2014</v>
+      </c>
+      <c r="E5" t="s">
+        <v>501</v>
+      </c>
+      <c r="F5" t="s">
+        <v>550</v>
+      </c>
+      <c r="G5" t="s">
+        <v>511</v>
+      </c>
+      <c r="H5" t="s">
+        <v>508</v>
+      </c>
+      <c r="I5" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6">
+        <v>2015</v>
+      </c>
+      <c r="D6">
+        <v>2015</v>
+      </c>
+      <c r="E6" t="s">
+        <v>501</v>
+      </c>
+      <c r="F6" t="s">
+        <v>550</v>
+      </c>
+      <c r="G6" t="s">
+        <v>431</v>
+      </c>
+      <c r="H6" t="s">
+        <v>509</v>
+      </c>
+      <c r="I6" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>502</v>
+      </c>
+      <c r="C7">
+        <v>2007</v>
+      </c>
+      <c r="D7">
+        <v>2007</v>
+      </c>
+      <c r="E7" t="s">
+        <v>510</v>
+      </c>
+      <c r="F7" t="s">
+        <v>505</v>
+      </c>
+      <c r="G7" t="s">
+        <v>506</v>
+      </c>
+      <c r="H7" t="s">
+        <v>507</v>
+      </c>
+      <c r="I7" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>502</v>
+      </c>
+      <c r="C8">
+        <v>2016</v>
+      </c>
+      <c r="D8">
+        <v>2018</v>
+      </c>
+      <c r="E8" t="s">
+        <v>510</v>
+      </c>
+      <c r="F8" t="s">
+        <v>505</v>
+      </c>
+      <c r="G8" t="s">
+        <v>506</v>
+      </c>
+      <c r="H8" t="s">
+        <v>71</v>
+      </c>
+      <c r="I8" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9">
+        <v>2007</v>
+      </c>
+      <c r="D9">
+        <v>2007</v>
+      </c>
+      <c r="E9" t="s">
+        <v>561</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="I9" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10">
+        <v>2009</v>
+      </c>
+      <c r="D10">
+        <v>2018</v>
+      </c>
+      <c r="E10" t="s">
+        <v>560</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="I10" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>516</v>
+      </c>
+      <c r="C11">
+        <v>2011</v>
+      </c>
+      <c r="D11">
+        <v>2018</v>
+      </c>
+      <c r="E11" t="s">
+        <v>517</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="I11" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>518</v>
+      </c>
+      <c r="C12">
+        <v>2007</v>
+      </c>
+      <c r="D12">
+        <v>2010</v>
+      </c>
+      <c r="E12" t="s">
+        <v>519</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>518</v>
+      </c>
+      <c r="C13">
+        <v>2006</v>
+      </c>
+      <c r="D13">
+        <v>2006</v>
+      </c>
+      <c r="E13" t="s">
+        <v>519</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>520</v>
+      </c>
+      <c r="C14">
+        <v>2011</v>
+      </c>
+      <c r="D14">
+        <v>2015</v>
+      </c>
+      <c r="E14" t="s">
+        <v>521</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>520</v>
+      </c>
+      <c r="C15">
+        <v>2009</v>
+      </c>
+      <c r="D15">
+        <v>2009</v>
+      </c>
+      <c r="E15" t="s">
+        <v>521</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="H15" t="s">
+        <v>524</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>526</v>
+      </c>
+      <c r="C16">
+        <v>2009</v>
+      </c>
+      <c r="D16">
+        <v>2009</v>
+      </c>
+      <c r="E16" t="s">
+        <v>527</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>528</v>
+      </c>
+      <c r="C17">
+        <v>2017</v>
+      </c>
+      <c r="D17">
+        <v>2017</v>
+      </c>
+      <c r="E17" t="s">
+        <v>543</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="H17" t="s">
+        <v>508</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18">
+        <v>2011</v>
+      </c>
+      <c r="D18">
+        <v>2011</v>
+      </c>
+      <c r="E18" t="s">
+        <v>551</v>
+      </c>
+      <c r="F18" t="s">
+        <v>534</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="H18" t="s">
+        <v>531</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19">
         <v>2012</v>
       </c>
-      <c r="E4" t="s">
-        <v>441</v>
-      </c>
-      <c r="F4" t="s">
-        <v>433</v>
-      </c>
-      <c r="G4" t="s">
-        <v>440</v>
-      </c>
-      <c r="H4" t="s">
-        <v>435</v>
-      </c>
-      <c r="I4" t="s">
-        <v>436</v>
+      <c r="D19">
+        <v>2015</v>
+      </c>
+      <c r="E19" t="s">
+        <v>552</v>
+      </c>
+      <c r="F19" t="s">
+        <v>534</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="H19" t="s">
+        <v>508</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20">
+        <v>2016</v>
+      </c>
+      <c r="D20">
+        <v>2016</v>
+      </c>
+      <c r="E20" t="s">
+        <v>553</v>
+      </c>
+      <c r="F20" t="s">
+        <v>534</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="H20" t="s">
+        <v>532</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21">
+        <v>2017</v>
+      </c>
+      <c r="D21">
+        <v>2017</v>
+      </c>
+      <c r="E21" t="s">
+        <v>555</v>
+      </c>
+      <c r="F21" t="s">
+        <v>534</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="H21" t="s">
+        <v>533</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>529</v>
+      </c>
+      <c r="C22">
+        <v>2013</v>
+      </c>
+      <c r="D22">
+        <v>2015</v>
+      </c>
+      <c r="E22" t="s">
+        <v>554</v>
+      </c>
+      <c r="F22" t="s">
+        <v>535</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="H22" t="s">
+        <v>508</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>530</v>
+      </c>
+      <c r="C23">
+        <v>2010</v>
+      </c>
+      <c r="D23">
+        <v>2010</v>
+      </c>
+      <c r="E23" t="s">
+        <v>556</v>
+      </c>
+      <c r="F23" t="s">
+        <v>544</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="H23" t="s">
+        <v>531</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>530</v>
+      </c>
+      <c r="C24">
+        <v>2011</v>
+      </c>
+      <c r="D24">
+        <v>2011</v>
+      </c>
+      <c r="E24" t="s">
+        <v>556</v>
+      </c>
+      <c r="F24" t="s">
+        <v>544</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="H24" t="s">
+        <v>533</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>558</v>
+      </c>
+      <c r="C25">
+        <v>2010</v>
+      </c>
+      <c r="D25">
+        <v>2010</v>
+      </c>
+      <c r="E25" t="s">
+        <v>559</v>
+      </c>
+      <c r="H25" t="s">
+        <v>557</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>563</v>
+      </c>
+      <c r="C26">
+        <v>2006</v>
+      </c>
+      <c r="D26">
+        <v>2006</v>
+      </c>
+      <c r="E26" t="s">
+        <v>564</v>
+      </c>
+      <c r="F26" t="s">
+        <v>566</v>
+      </c>
+      <c r="G26" t="s">
+        <v>431</v>
+      </c>
+      <c r="H26" t="s">
+        <v>102</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>563</v>
+      </c>
+      <c r="C27">
+        <v>2007</v>
+      </c>
+      <c r="D27">
+        <v>2007</v>
+      </c>
+      <c r="E27" t="s">
+        <v>564</v>
+      </c>
+      <c r="F27" t="s">
+        <v>566</v>
+      </c>
+      <c r="G27" t="s">
+        <v>431</v>
+      </c>
+      <c r="H27" t="s">
+        <v>567</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>563</v>
+      </c>
+      <c r="C28">
+        <v>2008</v>
+      </c>
+      <c r="D28">
+        <v>2008</v>
+      </c>
+      <c r="E28" t="s">
+        <v>564</v>
+      </c>
+      <c r="F28" t="s">
+        <v>565</v>
+      </c>
+      <c r="G28" t="s">
+        <v>431</v>
+      </c>
+      <c r="H28" t="s">
+        <v>567</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>568</v>
+      </c>
+      <c r="C29">
+        <v>2010</v>
+      </c>
+      <c r="D29">
+        <v>2010</v>
+      </c>
+      <c r="E29" t="s">
+        <v>569</v>
+      </c>
+      <c r="F29" t="s">
+        <v>570</v>
+      </c>
+      <c r="G29" t="s">
+        <v>431</v>
+      </c>
+      <c r="H29" t="s">
+        <v>567</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>504</v>
       </c>
     </row>
   </sheetData>
@@ -4656,7 +5967,7 @@
         <v>222</v>
       </c>
       <c r="E1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F1" t="s">
         <v>60</v>
@@ -4679,7 +5990,7 @@
         <v>223</v>
       </c>
       <c r="E2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F2" t="s">
         <v>61</v>
@@ -4699,13 +6010,13 @@
         <v>225</v>
       </c>
       <c r="D3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G3" t="s">
         <v>203</v>
@@ -4722,13 +6033,13 @@
         <v>226</v>
       </c>
       <c r="D4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G4" t="s">
         <v>203</v>
@@ -4745,13 +6056,13 @@
         <v>227</v>
       </c>
       <c r="D5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G5" t="s">
         <v>203</v>
@@ -4768,13 +6079,13 @@
         <v>230</v>
       </c>
       <c r="D6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G6" t="s">
         <v>203</v>
@@ -4791,13 +6102,13 @@
         <v>226</v>
       </c>
       <c r="D7" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E7" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F7" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G7" t="s">
         <v>203</v>
@@ -4814,13 +6125,13 @@
         <v>233</v>
       </c>
       <c r="D8" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E8" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G8" t="s">
         <v>203</v>
@@ -4837,13 +6148,13 @@
         <v>227</v>
       </c>
       <c r="D9" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E9" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F9" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G9" t="s">
         <v>203</v>
@@ -4860,13 +6171,13 @@
         <v>240</v>
       </c>
       <c r="D10" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F10" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G10" t="s">
         <v>203</v>
@@ -4883,13 +6194,13 @@
         <v>230</v>
       </c>
       <c r="D11" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E11" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F11" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G11" t="s">
         <v>203</v>
@@ -4906,13 +6217,13 @@
         <v>229</v>
       </c>
       <c r="D12" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E12" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F12" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G12" t="s">
         <v>203</v>
@@ -4929,13 +6240,13 @@
         <v>233</v>
       </c>
       <c r="D13" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E13" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F13" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G13" t="s">
         <v>203</v>
@@ -4952,13 +6263,13 @@
         <v>226</v>
       </c>
       <c r="D14" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E14" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F14" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G14" t="s">
         <v>203</v>
@@ -4975,13 +6286,13 @@
         <v>229</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E15" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F15" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G15" t="s">
         <v>203</v>
@@ -4998,13 +6309,13 @@
         <v>2017</v>
       </c>
       <c r="D16" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E16" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F16" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G16" t="s">
         <v>244</v>
@@ -5018,13 +6329,13 @@
         <v>243</v>
       </c>
       <c r="D17" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F17" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G17" t="s">
         <v>244</v>
@@ -5041,13 +6352,13 @@
         <v>2013</v>
       </c>
       <c r="D18" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E18" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G18" t="s">
         <v>245</v>
@@ -5064,13 +6375,13 @@
         <v>2006</v>
       </c>
       <c r="D19" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E19" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F19" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G19" t="s">
         <v>241</v>
@@ -5087,13 +6398,13 @@
         <v>2014</v>
       </c>
       <c r="D20" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E20" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F20" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G20" t="s">
         <v>248</v>
@@ -5110,13 +6421,13 @@
         <v>2010</v>
       </c>
       <c r="D21" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E21" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F21" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G21" t="s">
         <v>214</v>
@@ -5133,13 +6444,13 @@
         <v>2012</v>
       </c>
       <c r="D22" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E22" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F22" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G22" t="s">
         <v>214</v>
@@ -5156,13 +6467,13 @@
         <v>2014</v>
       </c>
       <c r="D23" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E23" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F23" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G23" t="s">
         <v>214</v>
@@ -5176,16 +6487,16 @@
         <v>250</v>
       </c>
       <c r="C24" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D24" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E24" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F24" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G24" t="s">
         <v>251</v>
@@ -5202,13 +6513,13 @@
         <v>2010</v>
       </c>
       <c r="D25" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E25" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F25" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G25" t="s">
         <v>253</v>
@@ -5225,13 +6536,13 @@
         <v>2015</v>
       </c>
       <c r="D26" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E26" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F26" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G26" t="s">
         <v>214</v>
@@ -5248,13 +6559,13 @@
         <v>2014</v>
       </c>
       <c r="D27" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E27" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F27" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G27" t="s">
         <v>214</v>
@@ -5271,13 +6582,13 @@
         <v>2010</v>
       </c>
       <c r="D28" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E28" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F28" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G28" t="s">
         <v>214</v>
@@ -5294,13 +6605,13 @@
         <v>2009</v>
       </c>
       <c r="D29" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E29" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F29" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G29" t="s">
         <v>214</v>
@@ -5317,13 +6628,13 @@
         <v>2008</v>
       </c>
       <c r="D30" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E30" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F30" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G30" t="s">
         <v>333</v>
@@ -5340,13 +6651,13 @@
         <v>2008</v>
       </c>
       <c r="D31" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E31" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F31" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G31" t="s">
         <v>214</v>
@@ -5357,19 +6668,19 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C32">
         <v>2015</v>
       </c>
       <c r="D32" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E32" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F32" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G32" t="s">
         <v>220</v>
@@ -5384,11 +6695,340 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F22342A-9809-473D-ADB1-AF47B630B508}">
-  <dimension ref="A1:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D107D88-62EE-4992-AFEF-BB9D7FB2D529}">
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="34.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>353</v>
+      </c>
+      <c r="D1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s">
+        <v>367</v>
+      </c>
+      <c r="F1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" t="s">
+        <v>222</v>
+      </c>
+      <c r="H1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>349</v>
+      </c>
+      <c r="D2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" t="s">
+        <v>368</v>
+      </c>
+      <c r="F2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" t="s">
+        <v>223</v>
+      </c>
+      <c r="H2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>575</v>
+      </c>
+      <c r="D3" t="s">
+        <v>574</v>
+      </c>
+      <c r="E3" t="s">
+        <v>584</v>
+      </c>
+      <c r="F3" t="s">
+        <v>409</v>
+      </c>
+      <c r="G3" t="s">
+        <v>573</v>
+      </c>
+      <c r="H3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>576</v>
+      </c>
+      <c r="D4" t="s">
+        <v>582</v>
+      </c>
+      <c r="E4" t="s">
+        <v>585</v>
+      </c>
+      <c r="F4" t="s">
+        <v>409</v>
+      </c>
+      <c r="G4" t="s">
+        <v>573</v>
+      </c>
+      <c r="H4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>577</v>
+      </c>
+      <c r="D5" t="s">
+        <v>583</v>
+      </c>
+      <c r="E5" t="s">
+        <v>585</v>
+      </c>
+      <c r="F5" t="s">
+        <v>409</v>
+      </c>
+      <c r="G5" t="s">
+        <v>573</v>
+      </c>
+      <c r="H5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>578</v>
+      </c>
+      <c r="D6" t="s">
+        <v>574</v>
+      </c>
+      <c r="E6" t="s">
+        <v>584</v>
+      </c>
+      <c r="F6" t="s">
+        <v>409</v>
+      </c>
+      <c r="G6" t="s">
+        <v>573</v>
+      </c>
+      <c r="H6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>579</v>
+      </c>
+      <c r="D7" t="s">
+        <v>574</v>
+      </c>
+      <c r="E7" t="s">
+        <v>584</v>
+      </c>
+      <c r="F7" t="s">
+        <v>409</v>
+      </c>
+      <c r="G7" t="s">
+        <v>573</v>
+      </c>
+      <c r="H7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>580</v>
+      </c>
+      <c r="D8" t="s">
+        <v>574</v>
+      </c>
+      <c r="E8" t="s">
+        <v>584</v>
+      </c>
+      <c r="F8" t="s">
+        <v>409</v>
+      </c>
+      <c r="G8" t="s">
+        <v>573</v>
+      </c>
+      <c r="H8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>581</v>
+      </c>
+      <c r="D9" t="s">
+        <v>583</v>
+      </c>
+      <c r="E9" t="s">
+        <v>585</v>
+      </c>
+      <c r="F9" t="s">
+        <v>409</v>
+      </c>
+      <c r="G9" t="s">
+        <v>573</v>
+      </c>
+      <c r="H9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>605</v>
+      </c>
+      <c r="C10" t="s">
+        <v>586</v>
+      </c>
+      <c r="D10" t="s">
+        <v>607</v>
+      </c>
+      <c r="E10" t="s">
+        <v>593</v>
+      </c>
+      <c r="F10" t="s">
+        <v>589</v>
+      </c>
+      <c r="H10" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>606</v>
+      </c>
+      <c r="C11" t="s">
+        <v>586</v>
+      </c>
+      <c r="D11" t="s">
+        <v>607</v>
+      </c>
+      <c r="E11" t="s">
+        <v>594</v>
+      </c>
+      <c r="F11" t="s">
+        <v>589</v>
+      </c>
+      <c r="H11" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>592</v>
+      </c>
+      <c r="C12">
+        <v>2016</v>
+      </c>
+      <c r="D12" t="s">
+        <v>591</v>
+      </c>
+      <c r="E12" t="s">
+        <v>267</v>
+      </c>
+      <c r="F12" t="s">
+        <v>409</v>
+      </c>
+      <c r="G12" t="s">
+        <v>590</v>
+      </c>
+      <c r="H12" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>602</v>
+      </c>
+      <c r="C13">
+        <v>2014</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="E13" t="s">
+        <v>594</v>
+      </c>
+      <c r="F13" t="s">
+        <v>411</v>
+      </c>
+      <c r="G13" t="s">
+        <v>514</v>
+      </c>
+      <c r="H13" t="s">
+        <v>604</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F434878D-D55F-47A4-AC18-D55001D3C372}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5407,7 +7047,7 @@
         <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F1" t="s">
         <v>60</v>
@@ -5416,7 +7056,7 @@
         <v>222</v>
       </c>
       <c r="H1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I1" t="s">
         <v>82</v>
@@ -5436,7 +7076,7 @@
         <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F2" t="s">
         <v>61</v>
@@ -5445,7 +7085,7 @@
         <v>223</v>
       </c>
       <c r="H2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I2" t="s">
         <v>83</v>
@@ -5456,28 +7096,202 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>437</v>
+        <v>595</v>
       </c>
       <c r="C3">
+        <v>2014</v>
+      </c>
+      <c r="D3" t="s">
+        <v>596</v>
+      </c>
+      <c r="E3" t="s">
+        <v>597</v>
+      </c>
+      <c r="F3" t="s">
+        <v>411</v>
+      </c>
+      <c r="G3" t="s">
+        <v>600</v>
+      </c>
+      <c r="H3" t="s">
+        <v>611</v>
+      </c>
+      <c r="I3" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>599</v>
+      </c>
+      <c r="C4" t="s">
+        <v>601</v>
+      </c>
+      <c r="D4" t="s">
+        <v>596</v>
+      </c>
+      <c r="E4" t="s">
+        <v>597</v>
+      </c>
+      <c r="F4" t="s">
+        <v>411</v>
+      </c>
+      <c r="G4" t="s">
+        <v>600</v>
+      </c>
+      <c r="H4" t="s">
+        <v>611</v>
+      </c>
+      <c r="I4" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>327</v>
+      </c>
+      <c r="C5">
+        <v>2013</v>
+      </c>
+      <c r="D5" t="s">
+        <v>608</v>
+      </c>
+      <c r="E5" t="s">
+        <v>609</v>
+      </c>
+      <c r="F5" t="s">
+        <v>409</v>
+      </c>
+      <c r="G5" t="s">
+        <v>610</v>
+      </c>
+      <c r="H5" t="s">
+        <v>611</v>
+      </c>
+      <c r="I5" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>612</v>
+      </c>
+      <c r="C6">
+        <v>2012</v>
+      </c>
+      <c r="D6" t="s">
+        <v>608</v>
+      </c>
+      <c r="E6" t="s">
+        <v>609</v>
+      </c>
+      <c r="F6" t="s">
+        <v>411</v>
+      </c>
+      <c r="G6" t="s">
+        <v>610</v>
+      </c>
+      <c r="H6" t="s">
+        <v>611</v>
+      </c>
+      <c r="I6" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>613</v>
+      </c>
+      <c r="C7">
+        <v>2012</v>
+      </c>
+      <c r="D7" t="s">
+        <v>608</v>
+      </c>
+      <c r="E7" t="s">
+        <v>609</v>
+      </c>
+      <c r="F7" t="s">
+        <v>615</v>
+      </c>
+      <c r="G7" t="s">
+        <v>610</v>
+      </c>
+      <c r="H7" t="s">
+        <v>611</v>
+      </c>
+      <c r="I7" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>614</v>
+      </c>
+      <c r="C8">
+        <v>2012</v>
+      </c>
+      <c r="D8" t="s">
+        <v>608</v>
+      </c>
+      <c r="E8" t="s">
+        <v>609</v>
+      </c>
+      <c r="F8" t="s">
+        <v>409</v>
+      </c>
+      <c r="G8" t="s">
+        <v>514</v>
+      </c>
+      <c r="H8" t="s">
+        <v>611</v>
+      </c>
+      <c r="I8" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>614</v>
+      </c>
+      <c r="C9">
         <v>2011</v>
       </c>
-      <c r="D3" t="s">
-        <v>432</v>
-      </c>
-      <c r="E3" t="s">
-        <v>433</v>
-      </c>
-      <c r="F3" t="s">
-        <v>434</v>
-      </c>
-      <c r="G3" t="s">
-        <v>435</v>
-      </c>
-      <c r="H3" t="s">
-        <v>436</v>
-      </c>
-      <c r="I3" t="s">
-        <v>438</v>
+      <c r="D9" t="s">
+        <v>608</v>
+      </c>
+      <c r="E9" t="s">
+        <v>609</v>
+      </c>
+      <c r="F9" t="s">
+        <v>409</v>
+      </c>
+      <c r="G9" t="s">
+        <v>514</v>
+      </c>
+      <c r="H9" t="s">
+        <v>616</v>
+      </c>
+      <c r="I9" t="s">
+        <v>473</v>
       </c>
     </row>
   </sheetData>
@@ -5485,7 +7299,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{820DCA41-7065-4B6F-8FCC-B838DB872725}">
   <dimension ref="A1:I45"/>
   <sheetViews>
@@ -5515,16 +7329,16 @@
         <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G1" t="s">
         <v>60</v>
       </c>
       <c r="H1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I1" t="s">
         <v>82</v>
@@ -5544,16 +7358,16 @@
         <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G2" t="s">
         <v>61</v>
       </c>
       <c r="H2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I2" t="s">
         <v>83</v>
@@ -5579,7 +7393,7 @@
         <v>49</v>
       </c>
       <c r="I3" t="s">
-        <v>484</v>
+        <v>474</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -5613,7 +7427,7 @@
         <v>2016</v>
       </c>
       <c r="E5" t="s">
-        <v>471</v>
+        <v>461</v>
       </c>
       <c r="F5" t="s">
         <v>302</v>
@@ -5625,7 +7439,7 @@
         <v>171</v>
       </c>
       <c r="I5" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -5639,7 +7453,7 @@
         <v>2016</v>
       </c>
       <c r="E6" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="F6" t="s">
         <v>302</v>
@@ -5648,7 +7462,7 @@
         <v>173</v>
       </c>
       <c r="H6" t="s">
-        <v>485</v>
+        <v>475</v>
       </c>
       <c r="I6" t="s">
         <v>172</v>
@@ -5665,7 +7479,7 @@
         <v>2015</v>
       </c>
       <c r="E7" t="s">
-        <v>488</v>
+        <v>478</v>
       </c>
       <c r="F7" t="s">
         <v>302</v>
@@ -5688,7 +7502,7 @@
         <v>2014</v>
       </c>
       <c r="E8" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
       <c r="F8" t="s">
         <v>302</v>
@@ -5700,7 +7514,7 @@
         <v>176</v>
       </c>
       <c r="I8" t="s">
-        <v>483</v>
+        <v>473</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -5740,7 +7554,7 @@
         <v>185</v>
       </c>
       <c r="H10" t="s">
-        <v>503</v>
+        <v>493</v>
       </c>
       <c r="I10" t="s">
         <v>179</v>
@@ -5763,7 +7577,7 @@
         <v>184</v>
       </c>
       <c r="H11" t="s">
-        <v>498</v>
+        <v>488</v>
       </c>
       <c r="I11" t="s">
         <v>181</v>
@@ -5786,7 +7600,7 @@
         <v>183</v>
       </c>
       <c r="H12" t="s">
-        <v>498</v>
+        <v>488</v>
       </c>
       <c r="I12" t="s">
         <v>182</v>
@@ -5826,7 +7640,7 @@
         <v>2015</v>
       </c>
       <c r="E14" t="s">
-        <v>473</v>
+        <v>463</v>
       </c>
       <c r="F14" t="s">
         <v>178</v>
@@ -5990,7 +7804,7 @@
         <v>2015</v>
       </c>
       <c r="E21" t="s">
-        <v>489</v>
+        <v>479</v>
       </c>
       <c r="F21" t="s">
         <v>301</v>
@@ -6266,7 +8080,7 @@
         <v>216</v>
       </c>
       <c r="H33" t="s">
-        <v>499</v>
+        <v>489</v>
       </c>
       <c r="I33" t="s">
         <v>214</v>
@@ -6283,7 +8097,7 @@
         <v>2015</v>
       </c>
       <c r="E34" t="s">
-        <v>490</v>
+        <v>480</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>313</v>
@@ -6309,7 +8123,7 @@
         <v>2015</v>
       </c>
       <c r="E35" t="s">
-        <v>472</v>
+        <v>462</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>313</v>
@@ -6318,7 +8132,7 @@
         <v>318</v>
       </c>
       <c r="H35" t="s">
-        <v>500</v>
+        <v>490</v>
       </c>
       <c r="I35" t="s">
         <v>317</v>
@@ -6364,7 +8178,7 @@
         <v>216</v>
       </c>
       <c r="H37" t="s">
-        <v>501</v>
+        <v>491</v>
       </c>
       <c r="I37" t="s">
         <v>214</v>
@@ -6387,7 +8201,7 @@
         <v>169</v>
       </c>
       <c r="H38" t="s">
-        <v>502</v>
+        <v>492</v>
       </c>
       <c r="I38" t="s">
         <v>248</v>
@@ -6507,25 +8321,25 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>475</v>
+        <v>465</v>
       </c>
       <c r="C44">
         <v>2016</v>
       </c>
       <c r="E44" t="s">
-        <v>487</v>
+        <v>477</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>178</v>
       </c>
       <c r="G44" t="s">
-        <v>474</v>
+        <v>464</v>
       </c>
       <c r="H44" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
       <c r="I44" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
@@ -6539,273 +8353,19 @@
         <v>2016</v>
       </c>
       <c r="E45" t="s">
-        <v>478</v>
+        <v>468</v>
       </c>
       <c r="F45" t="s">
         <v>178</v>
       </c>
       <c r="G45" t="s">
-        <v>479</v>
+        <v>469</v>
       </c>
       <c r="H45" t="s">
-        <v>480</v>
+        <v>470</v>
       </c>
       <c r="I45" t="s">
-        <v>481</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE156D2-7E33-4447-A53C-1EA25432072D}">
-  <dimension ref="A1:H11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>353</v>
-      </c>
-      <c r="D1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E1" t="s">
-        <v>385</v>
-      </c>
-      <c r="F1" t="s">
-        <v>505</v>
-      </c>
-      <c r="G1" t="s">
-        <v>368</v>
-      </c>
-      <c r="H1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>349</v>
-      </c>
-      <c r="D2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" t="s">
-        <v>373</v>
-      </c>
-      <c r="F2" t="s">
-        <v>462</v>
-      </c>
-      <c r="G2" t="s">
-        <v>369</v>
-      </c>
-      <c r="H2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>396</v>
-      </c>
-      <c r="C3">
-        <v>2017</v>
-      </c>
-      <c r="E3" t="s">
-        <v>449</v>
-      </c>
-      <c r="G3" t="s">
-        <v>442</v>
-      </c>
-      <c r="H3" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>444</v>
-      </c>
-      <c r="C4">
-        <v>2017</v>
-      </c>
-      <c r="E4" t="s">
-        <v>450</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>445</v>
-      </c>
-      <c r="C5">
-        <v>2017</v>
-      </c>
-      <c r="E5" t="s">
-        <v>451</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="H5" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>446</v>
-      </c>
-      <c r="C6">
-        <v>2017</v>
-      </c>
-      <c r="E6" t="s">
-        <v>452</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>447</v>
-      </c>
-      <c r="C7">
-        <v>2017</v>
-      </c>
-      <c r="E7" t="s">
-        <v>453</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="H7" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>448</v>
-      </c>
-      <c r="C8">
-        <v>2017</v>
-      </c>
-      <c r="E8" t="s">
-        <v>454</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>456</v>
-      </c>
-      <c r="C9">
-        <v>2018</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>510</v>
-      </c>
-      <c r="E9" t="s">
-        <v>457</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>508</v>
-      </c>
-      <c r="C10" s="2">
-        <v>2018</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>507</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="C11" s="2">
-        <v>2018</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2" t="s">
-        <v>506</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>461</v>
+        <v>471</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Service class implemented in model and templates
</commit_message>
<xml_diff>
--- a/data/CV.xlsx
+++ b/data/CV.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9048" tabRatio="714" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9048" tabRatio="714" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONFIG" sheetId="11" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="618">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1335" uniqueCount="618">
   <si>
     <t>ID</t>
   </si>
@@ -3636,7 +3636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
@@ -5090,7 +5090,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6698,8 +6698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D107D88-62EE-4992-AFEF-BB9D7FB2D529}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6939,6 +6939,9 @@
       <c r="F10" t="s">
         <v>589</v>
       </c>
+      <c r="G10" t="s">
+        <v>573</v>
+      </c>
       <c r="H10" t="s">
         <v>588</v>
       </c>
@@ -6961,6 +6964,9 @@
       </c>
       <c r="F11" t="s">
         <v>589</v>
+      </c>
+      <c r="G11" t="s">
+        <v>573</v>
       </c>
       <c r="H11" t="s">
         <v>587</v>

</xml_diff>

<commit_message>
Front-end changes made to work with latest back-end changes.
- Greatly simplified logic of the app.
</commit_message>
<xml_diff>
--- a/data/CV.xlsx
+++ b/data/CV.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9048" tabRatio="873" firstSheet="2" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9048" tabRatio="873" firstSheet="2" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONFIG" sheetId="11" r:id="rId1"/>
@@ -1343,33 +1343,12 @@
     <t>Viena</t>
   </si>
   <si>
-    <t>/static/images/lion.png</t>
-  </si>
-  <si>
-    <t>/static/images/manhat.png</t>
-  </si>
-  <si>
-    <t>/static/images/catwall.png</t>
-  </si>
-  <si>
-    <t>/static/images/girl.png</t>
-  </si>
-  <si>
-    <t>/static/images/husky.png</t>
-  </si>
-  <si>
-    <t>/static/images/viena.png</t>
-  </si>
-  <si>
     <t>drawing</t>
   </si>
   <si>
     <t>Map-man</t>
   </si>
   <si>
-    <t>/static/stories/mapman.txt</t>
-  </si>
-  <si>
     <t>short-story</t>
   </si>
   <si>
@@ -1512,9 +1491,6 @@
   </si>
   <si>
     <t>Youtube</t>
-  </si>
-  <si>
-    <t>/static/scores/Blues-Beer-Sheva.pdf</t>
   </si>
   <si>
     <t>This should embed YouTube videos</t>
@@ -2115,6 +2091,30 @@
   </si>
   <si>
     <t>True</t>
+  </si>
+  <si>
+    <t>lion.png</t>
+  </si>
+  <si>
+    <t>catwall.png</t>
+  </si>
+  <si>
+    <t>husky.png</t>
+  </si>
+  <si>
+    <t>girl.png</t>
+  </si>
+  <si>
+    <t>viena.png</t>
+  </si>
+  <si>
+    <t>mapman.txt</t>
+  </si>
+  <si>
+    <t>Blues-Beer-Sheva.pdf</t>
+  </si>
+  <si>
+    <t>manhat.png</t>
   </si>
 </sst>
 </file>
@@ -2483,7 +2483,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>675</v>
+        <v>667</v>
       </c>
       <c r="B1" s="7"/>
     </row>
@@ -2497,7 +2497,7 @@
         <v>340</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>686</v>
+        <v>678</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>341</v>
@@ -2514,7 +2514,7 @@
         <v>345</v>
       </c>
       <c r="B5" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
       <c r="D5" t="s">
         <v>367</v>
@@ -2525,7 +2525,7 @@
         <v>356</v>
       </c>
       <c r="B6" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
       <c r="C6" t="s">
         <v>345</v>
@@ -2539,7 +2539,7 @@
         <v>343</v>
       </c>
       <c r="B7" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="C7" t="s">
         <v>356</v>
@@ -2550,7 +2550,7 @@
         <v>359</v>
       </c>
       <c r="B8" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="C8" t="s">
         <v>356</v>
@@ -2564,7 +2564,7 @@
         <v>369</v>
       </c>
       <c r="B9" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="C9" t="s">
         <v>356</v>
@@ -2578,13 +2578,13 @@
         <v>358</v>
       </c>
       <c r="B10" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
       <c r="C10" t="s">
         <v>345</v>
       </c>
       <c r="D10" t="s">
-        <v>568</v>
+        <v>560</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -2592,7 +2592,7 @@
         <v>389</v>
       </c>
       <c r="B11" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="C11" t="s">
         <v>358</v>
@@ -2606,7 +2606,7 @@
         <v>344</v>
       </c>
       <c r="B12" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="C12" t="s">
         <v>358</v>
@@ -2617,10 +2617,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
       <c r="B13" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="C13" t="s">
         <v>358</v>
@@ -2634,7 +2634,7 @@
         <v>390</v>
       </c>
       <c r="B14" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="C14" t="s">
         <v>358</v>
@@ -2648,7 +2648,7 @@
         <v>366</v>
       </c>
       <c r="B15" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="C15" t="s">
         <v>358</v>
@@ -2665,7 +2665,7 @@
         <v>360</v>
       </c>
       <c r="B16" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
       <c r="C16" t="s">
         <v>345</v>
@@ -2676,7 +2676,7 @@
         <v>361</v>
       </c>
       <c r="B17" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="C17" t="s">
         <v>360</v>
@@ -2693,7 +2693,7 @@
         <v>365</v>
       </c>
       <c r="B18" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="C18" t="s">
         <v>360</v>
@@ -2710,7 +2710,7 @@
         <v>346</v>
       </c>
       <c r="B19" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
       <c r="C19" t="s">
         <v>345</v>
@@ -2724,7 +2724,7 @@
         <v>353</v>
       </c>
       <c r="B20" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="C20" t="s">
         <v>346</v>
@@ -2738,7 +2738,7 @@
         <v>347</v>
       </c>
       <c r="B21" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="C21" t="s">
         <v>346</v>
@@ -2755,7 +2755,7 @@
         <v>393</v>
       </c>
       <c r="B22" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="C22" t="s">
         <v>346</v>
@@ -2836,19 +2836,19 @@
         <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>571</v>
+        <v>563</v>
       </c>
       <c r="D3" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
       <c r="E3" t="s">
-        <v>580</v>
+        <v>572</v>
       </c>
       <c r="F3" t="s">
         <v>405</v>
       </c>
       <c r="G3" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="H3" t="s">
         <v>69</v>
@@ -2859,19 +2859,19 @@
         <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
       <c r="D4" t="s">
-        <v>578</v>
+        <v>570</v>
       </c>
       <c r="E4" t="s">
-        <v>581</v>
+        <v>573</v>
       </c>
       <c r="F4" t="s">
         <v>405</v>
       </c>
       <c r="G4" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="H4" t="s">
         <v>69</v>
@@ -2882,19 +2882,19 @@
         <v>82</v>
       </c>
       <c r="B5" t="s">
+        <v>565</v>
+      </c>
+      <c r="D5" t="s">
+        <v>571</v>
+      </c>
+      <c r="E5" t="s">
         <v>573</v>
-      </c>
-      <c r="D5" t="s">
-        <v>579</v>
-      </c>
-      <c r="E5" t="s">
-        <v>581</v>
       </c>
       <c r="F5" t="s">
         <v>405</v>
       </c>
       <c r="G5" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="H5" t="s">
         <v>69</v>
@@ -2905,19 +2905,19 @@
         <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>574</v>
+        <v>566</v>
       </c>
       <c r="D6" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
       <c r="E6" t="s">
-        <v>580</v>
+        <v>572</v>
       </c>
       <c r="F6" t="s">
         <v>405</v>
       </c>
       <c r="G6" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="H6" t="s">
         <v>69</v>
@@ -2928,19 +2928,19 @@
         <v>84</v>
       </c>
       <c r="B7" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
       <c r="D7" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
       <c r="E7" t="s">
-        <v>580</v>
+        <v>572</v>
       </c>
       <c r="F7" t="s">
         <v>405</v>
       </c>
       <c r="G7" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="H7" t="s">
         <v>69</v>
@@ -2951,19 +2951,19 @@
         <v>85</v>
       </c>
       <c r="B8" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="D8" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
       <c r="E8" t="s">
-        <v>580</v>
+        <v>572</v>
       </c>
       <c r="F8" t="s">
         <v>405</v>
       </c>
       <c r="G8" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="H8" t="s">
         <v>69</v>
@@ -2974,19 +2974,19 @@
         <v>86</v>
       </c>
       <c r="B9" t="s">
-        <v>577</v>
+        <v>569</v>
       </c>
       <c r="D9" t="s">
-        <v>579</v>
+        <v>571</v>
       </c>
       <c r="E9" t="s">
-        <v>581</v>
+        <v>573</v>
       </c>
       <c r="F9" t="s">
         <v>405</v>
       </c>
       <c r="G9" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="H9" t="s">
         <v>69</v>
@@ -2997,25 +2997,25 @@
         <v>87</v>
       </c>
       <c r="B10" t="s">
-        <v>601</v>
+        <v>593</v>
       </c>
       <c r="C10" t="s">
-        <v>582</v>
+        <v>574</v>
       </c>
       <c r="D10" t="s">
-        <v>603</v>
+        <v>595</v>
       </c>
       <c r="E10" t="s">
-        <v>589</v>
+        <v>581</v>
       </c>
       <c r="F10" t="s">
-        <v>585</v>
+        <v>577</v>
       </c>
       <c r="G10" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="H10" t="s">
-        <v>584</v>
+        <v>576</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -3023,25 +3023,25 @@
         <v>88</v>
       </c>
       <c r="B11" t="s">
-        <v>602</v>
+        <v>594</v>
       </c>
       <c r="C11" t="s">
+        <v>574</v>
+      </c>
+      <c r="D11" t="s">
+        <v>595</v>
+      </c>
+      <c r="E11" t="s">
         <v>582</v>
       </c>
-      <c r="D11" t="s">
-        <v>603</v>
-      </c>
-      <c r="E11" t="s">
-        <v>590</v>
-      </c>
       <c r="F11" t="s">
-        <v>585</v>
+        <v>577</v>
       </c>
       <c r="G11" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="H11" t="s">
-        <v>583</v>
+        <v>575</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -3049,13 +3049,13 @@
         <v>89</v>
       </c>
       <c r="B12" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
       <c r="C12">
         <v>2016</v>
       </c>
       <c r="D12" t="s">
-        <v>587</v>
+        <v>579</v>
       </c>
       <c r="E12" t="s">
         <v>267</v>
@@ -3064,10 +3064,10 @@
         <v>405</v>
       </c>
       <c r="G12" t="s">
-        <v>586</v>
+        <v>578</v>
       </c>
       <c r="H12" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -3075,25 +3075,25 @@
         <v>90</v>
       </c>
       <c r="B13" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
       <c r="C13">
         <v>2014</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>599</v>
+        <v>591</v>
       </c>
       <c r="E13" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
       <c r="F13" t="s">
         <v>407</v>
       </c>
       <c r="G13" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="H13" t="s">
-        <v>600</v>
+        <v>592</v>
       </c>
     </row>
   </sheetData>
@@ -3174,28 +3174,28 @@
         <v>91</v>
       </c>
       <c r="B3" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
       <c r="C3">
         <v>2014</v>
       </c>
       <c r="D3" t="s">
-        <v>592</v>
+        <v>584</v>
       </c>
       <c r="E3" t="s">
-        <v>593</v>
+        <v>585</v>
       </c>
       <c r="F3" t="s">
         <v>407</v>
       </c>
       <c r="G3" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
       <c r="H3" t="s">
-        <v>607</v>
+        <v>599</v>
       </c>
       <c r="I3" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -3203,28 +3203,28 @@
         <v>92</v>
       </c>
       <c r="B4" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
       <c r="C4" t="s">
-        <v>597</v>
+        <v>589</v>
       </c>
       <c r="D4" t="s">
-        <v>592</v>
+        <v>584</v>
       </c>
       <c r="E4" t="s">
-        <v>593</v>
+        <v>585</v>
       </c>
       <c r="F4" t="s">
         <v>407</v>
       </c>
       <c r="G4" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
       <c r="H4" t="s">
-        <v>607</v>
+        <v>599</v>
       </c>
       <c r="I4" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -3238,22 +3238,22 @@
         <v>2013</v>
       </c>
       <c r="D5" t="s">
-        <v>604</v>
+        <v>596</v>
       </c>
       <c r="E5" t="s">
-        <v>605</v>
+        <v>597</v>
       </c>
       <c r="F5" t="s">
         <v>405</v>
       </c>
       <c r="G5" t="s">
-        <v>606</v>
+        <v>598</v>
       </c>
       <c r="H5" t="s">
-        <v>607</v>
+        <v>599</v>
       </c>
       <c r="I5" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -3261,28 +3261,28 @@
         <v>94</v>
       </c>
       <c r="B6" t="s">
-        <v>608</v>
+        <v>600</v>
       </c>
       <c r="C6">
         <v>2012</v>
       </c>
       <c r="D6" t="s">
-        <v>604</v>
+        <v>596</v>
       </c>
       <c r="E6" t="s">
-        <v>605</v>
+        <v>597</v>
       </c>
       <c r="F6" t="s">
         <v>407</v>
       </c>
       <c r="G6" t="s">
-        <v>606</v>
+        <v>598</v>
       </c>
       <c r="H6" t="s">
-        <v>607</v>
+        <v>599</v>
       </c>
       <c r="I6" t="s">
-        <v>613</v>
+        <v>605</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -3290,28 +3290,28 @@
         <v>95</v>
       </c>
       <c r="B7" t="s">
-        <v>609</v>
+        <v>601</v>
       </c>
       <c r="C7">
         <v>2012</v>
       </c>
       <c r="D7" t="s">
-        <v>604</v>
+        <v>596</v>
       </c>
       <c r="E7" t="s">
-        <v>605</v>
+        <v>597</v>
       </c>
       <c r="F7" t="s">
-        <v>611</v>
+        <v>603</v>
       </c>
       <c r="G7" t="s">
-        <v>606</v>
+        <v>598</v>
       </c>
       <c r="H7" t="s">
-        <v>607</v>
+        <v>599</v>
       </c>
       <c r="I7" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -3319,28 +3319,28 @@
         <v>96</v>
       </c>
       <c r="B8" t="s">
-        <v>610</v>
+        <v>602</v>
       </c>
       <c r="C8">
         <v>2012</v>
       </c>
       <c r="D8" t="s">
-        <v>604</v>
+        <v>596</v>
       </c>
       <c r="E8" t="s">
-        <v>605</v>
+        <v>597</v>
       </c>
       <c r="F8" t="s">
         <v>405</v>
       </c>
       <c r="G8" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="H8" t="s">
-        <v>607</v>
+        <v>599</v>
       </c>
       <c r="I8" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -3348,28 +3348,28 @@
         <v>97</v>
       </c>
       <c r="B9" t="s">
-        <v>610</v>
+        <v>602</v>
       </c>
       <c r="C9">
         <v>2011</v>
       </c>
       <c r="D9" t="s">
-        <v>604</v>
+        <v>596</v>
       </c>
       <c r="E9" t="s">
-        <v>605</v>
+        <v>597</v>
       </c>
       <c r="F9" t="s">
         <v>405</v>
       </c>
       <c r="G9" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="H9" t="s">
-        <v>612</v>
+        <v>604</v>
       </c>
       <c r="I9" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
     </row>
   </sheetData>
@@ -3471,7 +3471,7 @@
         <v>49</v>
       </c>
       <c r="I3" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -3505,7 +3505,7 @@
         <v>2016</v>
       </c>
       <c r="E5" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="F5" t="s">
         <v>302</v>
@@ -3517,7 +3517,7 @@
         <v>171</v>
       </c>
       <c r="I5" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -3531,7 +3531,7 @@
         <v>2016</v>
       </c>
       <c r="E6" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="F6" t="s">
         <v>302</v>
@@ -3540,7 +3540,7 @@
         <v>173</v>
       </c>
       <c r="H6" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="I6" t="s">
         <v>172</v>
@@ -3557,7 +3557,7 @@
         <v>2015</v>
       </c>
       <c r="E7" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="F7" t="s">
         <v>302</v>
@@ -3580,7 +3580,7 @@
         <v>2014</v>
       </c>
       <c r="E8" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="F8" t="s">
         <v>302</v>
@@ -3592,7 +3592,7 @@
         <v>176</v>
       </c>
       <c r="I8" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -3632,7 +3632,7 @@
         <v>185</v>
       </c>
       <c r="H10" t="s">
-        <v>489</v>
+        <v>482</v>
       </c>
       <c r="I10" t="s">
         <v>179</v>
@@ -3655,7 +3655,7 @@
         <v>184</v>
       </c>
       <c r="H11" t="s">
-        <v>484</v>
+        <v>477</v>
       </c>
       <c r="I11" t="s">
         <v>181</v>
@@ -3678,7 +3678,7 @@
         <v>183</v>
       </c>
       <c r="H12" t="s">
-        <v>484</v>
+        <v>477</v>
       </c>
       <c r="I12" t="s">
         <v>182</v>
@@ -3718,7 +3718,7 @@
         <v>2015</v>
       </c>
       <c r="E14" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="F14" t="s">
         <v>178</v>
@@ -3882,7 +3882,7 @@
         <v>2015</v>
       </c>
       <c r="E21" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="F21" t="s">
         <v>301</v>
@@ -4158,7 +4158,7 @@
         <v>216</v>
       </c>
       <c r="H33" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
       <c r="I33" t="s">
         <v>214</v>
@@ -4175,7 +4175,7 @@
         <v>2015</v>
       </c>
       <c r="E34" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>313</v>
@@ -4201,7 +4201,7 @@
         <v>2015</v>
       </c>
       <c r="E35" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>313</v>
@@ -4210,7 +4210,7 @@
         <v>318</v>
       </c>
       <c r="H35" t="s">
-        <v>486</v>
+        <v>479</v>
       </c>
       <c r="I35" t="s">
         <v>317</v>
@@ -4256,7 +4256,7 @@
         <v>216</v>
       </c>
       <c r="H37" t="s">
-        <v>487</v>
+        <v>480</v>
       </c>
       <c r="I37" t="s">
         <v>214</v>
@@ -4279,7 +4279,7 @@
         <v>169</v>
       </c>
       <c r="H38" t="s">
-        <v>488</v>
+        <v>481</v>
       </c>
       <c r="I38" t="s">
         <v>248</v>
@@ -4399,25 +4399,25 @@
         <v>139</v>
       </c>
       <c r="B44" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="C44">
         <v>2016</v>
       </c>
       <c r="E44" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>178</v>
       </c>
       <c r="G44" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="H44" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="I44" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
@@ -4431,19 +4431,19 @@
         <v>2016</v>
       </c>
       <c r="E45" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="F45" t="s">
         <v>178</v>
       </c>
       <c r="G45" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="H45" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="I45" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
     </row>
   </sheetData>
@@ -4456,8 +4456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE156D2-7E33-4447-A53C-1EA25432072D}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4479,7 +4479,7 @@
         <v>380</v>
       </c>
       <c r="F1" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="G1" t="s">
         <v>363</v>
@@ -4505,7 +4505,7 @@
         <v>368</v>
       </c>
       <c r="F2" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="G2" t="s">
         <v>364</v>
@@ -4525,7 +4525,7 @@
         <v>2017</v>
       </c>
       <c r="E3" t="s">
-        <v>435</v>
+        <v>681</v>
       </c>
       <c r="G3" t="s">
         <v>428</v>
@@ -4545,7 +4545,7 @@
         <v>2017</v>
       </c>
       <c r="E4" t="s">
-        <v>436</v>
+        <v>688</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>429</v>
@@ -4565,10 +4565,10 @@
         <v>2017</v>
       </c>
       <c r="E5" t="s">
-        <v>437</v>
+        <v>682</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="H5" t="s">
         <v>392</v>
@@ -4585,10 +4585,10 @@
         <v>2017</v>
       </c>
       <c r="E6" t="s">
-        <v>438</v>
+        <v>684</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>392</v>
@@ -4605,10 +4605,10 @@
         <v>2017</v>
       </c>
       <c r="E7" t="s">
-        <v>439</v>
+        <v>683</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="H7" t="s">
         <v>392</v>
@@ -4625,10 +4625,10 @@
         <v>2017</v>
       </c>
       <c r="E8" t="s">
-        <v>440</v>
+        <v>685</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>392</v>
@@ -4639,19 +4639,19 @@
         <v>147</v>
       </c>
       <c r="B9" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="C9">
         <v>2018</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="E9" t="s">
-        <v>443</v>
+        <v>686</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -4659,23 +4659,23 @@
         <v>148</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="C10" s="2">
         <v>2018</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -4683,21 +4683,21 @@
         <v>149</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="C11" s="2">
         <v>2018</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>492</v>
+        <v>687</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
     </row>
   </sheetData>
@@ -4710,8 +4710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94D0DD9B-3A24-4EEE-B532-5A3AF00D7B57}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17:G22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4785,7 +4785,7 @@
         <v>119</v>
       </c>
       <c r="F3" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
       <c r="G3" t="s">
         <v>125</v>
@@ -4808,7 +4808,7 @@
         <v>148</v>
       </c>
       <c r="F4" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
       <c r="G4" t="s">
         <v>125</v>
@@ -4828,7 +4828,7 @@
         <v>2017</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -4898,7 +4898,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" t="s">
-        <v>480</v>
+        <v>473</v>
       </c>
       <c r="H8" t="s">
         <v>135</v>
@@ -4978,7 +4978,7 @@
         <v>159</v>
       </c>
       <c r="B12" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
       <c r="C12">
         <v>2016</v>
@@ -5005,7 +5005,7 @@
         <v>2010</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
       <c r="E13" s="2"/>
       <c r="G13" t="s">
@@ -5020,19 +5020,19 @@
         <v>161</v>
       </c>
       <c r="B14" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="C14">
         <v>2018</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>144</v>
@@ -6057,7 +6057,7 @@
         <v>384</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="I17" t="s">
         <v>254</v>
@@ -6084,7 +6084,7 @@
         <v>384</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="I18" t="s">
         <v>254</v>
@@ -6111,7 +6111,7 @@
         <v>384</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="I19" t="s">
         <v>254</v>
@@ -6138,7 +6138,7 @@
         <v>384</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="I20" t="s">
         <v>254</v>
@@ -6275,7 +6275,7 @@
         <v>384</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="I25" t="s">
         <v>160</v>
@@ -6295,7 +6295,7 @@
         <v>201</v>
       </c>
       <c r="B26" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="C26" s="2">
         <v>2015</v>
@@ -6307,7 +6307,7 @@
         <v>1505.0517</v>
       </c>
       <c r="I26" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>45</v>
@@ -6350,7 +6350,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>676</v>
+        <v>668</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -6358,13 +6358,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>614</v>
+        <v>606</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>677</v>
+        <v>669</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -6378,7 +6378,7 @@
         <v>337</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>679</v>
+        <v>671</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -6392,7 +6392,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>680</v>
+        <v>672</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -6403,10 +6403,10 @@
         <v>408</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>678</v>
+        <v>670</v>
       </c>
       <c r="D5" t="s">
-        <v>681</v>
+        <v>673</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -6420,7 +6420,7 @@
         <v>380</v>
       </c>
       <c r="D6" t="s">
-        <v>681</v>
+        <v>673</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -6434,7 +6434,7 @@
         <v>397</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>682</v>
+        <v>674</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -6442,13 +6442,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>684</v>
+        <v>676</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>683</v>
+        <v>675</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>685</v>
+        <v>677</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -6481,16 +6481,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>657</v>
+        <v>649</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>656</v>
+        <v>648</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>340</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>655</v>
+        <v>647</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -6498,16 +6498,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>614</v>
+        <v>606</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>654</v>
+        <v>646</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>653</v>
+        <v>645</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -6515,16 +6515,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>652</v>
+        <v>644</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>347</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>650</v>
+        <v>642</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -6532,10 +6532,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>649</v>
+        <v>641</v>
       </c>
       <c r="C4" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="D4" t="s">
         <v>369</v>
@@ -6546,10 +6546,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>647</v>
+        <v>639</v>
       </c>
       <c r="C5" t="s">
-        <v>646</v>
+        <v>638</v>
       </c>
       <c r="D5" t="s">
         <v>343</v>
@@ -6560,16 +6560,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>645</v>
+        <v>637</v>
       </c>
       <c r="C6" t="s">
-        <v>644</v>
+        <v>636</v>
       </c>
       <c r="D6" t="s">
         <v>361</v>
       </c>
       <c r="E6" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -6577,7 +6577,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>643</v>
+        <v>635</v>
       </c>
       <c r="C7" t="s">
         <v>359</v>
@@ -6591,16 +6591,16 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>641</v>
+        <v>633</v>
       </c>
       <c r="C8" t="s">
-        <v>642</v>
+        <v>634</v>
       </c>
       <c r="D8" t="s">
         <v>361</v>
       </c>
       <c r="E8" t="s">
-        <v>641</v>
+        <v>633</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -6608,10 +6608,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>640</v>
+        <v>632</v>
       </c>
       <c r="C9" t="s">
-        <v>639</v>
+        <v>631</v>
       </c>
       <c r="D9" t="s">
         <v>389</v>
@@ -6622,10 +6622,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>638</v>
+        <v>630</v>
       </c>
       <c r="C10" t="s">
-        <v>637</v>
+        <v>629</v>
       </c>
       <c r="D10" t="s">
         <v>365</v>
@@ -6640,16 +6640,16 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>636</v>
+        <v>628</v>
       </c>
       <c r="C11" t="s">
-        <v>635</v>
+        <v>627</v>
       </c>
       <c r="D11" t="s">
         <v>366</v>
       </c>
       <c r="E11" t="s">
-        <v>634</v>
+        <v>626</v>
       </c>
       <c r="H11" s="1"/>
     </row>
@@ -6658,16 +6658,16 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>633</v>
+        <v>625</v>
       </c>
       <c r="C12" t="s">
-        <v>632</v>
+        <v>624</v>
       </c>
       <c r="D12" t="s">
         <v>344</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>631</v>
+        <v>623</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -6675,10 +6675,10 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>630</v>
+        <v>622</v>
       </c>
       <c r="C13" t="s">
-        <v>629</v>
+        <v>621</v>
       </c>
       <c r="D13" t="s">
         <v>365</v>
@@ -6692,10 +6692,10 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>628</v>
+        <v>620</v>
       </c>
       <c r="C14" t="s">
-        <v>627</v>
+        <v>619</v>
       </c>
       <c r="D14" t="s">
         <v>365</v>
@@ -6709,10 +6709,10 @@
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>626</v>
+        <v>618</v>
       </c>
       <c r="C15" t="s">
-        <v>625</v>
+        <v>617</v>
       </c>
       <c r="D15" t="s">
         <v>365</v>
@@ -6723,13 +6723,13 @@
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>624</v>
+        <v>616</v>
       </c>
       <c r="C16" t="s">
-        <v>623</v>
+        <v>615</v>
       </c>
       <c r="D16" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -6737,10 +6737,10 @@
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>622</v>
+        <v>614</v>
       </c>
       <c r="C17" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
       <c r="D17" t="s">
         <v>390</v>
@@ -6751,10 +6751,10 @@
         <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="C18" t="s">
-        <v>619</v>
+        <v>611</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>347</v>
@@ -6768,10 +6768,10 @@
         <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>618</v>
+        <v>610</v>
       </c>
       <c r="C19" t="s">
-        <v>617</v>
+        <v>609</v>
       </c>
       <c r="D19" t="s">
         <v>353</v>
@@ -6782,16 +6782,16 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>616</v>
+        <v>608</v>
       </c>
       <c r="C20" t="s">
-        <v>615</v>
+        <v>607</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>361</v>
       </c>
       <c r="E20" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
     </row>
   </sheetData>
@@ -6820,13 +6820,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>674</v>
+        <v>666</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>656</v>
+        <v>648</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>673</v>
+        <v>665</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -6834,13 +6834,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>614</v>
+        <v>606</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>672</v>
+        <v>664</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -6849,13 +6849,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>671</v>
+        <v>663</v>
       </c>
       <c r="C3" t="s">
-        <v>670</v>
+        <v>662</v>
       </c>
       <c r="D3" t="s">
-        <v>669</v>
+        <v>661</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -6863,13 +6863,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>589</v>
+        <v>581</v>
       </c>
       <c r="C4" t="s">
-        <v>668</v>
+        <v>660</v>
       </c>
       <c r="D4" t="s">
-        <v>667</v>
+        <v>659</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -6877,13 +6877,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>666</v>
+        <v>658</v>
       </c>
       <c r="C5" t="s">
-        <v>665</v>
+        <v>657</v>
       </c>
       <c r="D5" t="s">
-        <v>664</v>
+        <v>656</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -6891,13 +6891,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>663</v>
+        <v>655</v>
       </c>
       <c r="C6" t="s">
-        <v>662</v>
+        <v>654</v>
       </c>
       <c r="D6" t="s">
-        <v>661</v>
+        <v>653</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -6905,13 +6905,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>660</v>
+        <v>652</v>
       </c>
       <c r="C7" t="s">
-        <v>659</v>
+        <v>651</v>
       </c>
       <c r="D7" t="s">
-        <v>658</v>
+        <v>650</v>
       </c>
     </row>
   </sheetData>
@@ -7677,19 +7677,19 @@
         <v>2009</v>
       </c>
       <c r="E3" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="F3" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
       <c r="G3" t="s">
-        <v>558</v>
+        <v>550</v>
       </c>
       <c r="H3" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="I3" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -7706,19 +7706,19 @@
         <v>2010</v>
       </c>
       <c r="E4" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="F4" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
       <c r="G4" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
       <c r="H4" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="I4" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -7735,19 +7735,19 @@
         <v>2014</v>
       </c>
       <c r="E5" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="F5" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
       <c r="G5" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
       <c r="H5" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="I5" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -7764,19 +7764,19 @@
         <v>2015</v>
       </c>
       <c r="E6" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="F6" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
       <c r="G6" t="s">
         <v>427</v>
       </c>
       <c r="H6" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
       <c r="I6" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -7784,7 +7784,7 @@
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="C7">
         <v>2007</v>
@@ -7793,19 +7793,19 @@
         <v>2007</v>
       </c>
       <c r="E7" t="s">
-        <v>506</v>
+        <v>498</v>
       </c>
       <c r="F7" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="G7" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="H7" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="I7" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -7813,7 +7813,7 @@
         <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="C8">
         <v>2016</v>
@@ -7822,19 +7822,19 @@
         <v>2018</v>
       </c>
       <c r="E8" t="s">
-        <v>506</v>
+        <v>498</v>
       </c>
       <c r="F8" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="G8" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="H8" t="s">
         <v>71</v>
       </c>
       <c r="I8" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -7851,19 +7851,19 @@
         <v>2007</v>
       </c>
       <c r="E9" t="s">
-        <v>557</v>
+        <v>549</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>541</v>
+        <v>533</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="I9" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -7880,19 +7880,19 @@
         <v>2018</v>
       </c>
       <c r="E10" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>541</v>
+        <v>533</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>406</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="I10" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -7900,7 +7900,7 @@
         <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="C11">
         <v>2011</v>
@@ -7909,19 +7909,19 @@
         <v>2018</v>
       </c>
       <c r="E11" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>542</v>
+        <v>534</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>405</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
       <c r="I11" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -7929,7 +7929,7 @@
         <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="C12">
         <v>2007</v>
@@ -7938,19 +7938,19 @@
         <v>2010</v>
       </c>
       <c r="E12" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>543</v>
+        <v>535</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>405</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -7958,7 +7958,7 @@
         <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="C13">
         <v>2006</v>
@@ -7967,19 +7967,19 @@
         <v>2006</v>
       </c>
       <c r="E13" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>543</v>
+        <v>535</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>405</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -7987,7 +7987,7 @@
         <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
       <c r="C14">
         <v>2011</v>
@@ -7996,19 +7996,19 @@
         <v>2015</v>
       </c>
       <c r="E14" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>405</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -8016,7 +8016,7 @@
         <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
       <c r="C15">
         <v>2009</v>
@@ -8025,19 +8025,19 @@
         <v>2009</v>
       </c>
       <c r="E15" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>405</v>
       </c>
       <c r="H15" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -8045,7 +8045,7 @@
         <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="C16">
         <v>2009</v>
@@ -8054,19 +8054,19 @@
         <v>2009</v>
       </c>
       <c r="E16" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>407</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -8074,7 +8074,7 @@
         <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="C17">
         <v>2017</v>
@@ -8083,19 +8083,19 @@
         <v>2017</v>
       </c>
       <c r="E17" t="s">
-        <v>539</v>
+        <v>531</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>545</v>
+        <v>537</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
       <c r="H17" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -8112,19 +8112,19 @@
         <v>2011</v>
       </c>
       <c r="E18" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
       <c r="F18" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
       <c r="H18" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -8141,19 +8141,19 @@
         <v>2015</v>
       </c>
       <c r="E19" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
       <c r="F19" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
       <c r="H19" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -8170,19 +8170,19 @@
         <v>2016</v>
       </c>
       <c r="E20" t="s">
-        <v>549</v>
+        <v>541</v>
       </c>
       <c r="F20" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
       <c r="H20" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -8199,19 +8199,19 @@
         <v>2017</v>
       </c>
       <c r="E21" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
       <c r="F21" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
       <c r="H21" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -8219,7 +8219,7 @@
         <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="C22">
         <v>2013</v>
@@ -8228,19 +8228,19 @@
         <v>2015</v>
       </c>
       <c r="E22" t="s">
-        <v>550</v>
+        <v>542</v>
       </c>
       <c r="F22" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
       <c r="H22" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -8248,7 +8248,7 @@
         <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="C23">
         <v>2010</v>
@@ -8257,19 +8257,19 @@
         <v>2010</v>
       </c>
       <c r="E23" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
       <c r="F23" t="s">
-        <v>540</v>
+        <v>532</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
       <c r="H23" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -8277,7 +8277,7 @@
         <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="C24">
         <v>2011</v>
@@ -8286,19 +8286,19 @@
         <v>2011</v>
       </c>
       <c r="E24" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
       <c r="F24" t="s">
-        <v>540</v>
+        <v>532</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>427</v>
       </c>
       <c r="H24" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -8306,7 +8306,7 @@
         <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>554</v>
+        <v>546</v>
       </c>
       <c r="C25">
         <v>2010</v>
@@ -8315,13 +8315,13 @@
         <v>2010</v>
       </c>
       <c r="E25" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
       <c r="H25" t="s">
-        <v>553</v>
+        <v>545</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="J25" s="1"/>
     </row>
@@ -8330,7 +8330,7 @@
         <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
       <c r="C26">
         <v>2006</v>
@@ -8339,10 +8339,10 @@
         <v>2006</v>
       </c>
       <c r="E26" t="s">
-        <v>560</v>
+        <v>552</v>
       </c>
       <c r="F26" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
       <c r="G26" t="s">
         <v>427</v>
@@ -8351,7 +8351,7 @@
         <v>102</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -8359,7 +8359,7 @@
         <v>47</v>
       </c>
       <c r="B27" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
       <c r="C27">
         <v>2007</v>
@@ -8368,19 +8368,19 @@
         <v>2007</v>
       </c>
       <c r="E27" t="s">
-        <v>560</v>
+        <v>552</v>
       </c>
       <c r="F27" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
       <c r="G27" t="s">
         <v>427</v>
       </c>
       <c r="H27" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -8388,7 +8388,7 @@
         <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
       <c r="C28">
         <v>2008</v>
@@ -8397,19 +8397,19 @@
         <v>2008</v>
       </c>
       <c r="E28" t="s">
-        <v>560</v>
+        <v>552</v>
       </c>
       <c r="F28" t="s">
-        <v>561</v>
+        <v>553</v>
       </c>
       <c r="G28" t="s">
         <v>427</v>
       </c>
       <c r="H28" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -8417,7 +8417,7 @@
         <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>564</v>
+        <v>556</v>
       </c>
       <c r="C29">
         <v>2010</v>
@@ -8426,19 +8426,19 @@
         <v>2010</v>
       </c>
       <c r="E29" t="s">
-        <v>565</v>
+        <v>557</v>
       </c>
       <c r="F29" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
       <c r="G29" t="s">
         <v>427</v>
       </c>
       <c r="H29" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor corrections to map and about page
</commit_message>
<xml_diff>
--- a/data/CV.xlsx
+++ b/data/CV.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="CONFIG" sheetId="1" state="visible" r:id="rId2"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="745">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1626" uniqueCount="747">
   <si>
     <t xml:space="preserve">ID Name</t>
   </si>
@@ -2070,61 +2070,67 @@
     <t xml:space="preserve">Accepted</t>
   </si>
   <si>
+    <t xml:space="preserve">In Press</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preprint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1701.02200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Márton Naszódi, Leonardo Martínez-Sandoval, Shakhar-Smorodinsky</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extended Abstract</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un baúl de problemas olvidado: Parte VI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://universo.math.org.mx/2018-2/Baul-VI/baul-VI.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J. Hernández-Santiago, D. López Aguayo, L. Martínez Sandoval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problem Solving</t>
+  </si>
+  <si>
+    <t xml:space="preserve">universo.math</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A geometric Hall-type theorem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1090/proc12733</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1412.66390</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A. Holmsen, L. Martínez-Sandoval, L. Montejano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proceedings of the AMS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">503-511</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L. Martínez-Sandoval, R. Tamam</t>
+  </si>
+  <si>
     <t xml:space="preserve">ArXiV e-prints</t>
   </si>
   <si>
-    <t xml:space="preserve">In Press</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preprint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1701.02200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Márton Naszódi, Leonardo Martínez-Sandoval, Shakhar-Smorodinsky</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extended Abstract</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Un baúl de problemas olvidado: Parte VI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J. Hernández-Santiago, D. López Aguayo, L. Martínez Sandoval</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Problem Solving</t>
-  </si>
-  <si>
-    <t xml:space="preserve">universo.math</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In Review</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A geometric Hall-type theorem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.1090/proc12733</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1412.66390</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A. Holmsen, L. Martínez-Sandoval, L. Montejano</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proceedings of the AMS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">503-511</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L. Martínez-Sandoval, R. Tamam</t>
-  </si>
-  <si>
     <t xml:space="preserve">Un baúl de problemas olvidado: Parte V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://universo.math.org.mx/2018-1/Baul-V/baul-V.html</t>
   </si>
   <si>
     <t xml:space="preserve">3(1)</t>
@@ -2502,10 +2508,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1052631578947"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.2064777327935"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.4210526315789"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5708502024291"/>
   </cols>
   <sheetData>
@@ -2814,7 +2820,7 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.5991902834008"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.8137651821862"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5708502024291"/>
   </cols>
   <sheetData>
@@ -3477,12 +3483,12 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.5627530364372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.8825910931174"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="65.4493927125506"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="65.9838056680162"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="60.9514170040486"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.4858299595142"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5708502024291"/>
   </cols>
   <sheetData>
@@ -5158,14 +5164,14 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5708502024291"/>
   </cols>
   <sheetData>
@@ -5555,7 +5561,7 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5708502024291"/>
   </cols>
   <sheetData>
@@ -5721,7 +5727,7 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.3157894736842"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5708502024291"/>
   </cols>
   <sheetData>
@@ -6060,22 +6066,22 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.17004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.5991902834008"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.3157894736842"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.5303643724696"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.6356275303644"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.8502024291498"/>
     <col collapsed="false" hidden="false" max="11" min="10" style="0" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="33.8502024291498"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="34.17004048583"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.89068825910931"/>
   </cols>
@@ -6330,13 +6336,13 @@
         <v>672</v>
       </c>
       <c r="L7" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="M7" s="0" t="s">
         <v>673</v>
       </c>
-      <c r="M7" s="0" t="s">
-        <v>674</v>
-      </c>
       <c r="N7" s="0" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6350,27 +6356,27 @@
         <v>2017</v>
       </c>
       <c r="E8" s="0" t="s">
+        <v>674</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>675</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="I8" s="0" t="s">
         <v>676</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="K8" s="0" t="s">
         <v>677</v>
-      </c>
-      <c r="K8" s="0" t="s">
-        <v>678</v>
       </c>
       <c r="L8" s="0" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>184</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>2017</v>
@@ -6380,6 +6386,9 @@
         <v>111</v>
       </c>
       <c r="G9" s="6"/>
+      <c r="H9" s="0" t="s">
+        <v>679</v>
+      </c>
       <c r="I9" s="0" t="s">
         <v>680</v>
       </c>
@@ -6453,16 +6462,16 @@
         <v>683</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>673</v>
+        <v>691</v>
       </c>
       <c r="M11" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>187</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>2016</v>
@@ -6471,6 +6480,9 @@
         <v>111</v>
       </c>
       <c r="G12" s="6"/>
+      <c r="H12" s="0" t="s">
+        <v>693</v>
+      </c>
       <c r="I12" s="0" t="s">
         <v>680</v>
       </c>
@@ -6482,7 +6494,7 @@
         <v>682</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6490,33 +6502,33 @@
         <v>188</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="G13" s="6"/>
       <c r="I13" s="0" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="0" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="M13" s="0" t="n">
         <v>50</v>
       </c>
       <c r="N13" s="0" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6530,10 +6542,10 @@
         <v>2015</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="G14" s="6"/>
       <c r="I14" s="0" t="s">
@@ -6541,16 +6553,16 @@
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="0" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="M14" s="0" t="n">
         <v>50</v>
       </c>
       <c r="N14" s="0" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6558,7 +6570,7 @@
         <v>190</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>2015</v>
@@ -6568,16 +6580,16 @@
       </c>
       <c r="G15" s="6"/>
       <c r="I15" s="0" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="J15" s="0" t="s">
         <v>189</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6585,7 +6597,7 @@
         <v>191</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>2015</v>
@@ -6595,7 +6607,7 @@
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="3" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="I16" s="0" t="s">
         <v>680</v>
@@ -6608,7 +6620,7 @@
         <v>682</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6616,7 +6628,7 @@
         <v>192</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>2015</v>
@@ -6626,7 +6638,7 @@
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="3" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="I17" s="0" t="s">
         <v>680</v>
@@ -6639,7 +6651,7 @@
         <v>682</v>
       </c>
       <c r="M17" s="0" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6647,7 +6659,7 @@
         <v>193</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>2015</v>
@@ -6657,7 +6669,7 @@
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="3" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="I18" s="0" t="s">
         <v>680</v>
@@ -6670,7 +6682,7 @@
         <v>682</v>
       </c>
       <c r="M18" s="0" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6678,25 +6690,25 @@
         <v>194</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>2015</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>673</v>
+        <v>691</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6713,25 +6725,25 @@
         <v>646</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="M20" s="0" t="n">
         <v>145</v>
       </c>
       <c r="N20" s="0" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6739,7 +6751,7 @@
         <v>196</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>2014</v>
@@ -6749,7 +6761,7 @@
       </c>
       <c r="G21" s="6"/>
       <c r="H21" s="3" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="I21" s="0" t="s">
         <v>680</v>
@@ -6762,7 +6774,7 @@
         <v>682</v>
       </c>
       <c r="M21" s="0" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6770,33 +6782,33 @@
         <v>197</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="G22" s="6"/>
       <c r="I22" s="0" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="J22" s="2"/>
       <c r="K22" s="0" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="M22" s="0" t="n">
         <v>44</v>
       </c>
       <c r="N22" s="0" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6804,7 +6816,7 @@
         <v>198</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>2011</v>
@@ -6814,16 +6826,16 @@
       </c>
       <c r="G23" s="6"/>
       <c r="I23" s="0" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="J23" s="0" t="s">
         <v>189</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6831,7 +6843,7 @@
         <v>199</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>2011</v>
@@ -6842,10 +6854,10 @@
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="3" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>204</v>
@@ -6854,13 +6866,13 @@
         <v>681</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="N24" s="6" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6868,7 +6880,7 @@
         <v>200</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>2011</v>
@@ -6879,10 +6891,10 @@
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="3" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>204</v>
@@ -6891,13 +6903,13 @@
         <v>681</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="N25" s="6" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6905,7 +6917,7 @@
         <v>201</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>2011</v>
@@ -6916,10 +6928,10 @@
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="3" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>155</v>
@@ -6928,7 +6940,7 @@
         <v>681</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="M26" s="0" t="n">
         <v>52</v>
@@ -6936,13 +6948,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H16" r:id="rId1" display="http://universo.math.org.mx/2015-1/Baul-II/baul-II.html"/>
-    <hyperlink ref="H17" r:id="rId2" display="http://universo.math.org.mx/2015-2/Baul-III/baul-III.html"/>
-    <hyperlink ref="H18" r:id="rId3" display="http://universo.math.org.mx/2015-3/Baul-IV/baul-IV.html"/>
-    <hyperlink ref="H21" r:id="rId4" display="http://universo.math.org.mx/2014-3/baul-I/baul-I.html"/>
-    <hyperlink ref="H24" r:id="rId5" display="http://www.ommenlinea.org/portfolio-items/tzaloa-2011-tercer-numero/?portfolioCats=10%2C11%2C12%2C14%2C15%2C27%2C32"/>
-    <hyperlink ref="H25" r:id="rId6" display="http://www.ommenlinea.org/portfolio-items/tzaloa-2011-segundo-numero/?portfolioCats=10%2C11%2C12%2C14%2C15%2C27%2C32"/>
-    <hyperlink ref="H26" r:id="rId7" display="http://www.miscelaneamatematica.org/Misc52/5203.pdf"/>
+    <hyperlink ref="H9" r:id="rId1" display="http://universo.math.org.mx/2018-2/Baul-VI/baul-VI.html"/>
+    <hyperlink ref="H12" r:id="rId2" display="http://universo.math.org.mx/2018-1/Baul-V/baul-V.html"/>
+    <hyperlink ref="H16" r:id="rId3" display="http://universo.math.org.mx/2015-1/Baul-II/baul-II.html"/>
+    <hyperlink ref="H17" r:id="rId4" display="http://universo.math.org.mx/2015-2/Baul-III/baul-III.html"/>
+    <hyperlink ref="H18" r:id="rId5" display="http://universo.math.org.mx/2015-3/Baul-IV/baul-IV.html"/>
+    <hyperlink ref="H21" r:id="rId6" display="http://universo.math.org.mx/2014-3/baul-I/baul-I.html"/>
+    <hyperlink ref="H24" r:id="rId7" display="http://www.ommenlinea.org/portfolio-items/tzaloa-2011-tercer-numero/?portfolioCats=10%2C11%2C12%2C14%2C15%2C27%2C32"/>
+    <hyperlink ref="H25" r:id="rId8" display="http://www.ommenlinea.org/portfolio-items/tzaloa-2011-segundo-numero/?portfolioCats=10%2C11%2C12%2C14%2C15%2C27%2C32"/>
+    <hyperlink ref="H26" r:id="rId9" display="http://www.miscelaneamatematica.org/Misc52/5203.pdf"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -7106,7 +7120,7 @@
   </sheetPr>
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -7459,7 +7473,7 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.246963562753"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="16.1740890688259"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5708502024291"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.89068825910931"/>
@@ -8310,7 +8324,7 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.4534412955466"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.7773279352227"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5708502024291"/>
   </cols>
   <sheetData>
@@ -9204,7 +9218,7 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.0647773279352"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.5708502024291"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5708502024291"/>

</xml_diff>

<commit_message>
Algunos cambios de CV
</commit_message>
<xml_diff>
--- a/data/CV.xlsx
+++ b/data/CV.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4508E5-A33E-44F2-8080-EC853E22B940}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578390F7-715D-4EF8-BE2C-DFBA16AEC98E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9048" tabRatio="873" firstSheet="2" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="9048" tabRatio="873" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONFIG" sheetId="11" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1622" uniqueCount="740">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1622" uniqueCount="741">
   <si>
     <t>ID</t>
   </si>
@@ -2269,6 +2269,9 @@
   </si>
   <si>
     <t>Institut Henri Poincaré</t>
+  </si>
+  <si>
+    <t>Seminaire GAC</t>
   </si>
 </sst>
 </file>
@@ -3564,8 +3567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{820DCA41-7065-4B6F-8FCC-B838DB872725}">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3654,7 +3657,7 @@
         <v>730</v>
       </c>
       <c r="H3" t="s">
-        <v>718</v>
+        <v>740</v>
       </c>
       <c r="I3" t="s">
         <v>739</v>
@@ -6113,8 +6116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
CV Update and some papers added
</commit_message>
<xml_diff>
--- a/data/CV.xlsx
+++ b/data/CV.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="CONFIG" sheetId="1" state="visible" r:id="rId2"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680" uniqueCount="769">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1694" uniqueCount="777">
   <si>
     <t xml:space="preserve">ID Name</t>
   </si>
@@ -660,7 +660,7 @@
     <t xml:space="preserve">Chair</t>
   </si>
   <si>
-    <t xml:space="preserve">Lead the organization of annual competition for students in 45 countries &lt;br&gt; Set up of official website (&lt;a href=’www.apmo-official’&gt;link &lt;/a&gt;) to publish resullts and statistics</t>
+    <t xml:space="preserve">Lead the organization of annual competition for students in 45 countries &lt;br&gt; Set up of official website (&lt;a href=’www.apmo-official’&gt;link&lt;/a&gt;) to publish resullts and statistics</t>
   </si>
   <si>
     <t xml:space="preserve">Asian Pacific Mathematical Olympiad</t>
@@ -2025,46 +2025,70 @@
     <t xml:space="preserve">pages</t>
   </si>
   <si>
+    <t xml:space="preserve">The convex dimension of hypergraphs and the hypersimplicial Van Kampen-Flores Theorem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preprint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L. Martínez-Sandoval, A. Padrol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preprint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ArXiV e-prints</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geometric systems of unbiased representatives</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ext-abs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.nekomath.com/static/papers/GSURs.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A. Banik, B. B. Bhattacharya, S. Bhore, L. Martínez-Sandoval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proceedings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCCG 2019 Proceedings</t>
+  </si>
+  <si>
     <t xml:space="preserve">Triangle areas determined by arrangements of planar lines</t>
   </si>
   <si>
-    <t xml:space="preserve">preprint</t>
-  </si>
-  <si>
     <t xml:space="preserve">G. Damásdi, L. Martínez-Sandoval, D. T. Nagy, Z. L. Nagy</t>
   </si>
   <si>
-    <t xml:space="preserve">Preprint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ArXiV e-prints</t>
-  </si>
-  <si>
     <t xml:space="preserve">On Erdös-Szekeres-type problems for k-convex point sets</t>
   </si>
   <si>
-    <t xml:space="preserve">ext-abs</t>
+    <t xml:space="preserve">10.1007/978-3-030-25005-8_4</t>
   </si>
   <si>
     <t xml:space="preserve">M. Balko, S. Bhore, L. Martínez-Sandoval, P. Valtr</t>
   </si>
   <si>
-    <t xml:space="preserve">Proceedings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IWOCA 2019</t>
+    <t xml:space="preserve">IWOCA 2019 Proceedings</t>
   </si>
   <si>
     <t xml:space="preserve">The convex dimension of k-uniform hypergraphs</t>
   </si>
   <si>
-    <t xml:space="preserve">L. Martínez-Sandoval, A. Padrol</t>
+    <t xml:space="preserve">http://www.nekomath.com/static/papers/SM-ConvDim.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">SMCG 2019 Book of Abstracts</t>
   </si>
   <si>
     <t xml:space="preserve">Perfect rainbow polygons for colored point sets in the plane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.nekomath.com/static/papers/SM-RainPol.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">D. Flores-Peñaloza, M. Kano, L. Martínez-Sandoval, D. Orden, J. Tejel, C.D. Tóth, J.Urrutia, B. Vogtenhuber</t>
@@ -2568,16 +2592,16 @@
   </sheetPr>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.3198380566802"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6356275303644"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5708502024291"/>
   </cols>
   <sheetData>
@@ -2886,7 +2910,7 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.0283400809717"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.4574898785425"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5708502024291"/>
   </cols>
   <sheetData>
@@ -3549,12 +3573,12 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.2064777327935"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.8502024291498"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.0647773279352"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.914979757085"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="62.9878542510121"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5708502024291"/>
   </cols>
   <sheetData>
@@ -5245,10 +5269,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.70445344129555"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.63967611336032"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.7085020242915"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6882591093117"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.9230769230769"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5708502024291"/>
   </cols>
   <sheetData>
@@ -5665,7 +5689,7 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.1376518218623"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5708502024291"/>
   </cols>
   <sheetData>
@@ -5831,7 +5855,7 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.1740890688259"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5708502024291"/>
   </cols>
   <sheetData>
@@ -6167,26 +6191,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K25" activeCellId="0" sqref="K25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.5627530364373"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.96356275303644"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.7449392712551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.3846153846154"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4251012145749"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.9230769230769"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="34.4939271255061"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="34.919028340081"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.89068825910931"/>
   </cols>
@@ -6279,11 +6303,11 @@
         <v>657</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>29</v>
-      </c>
-      <c r="B3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>658</v>
       </c>
       <c r="C3" s="0" t="n">
@@ -6293,7 +6317,7 @@
         <v>659</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>1902.03166</v>
+        <v>1909.01189</v>
       </c>
       <c r="I3" s="0" t="s">
         <v>660</v>
@@ -6305,11 +6329,11 @@
         <v>662</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="B4" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>663</v>
       </c>
       <c r="C4" s="0" t="n">
@@ -6318,42 +6342,48 @@
       <c r="E4" s="0" t="s">
         <v>664</v>
       </c>
+      <c r="H4" s="0" t="s">
+        <v>665</v>
+      </c>
       <c r="I4" s="0" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>666</v>
-      </c>
-      <c r="L4" s="0" t="s">
         <v>667</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>668</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>664</v>
+        <v>659</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>1902.03166</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>666</v>
-      </c>
-      <c r="L5" s="0" t="s">
-        <v>670</v>
+        <v>661</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>671</v>
@@ -6364,128 +6394,113 @@
       <c r="E6" s="0" t="s">
         <v>664</v>
       </c>
+      <c r="F6" s="0" t="s">
+        <v>672</v>
+      </c>
       <c r="I6" s="0" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>655</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>674</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>675</v>
+        <v>664</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>676</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>676</v>
-      </c>
-      <c r="J7" s="2"/>
+        <v>660</v>
+      </c>
       <c r="K7" s="0" t="s">
-        <v>651</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="M7" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="L7" s="0" t="s">
         <v>677</v>
       </c>
-      <c r="N7" s="2" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="8" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>678</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>655</v>
-      </c>
-      <c r="F8" s="0" t="s">
+        <v>664</v>
+      </c>
+      <c r="H8" s="0" t="s">
         <v>679</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="I8" s="0" t="s">
         <v>680</v>
       </c>
-      <c r="I8" s="0" t="s">
-        <v>681</v>
-      </c>
       <c r="K8" s="0" t="s">
-        <v>651</v>
+        <v>667</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>682</v>
-      </c>
-      <c r="M8" s="0" t="n">
-        <v>94</v>
-      </c>
-      <c r="N8" s="0" t="s">
-        <v>683</v>
+        <v>677</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>655</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>685</v>
-      </c>
-      <c r="G9" s="6" t="n">
-        <v>1601.00421</v>
+        <v>682</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>683</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>686</v>
-      </c>
+        <v>684</v>
+      </c>
+      <c r="J9" s="2"/>
       <c r="K9" s="0" t="s">
         <v>651</v>
       </c>
-      <c r="L9" s="0" t="s">
-        <v>687</v>
-      </c>
-      <c r="M9" s="0" t="s">
-        <v>688</v>
-      </c>
-      <c r="N9" s="0" t="s">
-        <v>689</v>
+      <c r="L9" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>685</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>2018</v>
@@ -6494,55 +6509,57 @@
         <v>655</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>691</v>
-      </c>
-      <c r="G10" s="6" t="n">
-        <v>1701.05529</v>
+        <v>687</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>688</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="K10" s="0" t="s">
         <v>651</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="M10" s="0" t="s">
-        <v>693</v>
+        <v>690</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>94</v>
       </c>
       <c r="N10" s="0" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>673</v>
+        <v>692</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>664</v>
+        <v>655</v>
       </c>
       <c r="F11" s="0" t="s">
+        <v>693</v>
+      </c>
+      <c r="G11" s="6" t="n">
+        <v>1601.00421</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>694</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>651</v>
+      </c>
+      <c r="L11" s="0" t="s">
         <v>695</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="I11" s="0" t="s">
-        <v>676</v>
-      </c>
-      <c r="K11" s="0" t="s">
-        <v>666</v>
-      </c>
-      <c r="L11" s="0" t="s">
+      <c r="M11" s="0" t="s">
         <v>696</v>
-      </c>
-      <c r="M11" s="0" t="n">
-        <v>99</v>
       </c>
       <c r="N11" s="0" t="s">
         <v>697</v>
@@ -6550,13 +6567,13 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>698</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>655</v>
@@ -6565,145 +6582,150 @@
         <v>699</v>
       </c>
       <c r="G12" s="6" t="n">
-        <v>1511.01315</v>
+        <v>1701.05529</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>686</v>
+        <v>700</v>
       </c>
       <c r="K12" s="0" t="s">
         <v>651</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>682</v>
-      </c>
-      <c r="M12" s="0" t="n">
-        <v>82</v>
+        <v>151</v>
+      </c>
+      <c r="M12" s="0" t="s">
+        <v>701</v>
       </c>
       <c r="N12" s="0" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>430</v>
+        <v>681</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>659</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>701</v>
-      </c>
+        <v>664</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>703</v>
+      </c>
+      <c r="G13" s="6"/>
       <c r="I13" s="0" t="s">
-        <v>702</v>
+        <v>684</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>703</v>
+        <v>704</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="N13" s="0" t="s">
+        <v>705</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>704</v>
-      </c>
-      <c r="C14" s="2" t="n">
+        <v>706</v>
+      </c>
+      <c r="C14" s="0" t="n">
         <v>2017</v>
       </c>
-      <c r="D14" s="2"/>
       <c r="E14" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="G14" s="6"/>
+        <v>655</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>707</v>
+      </c>
+      <c r="G14" s="6" t="n">
+        <v>1511.01315</v>
+      </c>
       <c r="I14" s="0" t="s">
-        <v>705</v>
-      </c>
-      <c r="J14" s="2"/>
+        <v>694</v>
+      </c>
       <c r="K14" s="0" t="s">
-        <v>706</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>707</v>
-      </c>
-      <c r="M14" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="L14" s="0" t="s">
+        <v>690</v>
+      </c>
+      <c r="M14" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="N14" s="0" t="s">
         <v>708</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>430</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>659</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>709</v>
       </c>
-      <c r="C15" s="0" t="n">
-        <v>2016</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>655</v>
-      </c>
-      <c r="F15" s="0" t="s">
+      <c r="I15" s="0" t="s">
         <v>710</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="K15" s="0" t="s">
+        <v>667</v>
+      </c>
+      <c r="L15" s="0" t="s">
         <v>711</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>712</v>
-      </c>
-      <c r="K15" s="0" t="s">
-        <v>651</v>
-      </c>
-      <c r="L15" s="0" t="s">
-        <v>713</v>
-      </c>
-      <c r="M15" s="0" t="n">
-        <v>144</v>
-      </c>
-      <c r="N15" s="0" t="s">
-        <v>714</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>319</v>
-      </c>
-      <c r="C16" s="0" t="n">
-        <v>2016</v>
-      </c>
+        <v>712</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>2017</v>
+      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="0" t="s">
-        <v>715</v>
-      </c>
-      <c r="G16" s="6" t="n">
-        <v>1612.03435</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>716</v>
+        <v>111</v>
+      </c>
+      <c r="G16" s="6"/>
+      <c r="I16" s="0" t="s">
+        <v>713</v>
       </c>
       <c r="J16" s="2"/>
       <c r="K16" s="0" t="s">
-        <v>661</v>
+        <v>714</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>662</v>
-      </c>
-      <c r="M16" s="4"/>
+        <v>715</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>716</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>717</v>
@@ -6712,94 +6734,89 @@
         <v>2016</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="G17" s="6"/>
-      <c r="I17" s="0" t="s">
-        <v>705</v>
-      </c>
-      <c r="J17" s="2"/>
+        <v>655</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>718</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>719</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>720</v>
+      </c>
       <c r="K17" s="0" t="s">
-        <v>706</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>707</v>
-      </c>
-      <c r="M17" s="0" t="s">
-        <v>718</v>
+        <v>651</v>
+      </c>
+      <c r="L17" s="0" t="s">
+        <v>721</v>
+      </c>
+      <c r="M17" s="0" t="n">
+        <v>144</v>
+      </c>
+      <c r="N17" s="0" t="s">
+        <v>722</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>719</v>
+        <v>319</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>664</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>720</v>
-      </c>
-      <c r="G18" s="6"/>
-      <c r="I18" s="0" t="s">
-        <v>721</v>
+        <v>723</v>
+      </c>
+      <c r="G18" s="6" t="n">
+        <v>1612.03435</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>724</v>
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="0" t="s">
-        <v>666</v>
+        <v>661</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>722</v>
-      </c>
-      <c r="M18" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="N18" s="0" t="s">
-        <v>723</v>
-      </c>
+        <v>662</v>
+      </c>
+      <c r="M18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>664</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>725</v>
+        <v>111</v>
       </c>
       <c r="G19" s="6"/>
       <c r="I19" s="0" t="s">
-        <v>686</v>
+        <v>713</v>
       </c>
       <c r="J19" s="2"/>
       <c r="K19" s="0" t="s">
-        <v>666</v>
+        <v>714</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>722</v>
-      </c>
-      <c r="M19" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="N19" s="0" t="s">
+        <v>715</v>
+      </c>
+      <c r="M19" s="0" t="s">
         <v>726</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>727</v>
@@ -6808,90 +6825,96 @@
         <v>2015</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>364</v>
+        <v>664</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>728</v>
       </c>
       <c r="G20" s="6"/>
       <c r="I20" s="0" t="s">
-        <v>728</v>
-      </c>
-      <c r="J20" s="0" t="s">
-        <v>189</v>
-      </c>
+        <v>729</v>
+      </c>
+      <c r="J20" s="2"/>
       <c r="K20" s="0" t="s">
-        <v>729</v>
+        <v>667</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>730</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M20" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="N20" s="0" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>111</v>
+        <v>664</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>733</v>
       </c>
       <c r="G21" s="6"/>
-      <c r="H21" s="3" t="s">
-        <v>732</v>
-      </c>
       <c r="I21" s="0" t="s">
-        <v>705</v>
+        <v>694</v>
       </c>
       <c r="J21" s="2"/>
       <c r="K21" s="0" t="s">
-        <v>706</v>
+        <v>667</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>707</v>
-      </c>
-      <c r="M21" s="0" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>730</v>
+      </c>
+      <c r="M21" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="N21" s="0" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>111</v>
+        <v>364</v>
       </c>
       <c r="G22" s="6"/>
-      <c r="H22" s="3" t="s">
-        <v>735</v>
-      </c>
       <c r="I22" s="0" t="s">
-        <v>705</v>
-      </c>
-      <c r="J22" s="2"/>
+        <v>736</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>189</v>
+      </c>
       <c r="K22" s="0" t="s">
-        <v>706</v>
+        <v>737</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>707</v>
-      </c>
-      <c r="M22" s="0" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>2015</v>
@@ -6901,252 +6924,240 @@
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="3" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>705</v>
+        <v>713</v>
       </c>
       <c r="J23" s="2"/>
       <c r="K23" s="0" t="s">
-        <v>706</v>
+        <v>714</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>707</v>
+        <v>715</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>740</v>
-      </c>
-      <c r="C24" s="2" t="n">
+        <v>742</v>
+      </c>
+      <c r="C24" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>659</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>741</v>
+        <v>111</v>
+      </c>
+      <c r="G24" s="6"/>
+      <c r="H24" s="3" t="s">
+        <v>743</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>742</v>
-      </c>
+        <v>713</v>
+      </c>
+      <c r="J24" s="2"/>
       <c r="K24" s="0" t="s">
-        <v>661</v>
+        <v>714</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>715</v>
+      </c>
+      <c r="M24" s="0" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>494</v>
+        <v>745</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>655</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>743</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>744</v>
+        <v>111</v>
+      </c>
+      <c r="G25" s="6"/>
+      <c r="H25" s="3" t="s">
+        <v>746</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>745</v>
-      </c>
+        <v>713</v>
+      </c>
+      <c r="J25" s="2"/>
       <c r="K25" s="0" t="s">
-        <v>651</v>
-      </c>
-      <c r="L25" s="0" t="s">
-        <v>746</v>
-      </c>
-      <c r="M25" s="0" t="n">
-        <v>145</v>
-      </c>
-      <c r="N25" s="0" t="s">
+        <v>714</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="M25" s="0" t="s">
         <v>747</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>748</v>
       </c>
-      <c r="C26" s="0" t="n">
-        <v>2014</v>
+      <c r="C26" s="2" t="n">
+        <v>2015</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="G26" s="6"/>
-      <c r="H26" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="G26" s="6" t="s">
         <v>749</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>705</v>
-      </c>
-      <c r="J26" s="2"/>
+        <v>750</v>
+      </c>
       <c r="K26" s="0" t="s">
-        <v>706</v>
+        <v>661</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>707</v>
-      </c>
-      <c r="M26" s="0" t="s">
-        <v>750</v>
+        <v>662</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B27" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>2015</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>655</v>
+      </c>
+      <c r="F27" s="0" t="s">
         <v>751</v>
       </c>
-      <c r="C27" s="0" t="n">
-        <v>2013</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>664</v>
-      </c>
-      <c r="F27" s="0" t="s">
+      <c r="G27" s="6" t="s">
         <v>752</v>
       </c>
-      <c r="G27" s="6"/>
       <c r="I27" s="0" t="s">
         <v>753</v>
       </c>
-      <c r="J27" s="2"/>
       <c r="K27" s="0" t="s">
-        <v>666</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>722</v>
+        <v>651</v>
+      </c>
+      <c r="L27" s="0" t="s">
+        <v>754</v>
       </c>
       <c r="M27" s="0" t="n">
+        <v>145</v>
+      </c>
+      <c r="N27" s="0" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>756</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>2014</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="G28" s="6"/>
+      <c r="H28" s="3" t="s">
+        <v>757</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>713</v>
+      </c>
+      <c r="J28" s="2"/>
+      <c r="K28" s="0" t="s">
+        <v>714</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="M28" s="0" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>759</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>2013</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>664</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>760</v>
+      </c>
+      <c r="G29" s="6"/>
+      <c r="I29" s="0" t="s">
+        <v>761</v>
+      </c>
+      <c r="J29" s="2"/>
+      <c r="K29" s="0" t="s">
+        <v>667</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>730</v>
+      </c>
+      <c r="M29" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="N27" s="0" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
+      <c r="N29" s="0" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
         <v>4</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>755</v>
-      </c>
-      <c r="C28" s="0" t="n">
-        <v>2011</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>364</v>
-      </c>
-      <c r="G28" s="6"/>
-      <c r="I28" s="0" t="s">
-        <v>756</v>
-      </c>
-      <c r="J28" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="K28" s="0" t="s">
-        <v>729</v>
-      </c>
-      <c r="L28" s="2" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>758</v>
-      </c>
-      <c r="C29" s="2" t="n">
-        <v>2011</v>
-      </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="G29" s="6"/>
-      <c r="H29" s="3" t="s">
-        <v>759</v>
-      </c>
-      <c r="I29" s="0" t="s">
-        <v>756</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="K29" s="0" t="s">
-        <v>706</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>760</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>761</v>
-      </c>
-      <c r="N29" s="6" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
-        <v>2</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>763</v>
       </c>
-      <c r="C30" s="2" t="n">
+      <c r="C30" s="0" t="n">
         <v>2011</v>
       </c>
-      <c r="D30" s="2"/>
       <c r="E30" s="0" t="s">
-        <v>111</v>
+        <v>364</v>
       </c>
       <c r="G30" s="6"/>
-      <c r="H30" s="3" t="s">
+      <c r="I30" s="0" t="s">
         <v>764</v>
       </c>
-      <c r="I30" s="0" t="s">
-        <v>756</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>204</v>
+      <c r="J30" s="0" t="s">
+        <v>189</v>
       </c>
       <c r="K30" s="0" t="s">
-        <v>706</v>
+        <v>737</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>760</v>
-      </c>
-      <c r="M30" s="2" t="s">
         <v>765</v>
-      </c>
-      <c r="N30" s="6" t="s">
-        <v>762</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>766</v>
@@ -7163,30 +7174,107 @@
         <v>767</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>756</v>
+        <v>764</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>155</v>
+        <v>204</v>
       </c>
       <c r="K31" s="0" t="s">
-        <v>706</v>
+        <v>714</v>
       </c>
       <c r="L31" s="2" t="s">
         <v>768</v>
       </c>
-      <c r="M31" s="0" t="n">
+      <c r="M31" s="2" t="s">
+        <v>769</v>
+      </c>
+      <c r="N31" s="6" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>771</v>
+      </c>
+      <c r="C32" s="2" t="n">
+        <v>2011</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="G32" s="6"/>
+      <c r="H32" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="I32" s="0" t="s">
+        <v>764</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="K32" s="0" t="s">
+        <v>714</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>773</v>
+      </c>
+      <c r="N32" s="6" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>774</v>
+      </c>
+      <c r="C33" s="2" t="n">
+        <v>2011</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="G33" s="6"/>
+      <c r="H33" s="3" t="s">
+        <v>775</v>
+      </c>
+      <c r="I33" s="0" t="s">
+        <v>764</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="K33" s="0" t="s">
+        <v>714</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="M33" s="0" t="n">
         <v>52</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H21" r:id="rId1" display="http://universo.math.org.mx/2015-1/Baul-II/baul-II.html"/>
-    <hyperlink ref="H22" r:id="rId2" display="http://universo.math.org.mx/2015-2/Baul-III/baul-III.html"/>
-    <hyperlink ref="H23" r:id="rId3" display="http://universo.math.org.mx/2015-3/Baul-IV/baul-IV.html"/>
-    <hyperlink ref="H26" r:id="rId4" display="http://universo.math.org.mx/2014-3/baul-I/baul-I.html"/>
-    <hyperlink ref="H29" r:id="rId5" display="http://www.ommenlinea.org/portfolio-items/tzaloa-2011-tercer-numero/?portfolioCats=10%2C11%2C12%2C14%2C15%2C27%2C32"/>
-    <hyperlink ref="H30" r:id="rId6" display="http://www.ommenlinea.org/portfolio-items/tzaloa-2011-segundo-numero/?portfolioCats=10%2C11%2C12%2C14%2C15%2C27%2C32"/>
-    <hyperlink ref="H31" r:id="rId7" display="http://www.miscelaneamatematica.org/Misc52/5203.pdf"/>
+    <hyperlink ref="H4" r:id="rId1" display="http://www.nekomath.com/static/papers/GSURs.pdf"/>
+    <hyperlink ref="H7" r:id="rId2" display="http://www.nekomath.com/static/papers/SM-ConvDim"/>
+    <hyperlink ref="H8" r:id="rId3" display="http://www.nekomath.com/static/papers/SM-RainPol"/>
+    <hyperlink ref="H23" r:id="rId4" display="http://universo.math.org.mx/2015-1/Baul-II/baul-II.html"/>
+    <hyperlink ref="H24" r:id="rId5" display="http://universo.math.org.mx/2015-2/Baul-III/baul-III.html"/>
+    <hyperlink ref="H25" r:id="rId6" display="http://universo.math.org.mx/2015-3/Baul-IV/baul-IV.html"/>
+    <hyperlink ref="H28" r:id="rId7" display="http://universo.math.org.mx/2014-3/baul-I/baul-I.html"/>
+    <hyperlink ref="H31" r:id="rId8" display="http://www.ommenlinea.org/portfolio-items/tzaloa-2011-tercer-numero/?portfolioCats=10%2C11%2C12%2C14%2C15%2C27%2C32"/>
+    <hyperlink ref="H32" r:id="rId9" display="http://www.ommenlinea.org/portfolio-items/tzaloa-2011-segundo-numero/?portfolioCats=10%2C11%2C12%2C14%2C15%2C27%2C32"/>
+    <hyperlink ref="H33" r:id="rId10" display="http://www.miscelaneamatematica.org/Misc52/5203.pdf"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -7703,7 +7791,7 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.246963562753"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5708502024291"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.89068825910931"/>
@@ -8284,8 +8372,8 @@
   </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8554,7 +8642,7 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.0971659919028"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.9554655870445"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5708502024291"/>
   </cols>
   <sheetData>
@@ -9477,7 +9565,7 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.3846153846154"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.8137651821862"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.5708502024291"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5708502024291"/>

</xml_diff>